<commit_message>
tinkering with execution time...
</commit_message>
<xml_diff>
--- a/calc/ozone STM calc setup v00a.xlsx
+++ b/calc/ozone STM calc setup v00a.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CalcDir\TRACI_ozone_stm\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2D86710-26AC-43BF-A5C8-D774ED1F1D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8AA780-4194-4192-9A71-AB0DBFD0C2F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
   </bookViews>
@@ -75,37 +75,19 @@
   <commentList>
     <comment ref="I5" authorId="0" shapeId="0" xr:uid="{C3F9C59B-D4CD-4335-8367-A9C7977F41DA}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This could be done in python, but it is calculated here.  Needed because the function fix_data_ids uses the path/file/extension to get the associated geofile.
 </t>
-        </r>
       </text>
     </comment>
     <comment ref="F41" authorId="1" shapeId="0" xr:uid="{C05BA83B-E4CC-4E37-B576-FA3EC5396FF7}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This is redundant for the GIS files.  However, it's necessary in case the others come from an excel file (e.g.) with a different ID name than what is used in the associated geofile.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -150,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1486" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1476" uniqueCount="263">
   <si>
     <t>File unique name</t>
   </si>
@@ -939,15 +921,6 @@
   </si>
   <si>
     <t>archetypes_Full_Urb3_v02</t>
-  </si>
-  <si>
-    <t>Pop2011</t>
-  </si>
-  <si>
-    <t>Pop2012</t>
-  </si>
-  <si>
-    <t>Pop2013</t>
   </si>
 </sst>
 </file>
@@ -957,7 +930,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#000\-00\-0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1082,7 +1055,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -1118,9 +1091,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="top"/>
     </xf>
@@ -1283,7 +1253,7 @@
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
     <keyFlags>
       <key name="_Self">
@@ -1424,8 +1394,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}" name="Tbl.SpatialTransforms" displayName="Tbl.SpatialTransforms" ref="B8:N12" totalsRowShown="0">
-  <autoFilter ref="B8:N12" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}" name="Tbl.SpatialTransforms" displayName="Tbl.SpatialTransforms" ref="B8:N10" totalsRowShown="0">
+  <autoFilter ref="B8:N10" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{87286839-84B9-43B8-B3CC-7A5ACD26A242}" name="STM unique name">
       <calculatedColumnFormula>Tbl.SpatialTransforms[[#This Row],[File name]]</calculatedColumnFormula>
@@ -1820,7 +1790,7 @@
     <text xml:space="preserve">This could be done in python, but it is calculated here.  Needed because the function fix_data_ids uses the path/file/extension to get the associated geofile.
 </text>
   </threadedComment>
-  <threadedComment ref="F35" dT="2024-03-27T18:27:30.51" personId="{6027BF47-3954-4784-9D7C-EBFA15F39BC9}" id="{C05BA83B-E4CC-4E37-B576-FA3EC5396FF7}">
+  <threadedComment ref="F41" dT="2024-03-27T18:27:30.51" personId="{6027BF47-3954-4784-9D7C-EBFA15F39BC9}" id="{C05BA83B-E4CC-4E37-B576-FA3EC5396FF7}">
     <text>This is redundant for the GIS files.  However, it's necessary in case the others come from an excel file (e.g.) with a different ID name than what is used in the associated geofile.</text>
   </threadedComment>
 </ThreadedComments>
@@ -1834,29 +1804,29 @@
       <selection activeCell="AC25" sqref="AC25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.875" customWidth="1"/>
-    <col min="3" max="3" width="19.75" customWidth="1"/>
-    <col min="4" max="4" width="23.625" customWidth="1"/>
-    <col min="5" max="5" width="24.75" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.75" customWidth="1"/>
-    <col min="7" max="7" width="23.25" customWidth="1"/>
-    <col min="8" max="8" width="20.75" customWidth="1"/>
-    <col min="9" max="9" width="15.625" customWidth="1"/>
-    <col min="10" max="10" width="20.75" customWidth="1"/>
-    <col min="12" max="13" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="43.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.7109375" customWidth="1"/>
+    <col min="12" max="13" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:22" ht="30">
+    <row r="7" spans="2:22" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1908,7 +1878,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="2:22">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>61</v>
       </c>
@@ -1950,8 +1920,8 @@
         <v>air_FF_NOx</v>
       </c>
       <c r="O8" t="str" cm="1">
-        <f t="array" ref="O8:O11">Tbl.SpatialTransforms[STM unique name]</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v01_New-Countries_Pop2010</v>
+        <f t="array" ref="O8:O9">Tbl.SpatialTransforms[STM unique name]</f>
+        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v02_New-Countries_Pop2010</v>
       </c>
       <c r="Q8" t="str" cm="1">
         <f t="array" ref="Q8:Q16">Tbl.Flows[Flow unique Name]</f>
@@ -1978,7 +1948,7 @@
         <v>AnthroVOCs_v01_gpkg</v>
       </c>
     </row>
-    <row r="9" spans="2:22">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>100</v>
       </c>
@@ -2013,7 +1983,7 @@
         <v>air_FF_NHx</v>
       </c>
       <c r="O9" t="str">
-        <v>STM3_newEmit_Orig-Arch_Full_Urb3_v01_New-Countries_Pop2011</v>
+        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v01_New-Countries_Pop2010</v>
       </c>
       <c r="Q9" t="str">
         <v>NO</v>
@@ -2028,7 +1998,7 @@
         <v>AnthroVOCs_v01_tif</v>
       </c>
     </row>
-    <row r="10" spans="2:22">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>159</v>
       </c>
@@ -2053,9 +2023,6 @@
       <c r="N10" t="str">
         <v>air_FF_SOx</v>
       </c>
-      <c r="O10" t="str">
-        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v02_New-Countries_Pop2012</v>
-      </c>
       <c r="Q10" t="str">
         <v>NO2</v>
       </c>
@@ -2069,7 +2036,7 @@
         <v>Pop2010</v>
       </c>
     </row>
-    <row r="11" spans="2:22">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>115</v>
       </c>
@@ -2091,9 +2058,6 @@
       <c r="N11" t="str">
         <v>ecoreg_EFs</v>
       </c>
-      <c r="O11" t="str">
-        <v>STM3_newEmit_Orig-Arch_Full_Urb3_v02_New-Countries_Pop2013</v>
-      </c>
       <c r="Q11" t="str">
         <v>NHx</v>
       </c>
@@ -2101,7 +2065,7 @@
         <v>Edgar Air Ag NH3</v>
       </c>
     </row>
-    <row r="12" spans="2:22">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>21</v>
       </c>
@@ -2121,7 +2085,7 @@
         <v>Edgar Air Ag NOx</v>
       </c>
     </row>
-    <row r="13" spans="2:22">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>45</v>
       </c>
@@ -2141,7 +2105,7 @@
         <v>Edgar Air Ag SO2</v>
       </c>
     </row>
-    <row r="14" spans="2:22">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>172</v>
       </c>
@@ -2164,7 +2128,7 @@
         <v>Edgar Air NonAg NH3</v>
       </c>
     </row>
-    <row r="15" spans="2:22">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L15" t="str">
         <v>Continents</v>
       </c>
@@ -2181,7 +2145,7 @@
         <v>Edgar Air NonAg NOx</v>
       </c>
     </row>
-    <row r="16" spans="2:22">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L16" t="str">
         <v>World</v>
       </c>
@@ -2198,7 +2162,7 @@
         <v>Edgar Air NonAg SO2</v>
       </c>
     </row>
-    <row r="17" spans="12:22">
+    <row r="17" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L17" t="str">
         <v>Ecoregions</v>
       </c>
@@ -2212,7 +2176,7 @@
         <v>Edgar Air Gen NH3</v>
       </c>
     </row>
-    <row r="18" spans="12:22">
+    <row r="18" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L18" t="str">
         <v>GeosGrid</v>
       </c>
@@ -2226,7 +2190,7 @@
         <v>Edgar Air Gen NOx</v>
       </c>
     </row>
-    <row r="19" spans="12:22">
+    <row r="19" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L19" t="str">
         <v>Pop2010</v>
       </c>
@@ -2240,7 +2204,7 @@
         <v>Edgar Air Gen SO2</v>
       </c>
     </row>
-    <row r="20" spans="12:22">
+    <row r="20" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L20" t="str">
         <v>EmitEdgarAgNH3</v>
       </c>
@@ -2251,7 +2215,7 @@
         <v>Edgar Air Ag NOx</v>
       </c>
     </row>
-    <row r="21" spans="12:22">
+    <row r="21" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L21" t="str">
         <v>EmitEdgarAgNOx</v>
       </c>
@@ -2262,7 +2226,7 @@
         <v>Edgar Air Ag SO2</v>
       </c>
     </row>
-    <row r="22" spans="12:22">
+    <row r="22" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L22" t="str">
         <v>EmitEdgarNonagNH3</v>
       </c>
@@ -2273,7 +2237,7 @@
         <v>Edgar Air NonAg NH3</v>
       </c>
     </row>
-    <row r="23" spans="12:22">
+    <row r="23" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L23" t="str">
         <v>EmitEdgarNonagNOx</v>
       </c>
@@ -2284,7 +2248,7 @@
         <v>Edgar Air NonAg NOx</v>
       </c>
     </row>
-    <row r="24" spans="12:22">
+    <row r="24" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L24" t="str">
         <v>EmitEdgarAgSO2</v>
       </c>
@@ -2295,7 +2259,7 @@
         <v>Edgar Air NonAg SO2</v>
       </c>
     </row>
-    <row r="25" spans="12:22">
+    <row r="25" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L25" t="str">
         <v>EmitEdgarNonagSO2</v>
       </c>
@@ -2306,7 +2270,7 @@
         <v>Edgar Air Gen NH3</v>
       </c>
     </row>
-    <row r="26" spans="12:22">
+    <row r="26" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L26" t="str">
         <v>EmitEdgarGenNH3</v>
       </c>
@@ -2317,7 +2281,7 @@
         <v>Edgar Air Gen NOx</v>
       </c>
     </row>
-    <row r="27" spans="12:22">
+    <row r="27" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L27" t="str">
         <v>EmitEdgarGenNOx</v>
       </c>
@@ -2328,7 +2292,7 @@
         <v>Edgar Air Gen SO2</v>
       </c>
     </row>
-    <row r="28" spans="12:22">
+    <row r="28" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L28" t="str">
         <v>EmitEdgarGenSO2</v>
       </c>
@@ -2336,42 +2300,42 @@
         <v>EmitEdgarGenSO2</v>
       </c>
     </row>
-    <row r="29" spans="12:22">
+    <row r="29" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L29" t="str">
         <v>file_FF_NOx</v>
       </c>
     </row>
-    <row r="30" spans="12:22">
+    <row r="30" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L30" t="str">
         <v>file_FF_NHx</v>
       </c>
     </row>
-    <row r="31" spans="12:22">
+    <row r="31" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L31" t="str">
         <v>file_FF_SOx</v>
       </c>
     </row>
-    <row r="32" spans="12:22">
+    <row r="32" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L32" t="str">
         <v>ecoreg_RFs_NH4_Lebrun</v>
       </c>
     </row>
-    <row r="33" spans="12:12">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L33" t="str">
         <v>ecoreg_RFs_NO3_Lebrun</v>
       </c>
     </row>
-    <row r="34" spans="12:12">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L34" t="str">
         <v>ecoreg_RFs_SO4_Lebrun</v>
       </c>
     </row>
-    <row r="35" spans="12:12">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L35" t="str">
         <v>ecoreg_EFs_Gade</v>
       </c>
     </row>
-    <row r="36" spans="12:12">
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L36" t="str">
         <v>ecoreg_GEPs</v>
       </c>
@@ -2386,56 +2350,56 @@
   <dimension ref="B2:O126"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.125" customWidth="1"/>
-    <col min="3" max="3" width="26.625" customWidth="1"/>
-    <col min="4" max="4" width="44.75" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" customWidth="1"/>
     <col min="5" max="5" width="58" customWidth="1"/>
-    <col min="6" max="6" width="31.375" customWidth="1"/>
-    <col min="7" max="7" width="68.625" customWidth="1"/>
-    <col min="8" max="8" width="18.75" customWidth="1"/>
-    <col min="9" max="9" width="23.625" customWidth="1"/>
-    <col min="10" max="10" width="22.875" customWidth="1"/>
-    <col min="11" max="11" width="32.375" customWidth="1"/>
-    <col min="12" max="12" width="21.375" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="7" max="7" width="68.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
     <col min="13" max="13" width="28" customWidth="1"/>
-    <col min="14" max="14" width="37.25" customWidth="1"/>
-    <col min="15" max="15" width="11.875" customWidth="1"/>
-    <col min="16" max="16" width="16.875" customWidth="1"/>
-    <col min="17" max="17" width="19.75" customWidth="1"/>
+    <col min="14" max="14" width="37.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" customWidth="1"/>
     <col min="18" max="22" width="18" customWidth="1"/>
-    <col min="23" max="23" width="14.875" customWidth="1"/>
-    <col min="24" max="24" width="19.625" customWidth="1"/>
-    <col min="25" max="26" width="23.375" customWidth="1"/>
-    <col min="27" max="28" width="20.125" customWidth="1"/>
-    <col min="29" max="29" width="10.25" customWidth="1"/>
-    <col min="31" max="31" width="14.875" customWidth="1"/>
-    <col min="32" max="32" width="18.625" customWidth="1"/>
-    <col min="33" max="33" width="11.875" customWidth="1"/>
-    <col min="34" max="34" width="15.625" customWidth="1"/>
-    <col min="35" max="35" width="23.375" customWidth="1"/>
-    <col min="36" max="36" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.375" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" customWidth="1"/>
+    <col min="24" max="24" width="19.5703125" customWidth="1"/>
+    <col min="25" max="26" width="23.42578125" customWidth="1"/>
+    <col min="27" max="28" width="20.140625" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" customWidth="1"/>
+    <col min="31" max="31" width="14.85546875" customWidth="1"/>
+    <col min="32" max="32" width="18.5703125" customWidth="1"/>
+    <col min="33" max="33" width="11.85546875" customWidth="1"/>
+    <col min="34" max="34" width="15.5703125" customWidth="1"/>
+    <col min="35" max="35" width="23.42578125" customWidth="1"/>
+    <col min="36" max="36" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>93</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2476,7 +2440,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -2485,11 +2449,11 @@
       </c>
       <c r="E6" t="str" cm="1">
         <f t="array" ref="E6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F6" t="str" cm="1">
         <f t="array" ref="F6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G6" t="str" cm="1">
         <f t="array" ref="G6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2515,10 +2479,10 @@
       </c>
       <c r="M6" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>254</v>
       </c>
@@ -2554,7 +2518,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>255</v>
       </c>
@@ -2590,7 +2554,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>256</v>
       </c>
@@ -2626,7 +2590,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>257</v>
       </c>
@@ -2662,7 +2626,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>250</v>
       </c>
@@ -2675,7 +2639,7 @@
       </c>
       <c r="F11" t="str" cm="1">
         <f t="array" ref="F11">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>anthro_compiled_v01</v>
       </c>
       <c r="G11" t="str" cm="1">
         <f t="array" ref="G11">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2695,10 +2659,10 @@
       </c>
       <c r="M11" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14">
+        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\anthro_compiled_v01</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>251</v>
       </c>
@@ -2734,7 +2698,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>29</v>
       </c>
@@ -2743,11 +2707,11 @@
       </c>
       <c r="E13" t="str" cm="1">
         <f t="array" ref="E13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F13" t="str" cm="1">
         <f t="array" ref="F13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G13" t="str" cm="1">
         <f t="array" ref="G13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2770,10 +2734,10 @@
       </c>
       <c r="M13" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="14" spans="2:14">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>30</v>
       </c>
@@ -2782,11 +2746,11 @@
       </c>
       <c r="E14" t="str" cm="1">
         <f t="array" ref="E14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F14" t="str" cm="1">
         <f t="array" ref="F14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G14" t="str" cm="1">
         <f t="array" ref="G14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2812,10 +2776,10 @@
       </c>
       <c r="M14" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>39</v>
       </c>
@@ -2824,7 +2788,7 @@
       </c>
       <c r="E15" t="str" cm="1">
         <f t="array" ref="E15">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>W:\data\geo\ecoregions_teow\Olson_2012\official</v>
       </c>
       <c r="F15" t="str" cm="1">
         <f t="array" ref="F15">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2851,10 +2815,10 @@
       </c>
       <c r="M15" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="16" spans="2:14">
+        <v>W:\data\geo\ecoregions_teow\Olson_2012\official\</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>31</v>
       </c>
@@ -2863,11 +2827,11 @@
       </c>
       <c r="E16" t="str" cm="1">
         <f t="array" ref="E16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F16" t="str" cm="1">
         <f t="array" ref="F16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G16" t="str" cm="1">
         <f t="array" ref="G16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2887,10 +2851,10 @@
       </c>
       <c r="M16" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>32</v>
       </c>
@@ -2899,11 +2863,11 @@
       </c>
       <c r="E17" t="str" cm="1">
         <f t="array" ref="E17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F17" t="str" cm="1">
         <f t="array" ref="F17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G17" t="str" cm="1">
         <f t="array" ref="G17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2923,10 +2887,10 @@
       </c>
       <c r="M17" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>33</v>
       </c>
@@ -2935,11 +2899,11 @@
       </c>
       <c r="E18" t="str" cm="1">
         <f t="array" ref="E18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F18" t="str" cm="1">
         <f t="array" ref="F18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G18" t="str" cm="1">
         <f t="array" ref="G18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2959,10 +2923,10 @@
       </c>
       <c r="M18" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>34</v>
       </c>
@@ -2971,11 +2935,11 @@
       </c>
       <c r="E19" t="str" cm="1">
         <f t="array" ref="E19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F19" t="str" cm="1">
         <f t="array" ref="F19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G19" t="str" cm="1">
         <f t="array" ref="G19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2995,10 +2959,10 @@
       </c>
       <c r="M19" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>35</v>
       </c>
@@ -3007,11 +2971,11 @@
       </c>
       <c r="E20" t="str" cm="1">
         <f t="array" ref="E20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F20" t="str" cm="1">
         <f t="array" ref="F20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G20" t="str" cm="1">
         <f t="array" ref="G20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3031,10 +2995,10 @@
       </c>
       <c r="M20" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>36</v>
       </c>
@@ -3043,11 +3007,11 @@
       </c>
       <c r="E21" t="str" cm="1">
         <f t="array" ref="E21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F21" t="str" cm="1">
         <f t="array" ref="F21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G21" t="str" cm="1">
         <f t="array" ref="G21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3067,10 +3031,10 @@
       </c>
       <c r="M21" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>37</v>
       </c>
@@ -3079,11 +3043,11 @@
       </c>
       <c r="E22" t="str" cm="1">
         <f t="array" ref="E22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input</v>
       </c>
       <c r="F22" t="str" cm="1">
         <f t="array" ref="F22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G22" t="str" cm="1">
         <f t="array" ref="G22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3103,10 +3067,10 @@
       </c>
       <c r="M22" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>38</v>
       </c>
@@ -3115,11 +3079,11 @@
       </c>
       <c r="E23" t="str" cm="1">
         <f t="array" ref="E23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input</v>
       </c>
       <c r="F23" t="str" cm="1">
         <f t="array" ref="F23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G23" t="str" cm="1">
         <f t="array" ref="G23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3139,10 +3103,10 @@
       </c>
       <c r="M23" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>226</v>
       </c>
@@ -3151,7 +3115,7 @@
       </c>
       <c r="E24" t="str" cm="1">
         <f t="array" ref="E24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
       </c>
       <c r="F24" t="str" cm="1">
         <f t="array" ref="F24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3173,10 +3137,10 @@
       </c>
       <c r="M24" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13">
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>227</v>
       </c>
@@ -3185,7 +3149,7 @@
       </c>
       <c r="E25" t="str" cm="1">
         <f t="array" ref="E25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
       </c>
       <c r="F25" t="str" cm="1">
         <f t="array" ref="F25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3207,10 +3171,10 @@
       </c>
       <c r="M25" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13">
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>228</v>
       </c>
@@ -3219,7 +3183,7 @@
       </c>
       <c r="E26" t="str" cm="1">
         <f t="array" ref="E26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
       </c>
       <c r="F26" t="str" cm="1">
         <f t="array" ref="F26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3241,10 +3205,10 @@
       </c>
       <c r="M26" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13">
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>191</v>
       </c>
@@ -3253,7 +3217,7 @@
       </c>
       <c r="E27" t="str" cm="1">
         <f t="array" ref="E27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
       </c>
       <c r="F27" t="str" cm="1">
         <f t="array" ref="F27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3274,10 +3238,10 @@
       </c>
       <c r="M27" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13">
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>192</v>
       </c>
@@ -3286,7 +3250,7 @@
       </c>
       <c r="E28" t="str" cm="1">
         <f t="array" ref="E28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
       </c>
       <c r="F28" t="str" cm="1">
         <f t="array" ref="F28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3307,10 +3271,10 @@
       </c>
       <c r="M28" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13">
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>193</v>
       </c>
@@ -3319,7 +3283,7 @@
       </c>
       <c r="E29" t="str" cm="1">
         <f t="array" ref="E29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
       </c>
       <c r="F29" t="str" cm="1">
         <f t="array" ref="F29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3340,10 +3304,10 @@
       </c>
       <c r="M29" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13">
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>141</v>
       </c>
@@ -3352,7 +3316,7 @@
       </c>
       <c r="E30" t="str" cm="1">
         <f t="array" ref="E30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
       </c>
       <c r="F30" t="str" cm="1">
         <f t="array" ref="F30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3373,10 +3337,10 @@
       </c>
       <c r="M30" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13">
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>143</v>
       </c>
@@ -3385,7 +3349,7 @@
       </c>
       <c r="E31" t="str" cm="1">
         <f t="array" ref="E31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
       </c>
       <c r="F31" t="str" cm="1">
         <f t="array" ref="F31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3406,10 +3370,10 @@
       </c>
       <c r="M31" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13">
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>142</v>
       </c>
@@ -3418,7 +3382,7 @@
       </c>
       <c r="E32" t="str" cm="1">
         <f t="array" ref="E32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
       </c>
       <c r="F32" t="str" cm="1">
         <f t="array" ref="F32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3439,10 +3403,10 @@
       </c>
       <c r="M32" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15">
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>57</v>
       </c>
@@ -3451,7 +3415,7 @@
       </c>
       <c r="E33" t="str" cm="1">
         <f t="array" ref="E33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
       </c>
       <c r="F33" t="str" cm="1">
         <f t="array" ref="F33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3472,10 +3436,10 @@
       </c>
       <c r="M33" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15">
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>50</v>
       </c>
@@ -3484,7 +3448,7 @@
       </c>
       <c r="E34" t="str" cm="1">
         <f t="array" ref="E34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
       </c>
       <c r="F34" t="str" cm="1">
         <f t="array" ref="F34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3505,15 +3469,15 @@
       </c>
       <c r="M34" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="40" spans="2:15">
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="41" spans="2:15">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" s="3" t="s">
         <v>42</v>
       </c>
@@ -3557,7 +3521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="2:15">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>46</v>
       </c>
@@ -3581,7 +3545,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="2:15">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>47</v>
       </c>
@@ -3605,7 +3569,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="44" spans="2:15">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>48</v>
       </c>
@@ -3629,7 +3593,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="2:15">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>49</v>
       </c>
@@ -3656,7 +3620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:15">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>50</v>
       </c>
@@ -3683,7 +3647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:15">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>151</v>
       </c>
@@ -3710,7 +3674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>152</v>
       </c>
@@ -3737,7 +3701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:12">
+    <row r="49" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>153</v>
       </c>
@@ -3764,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:12">
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>250</v>
       </c>
@@ -3786,12 +3750,12 @@
       <c r="K50" t="s">
         <v>26</v>
       </c>
-      <c r="L50" s="13" t="b" cm="1">
+      <c r="L50" t="b" cm="1">
         <f t="array" ref="L50">_xlfn.XLOOKUP(Tbl.Data[[#This Row],[Source file unique name]],Tbl.Files[File unique name],Tbl.Files[File structure]=str.file_struct.matrix)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:12">
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>251</v>
       </c>
@@ -3813,12 +3777,12 @@
       <c r="K51" t="s">
         <v>26</v>
       </c>
-      <c r="L51" s="13" t="b" cm="1">
+      <c r="L51" t="b" cm="1">
         <f t="array" ref="L51">_xlfn.XLOOKUP(Tbl.Data[[#This Row],[Source file unique name]],Tbl.Files[File unique name],Tbl.Files[File structure]=str.file_struct.matrix)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:12">
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>32</v>
       </c>
@@ -3845,7 +3809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:12">
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>51</v>
       </c>
@@ -3872,7 +3836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:12">
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>52</v>
       </c>
@@ -3899,7 +3863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:12">
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>53</v>
       </c>
@@ -3926,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:12">
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>54</v>
       </c>
@@ -3953,7 +3917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:12">
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>55</v>
       </c>
@@ -3980,7 +3944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:12">
+    <row r="58" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>56</v>
       </c>
@@ -4007,7 +3971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:12">
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>223</v>
       </c>
@@ -4034,7 +3998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:12">
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>225</v>
       </c>
@@ -4061,7 +4025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:12">
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>224</v>
       </c>
@@ -4088,12 +4052,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:7">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="68" spans="2:7">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>71</v>
       </c>
@@ -4113,7 +4077,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="69" spans="2:7">
+    <row r="69" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
         <v>28</v>
       </c>
@@ -4133,7 +4097,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="70" spans="2:7">
+    <row r="70" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
         <v>254</v>
       </c>
@@ -4150,7 +4114,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="71" spans="2:7">
+    <row r="71" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
         <v>255</v>
       </c>
@@ -4167,7 +4131,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="72" spans="2:7">
+    <row r="72" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>256</v>
       </c>
@@ -4184,7 +4148,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="73" spans="2:7">
+    <row r="73" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>257</v>
       </c>
@@ -4201,7 +4165,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="2:7">
+    <row r="74" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>250</v>
       </c>
@@ -4221,7 +4185,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="75" spans="2:7">
+    <row r="75" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>251</v>
       </c>
@@ -4238,7 +4202,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="76" spans="2:7">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>29</v>
       </c>
@@ -4258,7 +4222,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="2:7">
+    <row r="77" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>30</v>
       </c>
@@ -4278,7 +4242,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="78" spans="2:7">
+    <row r="78" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>39</v>
       </c>
@@ -4295,7 +4259,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="79" spans="2:7">
+    <row r="79" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>31</v>
       </c>
@@ -4315,7 +4279,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="2:7">
+    <row r="80" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>32</v>
       </c>
@@ -4335,7 +4299,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="2:7">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>33</v>
       </c>
@@ -4355,7 +4319,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="2:7">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>34</v>
       </c>
@@ -4375,7 +4339,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="2:7">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>35</v>
       </c>
@@ -4395,7 +4359,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="2:7">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>36</v>
       </c>
@@ -4415,7 +4379,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="85" spans="2:7">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>37</v>
       </c>
@@ -4435,7 +4399,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="2:7">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>38</v>
       </c>
@@ -4455,7 +4419,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="2:7">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>226</v>
       </c>
@@ -4472,7 +4436,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="88" spans="2:7">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>227</v>
       </c>
@@ -4489,7 +4453,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="2:7">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>228</v>
       </c>
@@ -4506,7 +4470,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="2:7">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>191</v>
       </c>
@@ -4523,7 +4487,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="91" spans="2:7">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>192</v>
       </c>
@@ -4540,7 +4504,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="92" spans="2:7">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>193</v>
       </c>
@@ -4557,7 +4521,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="93" spans="2:7">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>141</v>
       </c>
@@ -4574,7 +4538,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="94" spans="2:7">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>143</v>
       </c>
@@ -4591,7 +4555,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="95" spans="2:7">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>142</v>
       </c>
@@ -4608,7 +4572,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="96" spans="2:7">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>57</v>
       </c>
@@ -4625,7 +4589,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="97" spans="2:7">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>50</v>
       </c>
@@ -4642,525 +4606,525 @@
         <v>146</v>
       </c>
     </row>
-    <row r="98" spans="2:7">
-      <c r="B98" s="14" t="s">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B98" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C98" s="14" t="s">
+      <c r="C98" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D98" s="14" t="s">
+      <c r="D98" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E98" s="14"/>
-      <c r="F98" s="14" t="s">
+      <c r="E98" s="13"/>
+      <c r="F98" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="G98" s="14" t="s">
+      <c r="G98" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="2:7">
-      <c r="B99" s="14" t="s">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B99" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="C99" s="14" t="s">
+      <c r="C99" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D99" s="14" t="s">
+      <c r="D99" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="E99" s="14"/>
-      <c r="F99" s="14" t="s">
+      <c r="E99" s="13"/>
+      <c r="F99" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="G99" s="14" t="s">
+      <c r="G99" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="100" spans="2:7">
-      <c r="B100" s="14" t="s">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B100" s="13" t="s">
         <v>255</v>
       </c>
-      <c r="C100" s="14" t="s">
+      <c r="C100" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D100" s="14" t="s">
+      <c r="D100" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="E100" s="14"/>
-      <c r="F100" s="14" t="s">
+      <c r="E100" s="13"/>
+      <c r="F100" s="13" t="s">
         <v>260</v>
       </c>
-      <c r="G100" s="14" t="s">
+      <c r="G100" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="101" spans="2:7">
-      <c r="B101" s="14" t="s">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B101" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="C101" s="14" t="s">
+      <c r="C101" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D101" s="14" t="s">
+      <c r="D101" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="E101" s="14"/>
-      <c r="F101" s="14" t="s">
+      <c r="E101" s="13"/>
+      <c r="F101" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="G101" s="14" t="s">
+      <c r="G101" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="102" spans="2:7">
-      <c r="B102" s="14" t="s">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B102" s="13" t="s">
         <v>257</v>
       </c>
-      <c r="C102" s="14" t="s">
+      <c r="C102" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D102" s="14" t="s">
+      <c r="D102" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="E102" s="14"/>
-      <c r="F102" s="14" t="s">
+      <c r="E102" s="13"/>
+      <c r="F102" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="G102" s="14" t="s">
+      <c r="G102" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="103" spans="2:7">
-      <c r="B103" s="14" t="s">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B103" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="C103" s="14" t="s">
+      <c r="C103" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D103" s="14" t="s">
+      <c r="D103" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="E103" s="14"/>
-      <c r="F103" s="14" t="s">
+      <c r="E103" s="13"/>
+      <c r="F103" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="G103" s="14" t="s">
+      <c r="G103" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="104" spans="2:7">
-      <c r="B104" s="14" t="s">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B104" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="C104" s="14" t="s">
+      <c r="C104" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D104" s="14" t="s">
+      <c r="D104" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="E104" s="14"/>
-      <c r="F104" s="14" t="s">
+      <c r="E104" s="13"/>
+      <c r="F104" s="13" t="s">
         <v>249</v>
       </c>
-      <c r="G104" s="14" t="s">
+      <c r="G104" s="13" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="105" spans="2:7">
-      <c r="B105" s="14" t="s">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B105" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C105" s="14" t="s">
+      <c r="C105" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D105" s="14" t="s">
+      <c r="D105" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E105" s="14"/>
-      <c r="F105" s="14" t="s">
+      <c r="E105" s="13"/>
+      <c r="F105" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="G105" s="14" t="s">
+      <c r="G105" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="106" spans="2:7">
-      <c r="B106" s="14" t="s">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B106" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C106" s="14" t="s">
+      <c r="C106" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D106" s="14" t="s">
+      <c r="D106" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E106" s="14"/>
-      <c r="F106" s="14" t="s">
+      <c r="E106" s="13"/>
+      <c r="F106" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="G106" s="14" t="s">
+      <c r="G106" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="107" spans="2:7">
-      <c r="B107" s="14" t="s">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B107" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C107" s="14" t="s">
+      <c r="C107" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D107" s="14" t="s">
+      <c r="D107" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E107" s="14"/>
-      <c r="F107" s="14" t="s">
+      <c r="E107" s="13"/>
+      <c r="F107" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G107" s="14" t="s">
+      <c r="G107" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="108" spans="2:7">
-      <c r="B108" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C108" s="14" t="s">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B108" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C108" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D108" s="14" t="s">
+      <c r="D108" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E108" s="14"/>
-      <c r="F108" s="14" t="s">
+      <c r="E108" s="13"/>
+      <c r="F108" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="G108" s="14" t="s">
+      <c r="G108" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="109" spans="2:7">
-      <c r="B109" s="14" t="s">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B109" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C109" s="14" t="s">
+      <c r="C109" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D109" s="14" t="s">
+      <c r="D109" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E109" s="14"/>
-      <c r="F109" s="14" t="s">
+      <c r="E109" s="13"/>
+      <c r="F109" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="G109" s="14" t="s">
+      <c r="G109" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="110" spans="2:7">
-      <c r="B110" s="14" t="s">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B110" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C110" s="14" t="s">
+      <c r="C110" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D110" s="14" t="s">
+      <c r="D110" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E110" s="14"/>
-      <c r="F110" s="14" t="s">
+      <c r="E110" s="13"/>
+      <c r="F110" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="G110" s="14" t="s">
+      <c r="G110" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="111" spans="2:7">
-      <c r="B111" s="14" t="s">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B111" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C111" s="14" t="s">
+      <c r="C111" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D111" s="14" t="s">
+      <c r="D111" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E111" s="14"/>
-      <c r="F111" s="14" t="s">
+      <c r="E111" s="13"/>
+      <c r="F111" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="G111" s="14" t="s">
+      <c r="G111" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="112" spans="2:7">
-      <c r="B112" s="14" t="s">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B112" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C112" s="14" t="s">
+      <c r="C112" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D112" s="14" t="s">
+      <c r="D112" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E112" s="14"/>
-      <c r="F112" s="14" t="s">
+      <c r="E112" s="13"/>
+      <c r="F112" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G112" s="14" t="s">
+      <c r="G112" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="113" spans="2:7">
-      <c r="B113" s="14" t="s">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B113" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C113" s="14" t="s">
+      <c r="C113" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D113" s="14" t="s">
+      <c r="D113" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E113" s="14"/>
-      <c r="F113" s="14" t="s">
+      <c r="E113" s="13"/>
+      <c r="F113" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="G113" s="14" t="s">
+      <c r="G113" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="114" spans="2:7">
-      <c r="B114" s="14" t="s">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B114" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C114" s="14" t="s">
+      <c r="C114" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D114" s="14" t="s">
+      <c r="D114" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E114" s="14"/>
-      <c r="F114" s="14" t="s">
+      <c r="E114" s="13"/>
+      <c r="F114" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="G114" s="14" t="s">
+      <c r="G114" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="115" spans="2:7">
-      <c r="B115" s="14" t="s">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B115" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C115" s="14" t="s">
+      <c r="C115" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D115" s="14" t="s">
+      <c r="D115" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E115" s="14"/>
-      <c r="F115" s="14" t="s">
+      <c r="E115" s="13"/>
+      <c r="F115" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="G115" s="14" t="s">
+      <c r="G115" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="116" spans="2:7">
-      <c r="B116" s="14" t="s">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B116" s="13" t="s">
         <v>226</v>
       </c>
-      <c r="C116" s="14" t="s">
+      <c r="C116" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D116" s="14" t="s">
+      <c r="D116" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E116" s="14"/>
-      <c r="F116" s="14" t="s">
+      <c r="E116" s="13"/>
+      <c r="F116" s="13" t="s">
         <v>229</v>
       </c>
-      <c r="G116" s="14" t="s">
+      <c r="G116" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="117" spans="2:7">
-      <c r="B117" s="14" t="s">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B117" s="13" t="s">
         <v>227</v>
       </c>
-      <c r="C117" s="14" t="s">
+      <c r="C117" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D117" s="14" t="s">
+      <c r="D117" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E117" s="14"/>
-      <c r="F117" s="14" t="s">
+      <c r="E117" s="13"/>
+      <c r="F117" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="G117" s="14" t="s">
+      <c r="G117" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="2:7">
-      <c r="B118" s="14" t="s">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B118" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="C118" s="14" t="s">
+      <c r="C118" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D118" s="14" t="s">
+      <c r="D118" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E118" s="14"/>
-      <c r="F118" s="14" t="s">
+      <c r="E118" s="13"/>
+      <c r="F118" s="13" t="s">
         <v>231</v>
       </c>
-      <c r="G118" s="14" t="s">
+      <c r="G118" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="119" spans="2:7">
-      <c r="B119" s="14" t="s">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B119" s="13" t="s">
         <v>191</v>
       </c>
-      <c r="C119" s="14" t="s">
+      <c r="C119" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D119" s="14" t="s">
+      <c r="D119" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E119" s="14"/>
-      <c r="F119" s="14" t="s">
+      <c r="E119" s="13"/>
+      <c r="F119" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="G119" s="14" t="s">
+      <c r="G119" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="120" spans="2:7">
-      <c r="B120" s="14" t="s">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B120" s="13" t="s">
         <v>192</v>
       </c>
-      <c r="C120" s="14" t="s">
+      <c r="C120" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D120" s="14" t="s">
+      <c r="D120" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E120" s="14"/>
-      <c r="F120" s="14" t="s">
+      <c r="E120" s="13"/>
+      <c r="F120" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="G120" s="14" t="s">
+      <c r="G120" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="121" spans="2:7">
-      <c r="B121" s="14" t="s">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B121" s="13" t="s">
         <v>193</v>
       </c>
-      <c r="C121" s="14" t="s">
+      <c r="C121" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D121" s="14" t="s">
+      <c r="D121" s="13" t="s">
         <v>221</v>
       </c>
-      <c r="E121" s="14"/>
-      <c r="F121" s="14" t="s">
+      <c r="E121" s="13"/>
+      <c r="F121" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="G121" s="14" t="s">
+      <c r="G121" s="13" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="122" spans="2:7">
-      <c r="B122" s="14" t="s">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B122" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="C122" s="14" t="s">
+      <c r="C122" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D122" s="14" t="s">
+      <c r="D122" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="E122" s="14"/>
-      <c r="F122" s="14" t="s">
+      <c r="E122" s="13"/>
+      <c r="F122" s="13" t="s">
         <v>145</v>
       </c>
-      <c r="G122" s="14" t="s">
+      <c r="G122" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="123" spans="2:7">
-      <c r="B123" s="14" t="s">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B123" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="C123" s="14" t="s">
+      <c r="C123" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D123" s="14" t="s">
+      <c r="D123" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="E123" s="14"/>
-      <c r="F123" s="14" t="s">
+      <c r="E123" s="13"/>
+      <c r="F123" s="13" t="s">
         <v>147</v>
       </c>
-      <c r="G123" s="14" t="s">
+      <c r="G123" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="124" spans="2:7">
-      <c r="B124" s="14" t="s">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B124" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="C124" s="14" t="s">
+      <c r="C124" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D124" s="14" t="s">
+      <c r="D124" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="E124" s="14"/>
-      <c r="F124" s="14" t="s">
+      <c r="E124" s="13"/>
+      <c r="F124" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="G124" s="14" t="s">
+      <c r="G124" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="125" spans="2:7">
-      <c r="B125" s="14" t="s">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B125" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C125" s="14" t="s">
+      <c r="C125" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D125" s="14" t="s">
+      <c r="D125" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="E125" s="14"/>
-      <c r="F125" s="14" t="s">
+      <c r="E125" s="13"/>
+      <c r="F125" s="13" t="s">
         <v>197</v>
       </c>
-      <c r="G125" s="14" t="s">
+      <c r="G125" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="126" spans="2:7">
-      <c r="B126" s="14" t="s">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B126" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C126" s="14" t="s">
+      <c r="C126" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D126" s="14" t="s">
+      <c r="D126" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="E126" s="14"/>
-      <c r="F126" s="14" t="s">
+      <c r="E126" s="13"/>
+      <c r="F126" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="G126" s="14" t="s">
+      <c r="G126" s="13" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5208,24 +5172,24 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>102</v>
       </c>
@@ -5251,7 +5215,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>107</v>
       </c>
@@ -5272,7 +5236,7 @@
         <v>10102-43-9</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>202</v>
       </c>
@@ -5293,7 +5257,7 @@
         <v>10102-43-9</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>204</v>
       </c>
@@ -5314,7 +5278,7 @@
         <v>10102-44-0</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>108</v>
       </c>
@@ -5333,7 +5297,7 @@
         <v>000-00-0</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>128</v>
       </c>
@@ -5354,7 +5318,7 @@
         <v>7664-41-7</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>129</v>
       </c>
@@ -5375,7 +5339,7 @@
         <v>14798-03-9</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>109</v>
       </c>
@@ -5394,7 +5358,7 @@
         <v>000-00-0</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>132</v>
       </c>
@@ -5415,7 +5379,7 @@
         <v>7446-09-5</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>135</v>
       </c>
@@ -5451,34 +5415,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1D767F-008E-40CD-A786-127BCF11776D}">
-  <dimension ref="B4:N12"/>
+  <dimension ref="B4:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9:L12"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="7" max="7" width="73.125" customWidth="1"/>
-    <col min="9" max="9" width="17.625" customWidth="1"/>
-    <col min="10" max="10" width="20.875" customWidth="1"/>
-    <col min="11" max="11" width="16.25" customWidth="1"/>
-    <col min="12" max="12" width="24.125" customWidth="1"/>
-    <col min="13" max="13" width="29.125" customWidth="1"/>
+    <col min="7" max="7" width="73.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="13" width="29.140625" customWidth="1"/>
     <col min="14" max="14" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>137</v>
       </c>
       <c r="C4" t="str" cm="1">
-        <f t="array" ref="C4">_xlfn.TEXTJOIN(", ",TRUE, "'"&amp;B9:B12&amp;"'")</f>
-        <v>'STM3_newEmit_Orig-Arch_Full_Urb2_v01_New-Countries_Pop2010', 'STM3_newEmit_Orig-Arch_Full_Urb3_v01_New-Countries_Pop2011', 'STM3_newEmit_Orig-Arch_Full_Urb2_v02_New-Countries_Pop2012', 'STM3_newEmit_Orig-Arch_Full_Urb3_v02_New-Countries_Pop2013'</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14">
+        <f t="array" ref="C4">_xlfn.TEXTJOIN(", ",TRUE, "'"&amp;B9:B10&amp;"'")</f>
+        <v>'STM3_newEmit_Orig-Arch_Full_Urb2_v02_New-Countries_Pop2010', 'STM3_newEmit_Orig-Arch_Full_Urb2_v01_New-Countries_Pop2010'</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>58</v>
       </c>
@@ -5486,7 +5450,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>59</v>
       </c>
@@ -5527,17 +5491,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v02_New-Countries_Pop2010</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
       </c>
       <c r="G9" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v02_New-Countries_Pop2010</v>
       </c>
       <c r="H9" t="s">
         <v>194</v>
@@ -5546,7 +5510,7 @@
         <v>117</v>
       </c>
       <c r="J9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="K9" t="s">
         <v>28</v>
@@ -5557,129 +5521,59 @@
       <c r="M9" t="b">
         <v>1</v>
       </c>
-      <c r="N9" s="13" t="str">
+      <c r="N9" t="str">
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v02_New-Countries_Pop2010</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B10" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
+        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v01_New-Countries_Pop2010</v>
+      </c>
+      <c r="D10" t="b">
+        <v>1</v>
+      </c>
+      <c r="G10" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
+        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v01_New-Countries_Pop2010</v>
+      </c>
+      <c r="H10" t="s">
+        <v>194</v>
+      </c>
+      <c r="I10" t="s">
+        <v>117</v>
+      </c>
+      <c r="J10" t="s">
+        <v>254</v>
+      </c>
+      <c r="K10" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" t="s">
+        <v>32</v>
+      </c>
+      <c r="M10" t="b">
+        <v>1</v>
+      </c>
+      <c r="N10" t="str">
         <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
         <v>STM3_newEmit_Orig-Arch_Full_Urb2_v01_New-Countries_Pop2010</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14">
-      <c r="B10" t="str">
-        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb3_v01_New-Countries_Pop2011</v>
-      </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" t="str">
-        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb3_v01_New-Countries_Pop2011</v>
-      </c>
-      <c r="H10" t="s">
-        <v>194</v>
-      </c>
-      <c r="I10" t="s">
-        <v>117</v>
-      </c>
-      <c r="J10" t="s">
-        <v>255</v>
-      </c>
-      <c r="K10" t="s">
-        <v>28</v>
-      </c>
-      <c r="L10" t="s">
-        <v>263</v>
-      </c>
-      <c r="M10" t="b">
-        <v>1</v>
-      </c>
-      <c r="N10" s="13" t="str">
-        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb3_v01_New-Countries_Pop2011</v>
-      </c>
-    </row>
-    <row r="11" spans="2:14">
-      <c r="B11" t="str">
-        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v02_New-Countries_Pop2012</v>
-      </c>
-      <c r="D11" t="b">
-        <v>1</v>
-      </c>
-      <c r="G11" t="str">
-        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v02_New-Countries_Pop2012</v>
-      </c>
-      <c r="H11" t="s">
-        <v>194</v>
-      </c>
-      <c r="I11" t="s">
-        <v>117</v>
-      </c>
-      <c r="J11" t="s">
-        <v>256</v>
-      </c>
-      <c r="K11" t="s">
-        <v>28</v>
-      </c>
-      <c r="L11" t="s">
-        <v>264</v>
-      </c>
-      <c r="M11" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11" s="13" t="str">
-        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb2_v02_New-Countries_Pop2012</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14">
-      <c r="B12" t="str">
-        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb3_v02_New-Countries_Pop2013</v>
-      </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-      <c r="G12" t="str">
-        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb3_v02_New-Countries_Pop2013</v>
-      </c>
-      <c r="H12" t="s">
-        <v>194</v>
-      </c>
-      <c r="I12" t="s">
-        <v>117</v>
-      </c>
-      <c r="J12" t="s">
-        <v>257</v>
-      </c>
-      <c r="K12" t="s">
-        <v>28</v>
-      </c>
-      <c r="L12" t="s">
-        <v>265</v>
-      </c>
-      <c r="M12" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" s="13" t="str">
-        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM3_newEmit_Orig-Arch_Full_Urb3_v02_New-Countries_Pop2013</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I12" xr:uid="{E821405C-6957-4A9F-8765-11FEDC830D01}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I10" xr:uid="{E821405C-6957-4A9F-8765-11FEDC830D01}">
       <formula1>list.STM_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9:L12" xr:uid="{5BDCD423-46E4-4A7B-8628-5C9344A21620}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9:L10" xr:uid="{5BDCD423-46E4-4A7B-8628-5C9344A21620}">
       <formula1>list.Data_unique</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M12" xr:uid="{30B9C429-7EFE-4DEB-8979-C009F9C29D27}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M10" xr:uid="{30B9C429-7EFE-4DEB-8979-C009F9C29D27}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9:K12" xr:uid="{3AF342F9-C154-4566-A6D6-DF321DDA9F17}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9:K10" xr:uid="{3AF342F9-C154-4566-A6D6-DF321DDA9F17}">
       <formula1>list.Files_geo_unique</formula1>
     </dataValidation>
   </dataValidations>
@@ -5699,47 +5593,47 @@
       <selection activeCell="AE24" sqref="AE24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.25" customWidth="1"/>
-    <col min="3" max="3" width="17.625" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" customWidth="1"/>
     <col min="4" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.25" customWidth="1"/>
-    <col min="8" max="8" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.25" customWidth="1"/>
-    <col min="10" max="10" width="13.75" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="29.125" customWidth="1"/>
-    <col min="13" max="13" width="22.125" customWidth="1"/>
-    <col min="14" max="15" width="17.75" customWidth="1"/>
-    <col min="16" max="16" width="34.75" customWidth="1"/>
-    <col min="17" max="17" width="16.375" customWidth="1"/>
-    <col min="18" max="18" width="15.625" customWidth="1"/>
-    <col min="19" max="19" width="14.25" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="15" width="17.7109375" customWidth="1"/>
+    <col min="16" max="16" width="34.7109375" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14.28515625" customWidth="1"/>
     <col min="20" max="20" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:24">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X3" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="2:24">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="2:24">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="2:24">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X6" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:24">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>211</v>
       </c>
@@ -5753,7 +5647,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="2:24" ht="42.75">
+    <row r="8" spans="2:24" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>206</v>
       </c>
@@ -5821,7 +5715,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="2:24">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>208</v>
       </c>
@@ -5886,7 +5780,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="2:24">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>207</v>
       </c>
@@ -5951,7 +5845,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="2:24">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F11">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6007,7 +5901,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="2:24">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F12">
         <f t="shared" ref="F12:F25" si="1">IFERROR($F11+1,1)</f>
         <v>4</v>
@@ -6063,7 +5957,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="2:24">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F13">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -6119,7 +6013,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="2:24">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -6175,7 +6069,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="2:24">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -6231,7 +6125,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="2:24">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F16">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -6287,7 +6181,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="6:24">
+    <row r="17" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F17">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -6343,7 +6237,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="6:24">
+    <row r="18" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F18">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -6401,7 +6295,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="6:24">
+    <row r="19" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F19">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -6459,7 +6353,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="6:24">
+    <row r="20" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F20">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -6517,7 +6411,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="6:24">
+    <row r="21" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F21">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -6569,7 +6463,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="6:24">
+    <row r="22" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F22">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -6621,7 +6515,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="6:24">
+    <row r="23" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F23">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -6673,7 +6567,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="6:24">
+    <row r="24" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F24">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -6725,7 +6619,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="6:24">
+    <row r="25" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F25">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -6777,7 +6671,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="6:24">
+    <row r="26" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F26">
         <f t="shared" ref="F26:F53" si="2">IFERROR($F25+1,1)</f>
         <v>18</v>
@@ -6829,7 +6723,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="6:24">
+    <row r="27" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F27">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -6887,7 +6781,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="6:24">
+    <row r="28" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F28">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -6945,7 +6839,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="6:24">
+    <row r="29" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F29">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -7003,7 +6897,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="6:24">
+    <row r="30" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F30">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -7055,7 +6949,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="6:24">
+    <row r="31" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F31">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -7107,7 +7001,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="6:24">
+    <row r="32" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F32">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -7159,7 +7053,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="6:24">
+    <row r="33" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F33">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -7211,7 +7105,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="6:24">
+    <row r="34" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F34">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -7263,7 +7157,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="6:24">
+    <row r="35" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F35">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -7315,7 +7209,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="6:24">
+    <row r="36" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F36">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -7373,7 +7267,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="6:24">
+    <row r="37" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F37">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -7431,7 +7325,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="6:24">
+    <row r="38" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F38">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -7489,7 +7383,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="6:24">
+    <row r="39" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F39">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -7541,7 +7435,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="6:24">
+    <row r="40" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F40">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -7593,7 +7487,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="6:24">
+    <row r="41" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F41">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -7645,7 +7539,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="6:24">
+    <row r="42" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F42">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -7697,7 +7591,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="6:24">
+    <row r="43" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F43">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -7749,7 +7643,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="6:24">
+    <row r="44" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F44">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -7801,7 +7695,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="6:24">
+    <row r="45" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F45">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -7859,7 +7753,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="6:24">
+    <row r="46" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F46">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -7917,7 +7811,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="6:24">
+    <row r="47" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F47">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -7975,7 +7869,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="6:24">
+    <row r="48" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F48">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -8027,7 +7921,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="6:24">
+    <row r="49" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F49">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -8079,7 +7973,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="6:24">
+    <row r="50" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F50">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -8131,7 +8025,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="6:24">
+    <row r="51" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F51">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -8183,7 +8077,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="52" spans="6:24">
+    <row r="52" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F52">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -8235,7 +8129,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="6:24">
+    <row r="53" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F53">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -8287,7 +8181,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="54" spans="6:24">
+    <row r="54" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F54">
         <f t="shared" ref="F54:F71" si="3">IFERROR($F53+1,1)</f>
         <v>46</v>
@@ -8345,7 +8239,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="6:24">
+    <row r="55" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F55">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -8403,7 +8297,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="6:24">
+    <row r="56" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F56">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -8461,7 +8355,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="6:24">
+    <row r="57" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F57">
         <f t="shared" si="3"/>
         <v>49</v>
@@ -8513,7 +8407,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="6:24">
+    <row r="58" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F58">
         <f t="shared" si="3"/>
         <v>50</v>
@@ -8565,7 +8459,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="6:24">
+    <row r="59" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F59">
         <f t="shared" si="3"/>
         <v>51</v>
@@ -8617,7 +8511,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="6:24">
+    <row r="60" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F60">
         <f t="shared" si="3"/>
         <v>52</v>
@@ -8669,7 +8563,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="6:24">
+    <row r="61" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F61">
         <f t="shared" si="3"/>
         <v>53</v>
@@ -8721,7 +8615,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="6:24">
+    <row r="62" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F62">
         <f t="shared" si="3"/>
         <v>54</v>
@@ -8773,7 +8667,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="6:24">
+    <row r="63" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F63">
         <f t="shared" si="3"/>
         <v>55</v>
@@ -8831,7 +8725,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="6:24">
+    <row r="64" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F64">
         <f t="shared" si="3"/>
         <v>56</v>
@@ -8889,7 +8783,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="6:24">
+    <row r="65" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F65">
         <f t="shared" si="3"/>
         <v>57</v>
@@ -8947,7 +8841,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="66" spans="6:24">
+    <row r="66" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F66">
         <f t="shared" si="3"/>
         <v>58</v>
@@ -8999,7 +8893,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="6:24">
+    <row r="67" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F67">
         <f t="shared" si="3"/>
         <v>59</v>
@@ -9051,7 +8945,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="6:24">
+    <row r="68" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F68">
         <f t="shared" si="3"/>
         <v>60</v>
@@ -9103,7 +8997,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="6:24">
+    <row r="69" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F69">
         <f t="shared" si="3"/>
         <v>61</v>
@@ -9155,7 +9049,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="6:24">
+    <row r="70" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F70">
         <f t="shared" si="3"/>
         <v>62</v>
@@ -9207,7 +9101,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="71" spans="6:24">
+    <row r="71" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F71">
         <f t="shared" si="3"/>
         <v>63</v>

</xml_diff>

<commit_message>
add handling of unknown (not 'none' crs); add timing
</commit_message>
<xml_diff>
--- a/calc/ozone STM calc setup v00a.xlsx
+++ b/calc/ozone STM calc setup v00a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CalcDir\TRACI_ozone_stm\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1147A0F3-0CF0-444C-A7B4-FD6CA8C60078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AE523C-E9A9-41D3-AC7B-67D4E10E1D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -75,19 +75,37 @@
   <commentList>
     <comment ref="I5" authorId="0" shapeId="0" xr:uid="{C3F9C59B-D4CD-4335-8367-A9C7977F41DA}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This could be done in python, but it is calculated here.  Needed because the function fix_data_ids uses the path/file/extension to get the associated geofile.
 </t>
+        </r>
       </text>
     </comment>
     <comment ref="F44" authorId="1" shapeId="0" xr:uid="{C05BA83B-E4CC-4E37-B576-FA3EC5396FF7}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This is redundant for the GIS files.  However, it's necessary in case the others come from an excel file (e.g.) with a different ID name than what is used in the associated geofile.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -132,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="271">
   <si>
     <t>File unique name</t>
   </si>
@@ -954,7 +972,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#000\-00\-0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1277,7 +1295,7 @@
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <global>
     <keyFlags>
       <key name="_Self">
@@ -1384,8 +1402,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8294B1BA-ABF4-4D80-9C7A-5B7B2E284256}" name="Tbl.File_Locations" displayName="Tbl.File_Locations" ref="B71:G132" totalsRowShown="0">
-  <autoFilter ref="B71:G132" xr:uid="{8294B1BA-ABF4-4D80-9C7A-5B7B2E284256}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8294B1BA-ABF4-4D80-9C7A-5B7B2E284256}" name="Tbl.File_Locations" displayName="Tbl.File_Locations" ref="B71:G135" totalsRowShown="0">
+  <autoFilter ref="B71:G135" xr:uid="{8294B1BA-ABF4-4D80-9C7A-5B7B2E284256}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CBD61C72-14BB-4DB4-B8FE-FFBBB16D0157}" name="File Unique Name"/>
     <tableColumn id="2" xr3:uid="{E630A020-07CA-4AA2-A57D-9F15E52AC431}" name="User"/>
@@ -1828,29 +1846,29 @@
       <selection activeCell="AC25" sqref="AC25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="19.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.6640625" customWidth="1"/>
-    <col min="4" max="4" width="23.5546875" customWidth="1"/>
-    <col min="5" max="5" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="23.33203125" customWidth="1"/>
-    <col min="8" max="8" width="20.6640625" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" customWidth="1"/>
-    <col min="12" max="13" width="30.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="43.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="19.625" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" customWidth="1"/>
+    <col min="7" max="7" width="23.375" customWidth="1"/>
+    <col min="8" max="8" width="20.625" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
+    <col min="10" max="10" width="20.625" customWidth="1"/>
+    <col min="12" max="13" width="30.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:22" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:22" ht="30">
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1902,7 +1920,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:22">
       <c r="B8" t="s">
         <v>61</v>
       </c>
@@ -1972,7 +1990,7 @@
         <v>AnthroVOCs_v01_gpkg</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:22">
       <c r="C9" t="s">
         <v>100</v>
       </c>
@@ -2022,7 +2040,7 @@
         <v>AnthroVOCs_v01_tif</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:22">
       <c r="B10" t="s">
         <v>159</v>
       </c>
@@ -2063,7 +2081,7 @@
         <v>Pop2010</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:22">
       <c r="B11" t="s">
         <v>115</v>
       </c>
@@ -2095,7 +2113,7 @@
         <v>Edgar Air Ag NH3</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:22">
       <c r="E12" t="s">
         <v>21</v>
       </c>
@@ -2115,7 +2133,7 @@
         <v>Edgar Air Ag NOx</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:22">
       <c r="E13" t="s">
         <v>45</v>
       </c>
@@ -2135,7 +2153,7 @@
         <v>Edgar Air Ag SO2</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:22">
       <c r="D14" t="s">
         <v>172</v>
       </c>
@@ -2158,7 +2176,7 @@
         <v>Edgar Air NonAg NH3</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:22">
       <c r="L15" t="str">
         <v>Arch_Full_Urb3_v02</v>
       </c>
@@ -2175,7 +2193,7 @@
         <v>Edgar Air NonAg NOx</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:22">
       <c r="L16" t="str">
         <v>AnthroVOCs_v01_gpkg</v>
       </c>
@@ -2192,7 +2210,7 @@
         <v>Edgar Air NonAg SO2</v>
       </c>
     </row>
-    <row r="17" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="12:22">
       <c r="L17" t="str">
         <v>AnthroVOCs_v01_tif</v>
       </c>
@@ -2206,7 +2224,7 @@
         <v>Edgar Air Gen NH3</v>
       </c>
     </row>
-    <row r="18" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="12:22">
       <c r="L18" t="str">
         <v>Continents</v>
       </c>
@@ -2220,7 +2238,7 @@
         <v>Edgar Air Gen NOx</v>
       </c>
     </row>
-    <row r="19" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="12:22">
       <c r="L19" t="str">
         <v>World</v>
       </c>
@@ -2234,7 +2252,7 @@
         <v>Edgar Air Gen SO2</v>
       </c>
     </row>
-    <row r="20" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="12:22">
       <c r="L20" t="str">
         <v>Ecoregions</v>
       </c>
@@ -2245,7 +2263,7 @@
         <v>Edgar Air Ag NOx</v>
       </c>
     </row>
-    <row r="21" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="12:22">
       <c r="L21" t="str">
         <v>GeosGrid</v>
       </c>
@@ -2256,7 +2274,7 @@
         <v>Edgar Air Ag SO2</v>
       </c>
     </row>
-    <row r="22" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="12:22">
       <c r="L22" t="str">
         <v>Pop2010</v>
       </c>
@@ -2267,7 +2285,7 @@
         <v>Edgar Air NonAg NH3</v>
       </c>
     </row>
-    <row r="23" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="12:22">
       <c r="L23" t="str">
         <v>EmitEdgarAgNH3</v>
       </c>
@@ -2278,7 +2296,7 @@
         <v>Edgar Air NonAg NOx</v>
       </c>
     </row>
-    <row r="24" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="12:22">
       <c r="L24" t="str">
         <v>EmitEdgarAgNOx</v>
       </c>
@@ -2289,7 +2307,7 @@
         <v>Edgar Air NonAg SO2</v>
       </c>
     </row>
-    <row r="25" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="12:22">
       <c r="L25" t="str">
         <v>EmitEdgarNonagNH3</v>
       </c>
@@ -2300,7 +2318,7 @@
         <v>Edgar Air Gen NH3</v>
       </c>
     </row>
-    <row r="26" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="12:22">
       <c r="L26" t="str">
         <v>EmitEdgarNonagNOx</v>
       </c>
@@ -2311,7 +2329,7 @@
         <v>Edgar Air Gen NOx</v>
       </c>
     </row>
-    <row r="27" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="12:22">
       <c r="L27" t="str">
         <v>EmitEdgarAgSO2</v>
       </c>
@@ -2322,7 +2340,7 @@
         <v>Edgar Air Gen SO2</v>
       </c>
     </row>
-    <row r="28" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="12:22">
       <c r="L28" t="str">
         <v>EmitEdgarNonagSO2</v>
       </c>
@@ -2330,7 +2348,7 @@
         <v>EmitEdgarNonagSO2</v>
       </c>
     </row>
-    <row r="29" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="12:22">
       <c r="L29" t="str">
         <v>EmitEdgarGenNH3</v>
       </c>
@@ -2338,7 +2356,7 @@
         <v>EmitEdgarGenNH3</v>
       </c>
     </row>
-    <row r="30" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="12:22">
       <c r="L30" t="str">
         <v>EmitEdgarGenNOx</v>
       </c>
@@ -2346,7 +2364,7 @@
         <v>EmitEdgarGenNOx</v>
       </c>
     </row>
-    <row r="31" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="12:22">
       <c r="L31" t="str">
         <v>EmitEdgarGenSO2</v>
       </c>
@@ -2354,42 +2372,42 @@
         <v>EmitEdgarGenSO2</v>
       </c>
     </row>
-    <row r="32" spans="12:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="12:22">
       <c r="L32" t="str">
         <v>file_FF_NOx</v>
       </c>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="12:12">
       <c r="L33" t="str">
         <v>file_FF_NHx</v>
       </c>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="12:12">
       <c r="L34" t="str">
         <v>file_FF_SOx</v>
       </c>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="12:12">
       <c r="L35" t="str">
         <v>ecoreg_RFs_NH4_Lebrun</v>
       </c>
     </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="12:12">
       <c r="L36" t="str">
         <v>ecoreg_RFs_NO3_Lebrun</v>
       </c>
     </row>
-    <row r="37" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="12:12">
       <c r="L37" t="str">
         <v>ecoreg_RFs_SO4_Lebrun</v>
       </c>
     </row>
-    <row r="38" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="12:12">
       <c r="L38" t="str">
         <v>ecoreg_EFs_Gade</v>
       </c>
     </row>
-    <row r="39" spans="12:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="12:12">
       <c r="L39" t="str">
         <v>ecoreg_GEPs</v>
       </c>
@@ -2401,59 +2419,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2502FB-B45F-43BB-8645-D93E9F9C6CDF}">
-  <dimension ref="B2:O132"/>
+  <dimension ref="B2:O135"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="42.109375" customWidth="1"/>
-    <col min="3" max="3" width="26.5546875" customWidth="1"/>
-    <col min="4" max="4" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="42.125" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="44.625" customWidth="1"/>
     <col min="5" max="5" width="58" customWidth="1"/>
-    <col min="6" max="6" width="31.44140625" customWidth="1"/>
-    <col min="7" max="7" width="68.5546875" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" customWidth="1"/>
-    <col min="9" max="9" width="23.5546875" customWidth="1"/>
-    <col min="10" max="10" width="22.88671875" customWidth="1"/>
-    <col min="11" max="11" width="32.44140625" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" customWidth="1"/>
+    <col min="6" max="6" width="31.5" customWidth="1"/>
+    <col min="7" max="7" width="68.5" customWidth="1"/>
+    <col min="8" max="8" width="18.625" customWidth="1"/>
+    <col min="9" max="9" width="23.5" customWidth="1"/>
+    <col min="10" max="10" width="22.875" customWidth="1"/>
+    <col min="11" max="11" width="32.5" customWidth="1"/>
+    <col min="12" max="12" width="21.5" customWidth="1"/>
     <col min="13" max="13" width="28" customWidth="1"/>
-    <col min="14" max="14" width="37.33203125" customWidth="1"/>
-    <col min="15" max="15" width="11.88671875" customWidth="1"/>
-    <col min="16" max="16" width="16.88671875" customWidth="1"/>
-    <col min="17" max="17" width="19.6640625" customWidth="1"/>
+    <col min="14" max="14" width="37.375" customWidth="1"/>
+    <col min="15" max="15" width="11.875" customWidth="1"/>
+    <col min="16" max="16" width="16.875" customWidth="1"/>
+    <col min="17" max="17" width="19.625" customWidth="1"/>
     <col min="18" max="22" width="18" customWidth="1"/>
-    <col min="23" max="23" width="14.88671875" customWidth="1"/>
-    <col min="24" max="24" width="19.5546875" customWidth="1"/>
-    <col min="25" max="26" width="23.44140625" customWidth="1"/>
-    <col min="27" max="28" width="20.109375" customWidth="1"/>
-    <col min="29" max="29" width="10.33203125" customWidth="1"/>
-    <col min="31" max="31" width="14.88671875" customWidth="1"/>
-    <col min="32" max="32" width="18.5546875" customWidth="1"/>
-    <col min="33" max="33" width="11.88671875" customWidth="1"/>
-    <col min="34" max="34" width="15.5546875" customWidth="1"/>
-    <col min="35" max="35" width="23.44140625" customWidth="1"/>
-    <col min="36" max="36" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.44140625" customWidth="1"/>
+    <col min="23" max="23" width="14.875" customWidth="1"/>
+    <col min="24" max="24" width="19.5" customWidth="1"/>
+    <col min="25" max="26" width="23.5" customWidth="1"/>
+    <col min="27" max="28" width="20.125" customWidth="1"/>
+    <col min="29" max="29" width="10.375" customWidth="1"/>
+    <col min="31" max="31" width="14.875" customWidth="1"/>
+    <col min="32" max="32" width="18.5" customWidth="1"/>
+    <col min="33" max="33" width="11.875" customWidth="1"/>
+    <col min="34" max="34" width="15.5" customWidth="1"/>
+    <col min="35" max="35" width="23.5" customWidth="1"/>
+    <col min="36" max="36" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:14">
       <c r="E2" t="s">
         <v>93</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="B4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:14">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2494,7 +2512,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:14">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -2503,11 +2521,11 @@
       </c>
       <c r="E6" t="str" cm="1">
         <f t="array" ref="E6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F6" t="str" cm="1">
         <f t="array" ref="F6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G6" t="str" cm="1">
         <f t="array" ref="G6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2533,10 +2551,10 @@
       </c>
       <c r="M6" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
       <c r="B7" t="s">
         <v>266</v>
       </c>
@@ -2575,7 +2593,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14">
       <c r="B8" t="s">
         <v>268</v>
       </c>
@@ -2608,7 +2626,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14">
       <c r="B9" t="s">
         <v>263</v>
       </c>
@@ -2641,7 +2659,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14">
       <c r="B10" t="s">
         <v>254</v>
       </c>
@@ -2676,7 +2694,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14">
       <c r="B11" t="s">
         <v>255</v>
       </c>
@@ -2711,7 +2729,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14">
       <c r="B12" t="s">
         <v>256</v>
       </c>
@@ -2747,7 +2765,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:14">
       <c r="B13" t="s">
         <v>257</v>
       </c>
@@ -2783,7 +2801,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:14">
       <c r="B14" t="s">
         <v>250</v>
       </c>
@@ -2796,7 +2814,7 @@
       </c>
       <c r="F14" t="str" cm="1">
         <f t="array" ref="F14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>anthro_compiled_v01</v>
+        <v/>
       </c>
       <c r="G14" t="str" cm="1">
         <f t="array" ref="G14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2816,10 +2834,10 @@
       </c>
       <c r="M14" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\anthro_compiled_v01</v>
-      </c>
-    </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14">
       <c r="B15" t="s">
         <v>251</v>
       </c>
@@ -2855,7 +2873,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:14">
       <c r="B16" t="s">
         <v>29</v>
       </c>
@@ -2864,11 +2882,11 @@
       </c>
       <c r="E16" t="str" cm="1">
         <f t="array" ref="E16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F16" t="str" cm="1">
         <f t="array" ref="F16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G16" t="str" cm="1">
         <f t="array" ref="G16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2891,10 +2909,10 @@
       </c>
       <c r="M16" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13">
       <c r="B17" t="s">
         <v>30</v>
       </c>
@@ -2903,11 +2921,11 @@
       </c>
       <c r="E17" t="str" cm="1">
         <f t="array" ref="E17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F17" t="str" cm="1">
         <f t="array" ref="F17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G17" t="str" cm="1">
         <f t="array" ref="G17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2933,10 +2951,10 @@
       </c>
       <c r="M17" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13">
       <c r="B18" t="s">
         <v>39</v>
       </c>
@@ -2945,7 +2963,7 @@
       </c>
       <c r="E18" t="str" cm="1">
         <f t="array" ref="E18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>W:\data\geo\ecoregions_teow\Olson_2012\official</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F18" t="str" cm="1">
         <f t="array" ref="F18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2972,10 +2990,10 @@
       </c>
       <c r="M18" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>W:\data\geo\ecoregions_teow\Olson_2012\official\</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19" t="s">
         <v>31</v>
       </c>
@@ -2984,11 +3002,11 @@
       </c>
       <c r="E19" t="str" cm="1">
         <f t="array" ref="E19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F19" t="str" cm="1">
         <f t="array" ref="F19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G19" t="str" cm="1">
         <f t="array" ref="G19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3008,10 +3026,10 @@
       </c>
       <c r="M19" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13">
       <c r="B20" t="s">
         <v>32</v>
       </c>
@@ -3020,11 +3038,11 @@
       </c>
       <c r="E20" t="str" cm="1">
         <f t="array" ref="E20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F20" t="str" cm="1">
         <f t="array" ref="F20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G20" t="str" cm="1">
         <f t="array" ref="G20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3044,10 +3062,10 @@
       </c>
       <c r="M20" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
       <c r="B21" t="s">
         <v>33</v>
       </c>
@@ -3056,11 +3074,11 @@
       </c>
       <c r="E21" t="str" cm="1">
         <f t="array" ref="E21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F21" t="str" cm="1">
         <f t="array" ref="F21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G21" t="str" cm="1">
         <f t="array" ref="G21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3080,10 +3098,10 @@
       </c>
       <c r="M21" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22" t="s">
         <v>34</v>
       </c>
@@ -3092,11 +3110,11 @@
       </c>
       <c r="E22" t="str" cm="1">
         <f t="array" ref="E22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F22" t="str" cm="1">
         <f t="array" ref="F22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G22" t="str" cm="1">
         <f t="array" ref="G22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3116,10 +3134,10 @@
       </c>
       <c r="M22" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
       <c r="B23" t="s">
         <v>35</v>
       </c>
@@ -3128,11 +3146,11 @@
       </c>
       <c r="E23" t="str" cm="1">
         <f t="array" ref="E23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F23" t="str" cm="1">
         <f t="array" ref="F23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G23" t="str" cm="1">
         <f t="array" ref="G23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3152,10 +3170,10 @@
       </c>
       <c r="M23" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13">
       <c r="B24" t="s">
         <v>36</v>
       </c>
@@ -3164,11 +3182,11 @@
       </c>
       <c r="E24" t="str" cm="1">
         <f t="array" ref="E24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F24" t="str" cm="1">
         <f t="array" ref="F24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G24" t="str" cm="1">
         <f t="array" ref="G24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3188,10 +3206,10 @@
       </c>
       <c r="M24" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
       <c r="B25" t="s">
         <v>37</v>
       </c>
@@ -3200,11 +3218,11 @@
       </c>
       <c r="E25" t="str" cm="1">
         <f t="array" ref="E25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F25" t="str" cm="1">
         <f t="array" ref="F25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G25" t="str" cm="1">
         <f t="array" ref="G25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3224,10 +3242,10 @@
       </c>
       <c r="M25" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13">
       <c r="B26" t="s">
         <v>38</v>
       </c>
@@ -3236,11 +3254,11 @@
       </c>
       <c r="E26" t="str" cm="1">
         <f t="array" ref="E26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F26" t="str" cm="1">
         <f t="array" ref="F26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G26" t="str" cm="1">
         <f t="array" ref="G26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3260,10 +3278,10 @@
       </c>
       <c r="M26" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13">
       <c r="B27" t="s">
         <v>226</v>
       </c>
@@ -3272,7 +3290,7 @@
       </c>
       <c r="E27" t="str" cm="1">
         <f t="array" ref="E27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F27" t="str" cm="1">
         <f t="array" ref="F27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3294,10 +3312,10 @@
       </c>
       <c r="M27" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13">
       <c r="B28" t="s">
         <v>227</v>
       </c>
@@ -3306,7 +3324,7 @@
       </c>
       <c r="E28" t="str" cm="1">
         <f t="array" ref="E28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F28" t="str" cm="1">
         <f t="array" ref="F28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3328,10 +3346,10 @@
       </c>
       <c r="M28" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
       <c r="B29" t="s">
         <v>228</v>
       </c>
@@ -3340,7 +3358,7 @@
       </c>
       <c r="E29" t="str" cm="1">
         <f t="array" ref="E29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F29" t="str" cm="1">
         <f t="array" ref="F29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3362,10 +3380,10 @@
       </c>
       <c r="M29" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13">
       <c r="B30" t="s">
         <v>191</v>
       </c>
@@ -3374,7 +3392,7 @@
       </c>
       <c r="E30" t="str" cm="1">
         <f t="array" ref="E30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F30" t="str" cm="1">
         <f t="array" ref="F30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3395,10 +3413,10 @@
       </c>
       <c r="M30" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13">
       <c r="B31" t="s">
         <v>192</v>
       </c>
@@ -3407,7 +3425,7 @@
       </c>
       <c r="E31" t="str" cm="1">
         <f t="array" ref="E31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F31" t="str" cm="1">
         <f t="array" ref="F31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3428,10 +3446,10 @@
       </c>
       <c r="M31" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13">
       <c r="B32" t="s">
         <v>193</v>
       </c>
@@ -3440,7 +3458,7 @@
       </c>
       <c r="E32" t="str" cm="1">
         <f t="array" ref="E32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F32" t="str" cm="1">
         <f t="array" ref="F32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3461,10 +3479,10 @@
       </c>
       <c r="M32" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15">
       <c r="B33" t="s">
         <v>141</v>
       </c>
@@ -3473,7 +3491,7 @@
       </c>
       <c r="E33" t="str" cm="1">
         <f t="array" ref="E33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F33" t="str" cm="1">
         <f t="array" ref="F33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3494,10 +3512,10 @@
       </c>
       <c r="M33" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15">
       <c r="B34" t="s">
         <v>143</v>
       </c>
@@ -3506,7 +3524,7 @@
       </c>
       <c r="E34" t="str" cm="1">
         <f t="array" ref="E34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F34" t="str" cm="1">
         <f t="array" ref="F34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3527,10 +3545,10 @@
       </c>
       <c r="M34" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15">
       <c r="B35" t="s">
         <v>142</v>
       </c>
@@ -3539,7 +3557,7 @@
       </c>
       <c r="E35" t="str" cm="1">
         <f t="array" ref="E35">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F35" t="str" cm="1">
         <f t="array" ref="F35">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3560,10 +3578,10 @@
       </c>
       <c r="M35" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15">
       <c r="B36" t="s">
         <v>57</v>
       </c>
@@ -3572,7 +3590,7 @@
       </c>
       <c r="E36" t="str" cm="1">
         <f t="array" ref="E36">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F36" t="str" cm="1">
         <f t="array" ref="F36">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3593,10 +3611,10 @@
       </c>
       <c r="M36" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15">
       <c r="B37" t="s">
         <v>50</v>
       </c>
@@ -3605,7 +3623,7 @@
       </c>
       <c r="E37" t="str" cm="1">
         <f t="array" ref="E37">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F37" t="str" cm="1">
         <f t="array" ref="F37">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3626,15 +3644,15 @@
       </c>
       <c r="M37" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.3">
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15">
       <c r="B43" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:15">
       <c r="B44" s="3" t="s">
         <v>42</v>
       </c>
@@ -3678,7 +3696,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:15">
       <c r="B45" t="s">
         <v>46</v>
       </c>
@@ -3702,7 +3720,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:15">
       <c r="B46" t="s">
         <v>47</v>
       </c>
@@ -3726,7 +3744,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:15">
       <c r="B47" t="s">
         <v>48</v>
       </c>
@@ -3750,7 +3768,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:15">
       <c r="B48" t="s">
         <v>49</v>
       </c>
@@ -3777,7 +3795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:12">
       <c r="B49" t="s">
         <v>50</v>
       </c>
@@ -3804,7 +3822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:12">
       <c r="B50" t="s">
         <v>151</v>
       </c>
@@ -3831,7 +3849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:12">
       <c r="B51" t="s">
         <v>152</v>
       </c>
@@ -3858,7 +3876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:12">
       <c r="B52" t="s">
         <v>153</v>
       </c>
@@ -3885,7 +3903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:12">
       <c r="B53" t="s">
         <v>250</v>
       </c>
@@ -3912,7 +3930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:12">
       <c r="B54" t="s">
         <v>251</v>
       </c>
@@ -3939,7 +3957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:12">
       <c r="B55" t="s">
         <v>32</v>
       </c>
@@ -3966,7 +3984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:12">
       <c r="B56" t="s">
         <v>51</v>
       </c>
@@ -3993,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:12">
       <c r="B57" t="s">
         <v>52</v>
       </c>
@@ -4020,7 +4038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:12">
       <c r="B58" t="s">
         <v>53</v>
       </c>
@@ -4047,7 +4065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:12">
       <c r="B59" t="s">
         <v>54</v>
       </c>
@@ -4074,7 +4092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:12">
       <c r="B60" t="s">
         <v>55</v>
       </c>
@@ -4101,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:12">
       <c r="B61" t="s">
         <v>56</v>
       </c>
@@ -4128,7 +4146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:12">
       <c r="B62" t="s">
         <v>223</v>
       </c>
@@ -4155,7 +4173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:12">
       <c r="B63" t="s">
         <v>225</v>
       </c>
@@ -4182,7 +4200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:12">
       <c r="B64" t="s">
         <v>224</v>
       </c>
@@ -4209,12 +4227,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:7">
       <c r="B70" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:7">
       <c r="B71" t="s">
         <v>71</v>
       </c>
@@ -4234,7 +4252,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:7">
       <c r="B72" t="s">
         <v>28</v>
       </c>
@@ -4254,7 +4272,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:7">
       <c r="B73" t="s">
         <v>266</v>
       </c>
@@ -4271,7 +4289,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:7">
       <c r="B74" t="s">
         <v>268</v>
       </c>
@@ -4288,7 +4306,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:7">
       <c r="B75" t="s">
         <v>263</v>
       </c>
@@ -4305,7 +4323,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:7">
       <c r="B76" t="s">
         <v>254</v>
       </c>
@@ -4322,7 +4340,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:7">
       <c r="B77" t="s">
         <v>255</v>
       </c>
@@ -4339,7 +4357,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:7">
       <c r="B78" t="s">
         <v>256</v>
       </c>
@@ -4356,7 +4374,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:7">
       <c r="B79" t="s">
         <v>257</v>
       </c>
@@ -4373,7 +4391,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:7">
       <c r="B80" t="s">
         <v>250</v>
       </c>
@@ -4393,7 +4411,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:7">
       <c r="B81" t="s">
         <v>251</v>
       </c>
@@ -4410,7 +4428,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:7">
       <c r="B82" t="s">
         <v>29</v>
       </c>
@@ -4430,7 +4448,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:7">
       <c r="B83" t="s">
         <v>30</v>
       </c>
@@ -4450,7 +4468,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:7">
       <c r="B84" t="s">
         <v>39</v>
       </c>
@@ -4467,7 +4485,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:7">
       <c r="B85" t="s">
         <v>31</v>
       </c>
@@ -4487,7 +4505,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:7">
       <c r="B86" t="s">
         <v>32</v>
       </c>
@@ -4507,7 +4525,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:7">
       <c r="B87" t="s">
         <v>33</v>
       </c>
@@ -4527,7 +4545,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:7">
       <c r="B88" t="s">
         <v>34</v>
       </c>
@@ -4547,7 +4565,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:7">
       <c r="B89" t="s">
         <v>35</v>
       </c>
@@ -4567,7 +4585,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:7">
       <c r="B90" t="s">
         <v>36</v>
       </c>
@@ -4587,7 +4605,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:7">
       <c r="B91" t="s">
         <v>37</v>
       </c>
@@ -4607,7 +4625,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:7">
       <c r="B92" t="s">
         <v>38</v>
       </c>
@@ -4627,7 +4645,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:7">
       <c r="B93" t="s">
         <v>226</v>
       </c>
@@ -4644,7 +4662,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:7">
       <c r="B94" t="s">
         <v>227</v>
       </c>
@@ -4661,7 +4679,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:7">
       <c r="B95" t="s">
         <v>228</v>
       </c>
@@ -4678,7 +4696,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:7">
       <c r="B96" t="s">
         <v>191</v>
       </c>
@@ -4695,7 +4713,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:7">
       <c r="B97" t="s">
         <v>192</v>
       </c>
@@ -4712,7 +4730,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:7">
       <c r="B98" t="s">
         <v>193</v>
       </c>
@@ -4729,7 +4747,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:7">
       <c r="B99" t="s">
         <v>141</v>
       </c>
@@ -4746,7 +4764,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:7">
       <c r="B100" t="s">
         <v>143</v>
       </c>
@@ -4763,7 +4781,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:7">
       <c r="B101" t="s">
         <v>142</v>
       </c>
@@ -4780,7 +4798,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:7">
       <c r="B102" t="s">
         <v>57</v>
       </c>
@@ -4797,7 +4815,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:7">
       <c r="B103" t="s">
         <v>50</v>
       </c>
@@ -4814,7 +4832,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:7">
       <c r="B104" s="13" t="s">
         <v>28</v>
       </c>
@@ -4832,63 +4850,63 @@
         <v>76</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:7">
       <c r="B105" s="13" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="C105" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D105" s="13" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E105" s="13"/>
       <c r="F105" s="13" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
       <c r="G105" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:7">
       <c r="B106" s="13" t="s">
-        <v>255</v>
+        <v>268</v>
       </c>
       <c r="C106" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D106" s="13" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E106" s="13"/>
       <c r="F106" s="13" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="G106" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:7">
       <c r="B107" s="13" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="C107" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D107" s="13" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E107" s="13"/>
       <c r="F107" s="13" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="G107" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:7">
       <c r="B108" s="13" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C108" s="13" t="s">
         <v>220</v>
@@ -4898,105 +4916,105 @@
       </c>
       <c r="E108" s="13"/>
       <c r="F108" s="13" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G108" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:7">
       <c r="B109" s="13" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C109" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D109" s="13" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="E109" s="13"/>
       <c r="F109" s="13" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="G109" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:7">
       <c r="B110" s="13" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="C110" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D110" s="13" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="E110" s="13"/>
       <c r="F110" s="13" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="G110" s="13" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="111" spans="2:7">
       <c r="B111" s="13" t="s">
-        <v>29</v>
+        <v>257</v>
       </c>
       <c r="C111" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D111" s="13" t="s">
-        <v>221</v>
+        <v>258</v>
       </c>
       <c r="E111" s="13"/>
       <c r="F111" s="13" t="s">
-        <v>80</v>
+        <v>262</v>
       </c>
       <c r="G111" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="112" spans="2:7">
       <c r="B112" s="13" t="s">
-        <v>30</v>
+        <v>250</v>
       </c>
       <c r="C112" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D112" s="13" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="E112" s="13"/>
       <c r="F112" s="13" t="s">
-        <v>81</v>
+        <v>249</v>
       </c>
       <c r="G112" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.3">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="113" spans="2:7">
       <c r="B113" s="13" t="s">
-        <v>39</v>
+        <v>251</v>
       </c>
       <c r="C113" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D113" s="13" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="E113" s="13"/>
       <c r="F113" s="13" t="s">
-        <v>75</v>
+        <v>249</v>
       </c>
       <c r="G113" s="13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.3">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="114" spans="2:7">
       <c r="B114" s="13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C114" s="13" t="s">
         <v>220</v>
@@ -5006,15 +5024,15 @@
       </c>
       <c r="E114" s="13"/>
       <c r="F114" s="13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G114" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:7">
       <c r="B115" s="13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C115" s="13" t="s">
         <v>220</v>
@@ -5024,15 +5042,15 @@
       </c>
       <c r="E115" s="13"/>
       <c r="F115" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G115" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:7">
       <c r="B116" s="13" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C116" s="13" t="s">
         <v>220</v>
@@ -5042,15 +5060,15 @@
       </c>
       <c r="E116" s="13"/>
       <c r="F116" s="13" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="G116" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:7">
       <c r="B117" s="13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C117" s="13" t="s">
         <v>220</v>
@@ -5060,15 +5078,15 @@
       </c>
       <c r="E117" s="13"/>
       <c r="F117" s="13" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="G117" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:7">
       <c r="B118" s="13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C118" s="13" t="s">
         <v>220</v>
@@ -5078,15 +5096,15 @@
       </c>
       <c r="E118" s="13"/>
       <c r="F118" s="13" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="G118" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:7">
       <c r="B119" s="13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C119" s="13" t="s">
         <v>220</v>
@@ -5096,15 +5114,15 @@
       </c>
       <c r="E119" s="13"/>
       <c r="F119" s="13" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="G119" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:7">
       <c r="B120" s="13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C120" s="13" t="s">
         <v>220</v>
@@ -5114,15 +5132,15 @@
       </c>
       <c r="E120" s="13"/>
       <c r="F120" s="13" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G120" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:7">
       <c r="B121" s="13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C121" s="13" t="s">
         <v>220</v>
@@ -5132,15 +5150,15 @@
       </c>
       <c r="E121" s="13"/>
       <c r="F121" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G121" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:7">
       <c r="B122" s="13" t="s">
-        <v>226</v>
+        <v>36</v>
       </c>
       <c r="C122" s="13" t="s">
         <v>220</v>
@@ -5150,15 +5168,15 @@
       </c>
       <c r="E122" s="13"/>
       <c r="F122" s="13" t="s">
-        <v>229</v>
+        <v>87</v>
       </c>
       <c r="G122" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:7">
       <c r="B123" s="13" t="s">
-        <v>227</v>
+        <v>37</v>
       </c>
       <c r="C123" s="13" t="s">
         <v>220</v>
@@ -5168,15 +5186,15 @@
       </c>
       <c r="E123" s="13"/>
       <c r="F123" s="13" t="s">
-        <v>230</v>
+        <v>88</v>
       </c>
       <c r="G123" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:7">
       <c r="B124" s="13" t="s">
-        <v>228</v>
+        <v>38</v>
       </c>
       <c r="C124" s="13" t="s">
         <v>220</v>
@@ -5186,15 +5204,15 @@
       </c>
       <c r="E124" s="13"/>
       <c r="F124" s="13" t="s">
-        <v>231</v>
+        <v>89</v>
       </c>
       <c r="G124" s="13" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:7">
       <c r="B125" s="13" t="s">
-        <v>191</v>
+        <v>226</v>
       </c>
       <c r="C125" s="13" t="s">
         <v>220</v>
@@ -5204,15 +5222,15 @@
       </c>
       <c r="E125" s="13"/>
       <c r="F125" s="13" t="s">
-        <v>91</v>
+        <v>229</v>
       </c>
       <c r="G125" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="126" spans="2:7">
       <c r="B126" s="13" t="s">
-        <v>192</v>
+        <v>227</v>
       </c>
       <c r="C126" s="13" t="s">
         <v>220</v>
@@ -5222,15 +5240,15 @@
       </c>
       <c r="E126" s="13"/>
       <c r="F126" s="13" t="s">
-        <v>90</v>
+        <v>230</v>
       </c>
       <c r="G126" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="127" spans="2:7">
       <c r="B127" s="13" t="s">
-        <v>193</v>
+        <v>228</v>
       </c>
       <c r="C127" s="13" t="s">
         <v>220</v>
@@ -5240,69 +5258,69 @@
       </c>
       <c r="E127" s="13"/>
       <c r="F127" s="13" t="s">
-        <v>140</v>
+        <v>231</v>
       </c>
       <c r="G127" s="13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="128" spans="2:7">
       <c r="B128" s="13" t="s">
-        <v>141</v>
+        <v>191</v>
       </c>
       <c r="C128" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D128" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E128" s="13"/>
       <c r="F128" s="13" t="s">
-        <v>145</v>
+        <v>91</v>
       </c>
       <c r="G128" s="13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="129" spans="2:7">
       <c r="B129" s="13" t="s">
-        <v>143</v>
+        <v>192</v>
       </c>
       <c r="C129" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D129" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E129" s="13"/>
       <c r="F129" s="13" t="s">
-        <v>147</v>
+        <v>90</v>
       </c>
       <c r="G129" s="13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="130" spans="2:7">
       <c r="B130" s="13" t="s">
-        <v>142</v>
+        <v>193</v>
       </c>
       <c r="C130" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D130" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E130" s="13"/>
       <c r="F130" s="13" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="G130" s="13" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="131" spans="2:7">
       <c r="B131" s="13" t="s">
-        <v>57</v>
+        <v>141</v>
       </c>
       <c r="C131" s="13" t="s">
         <v>220</v>
@@ -5312,15 +5330,15 @@
       </c>
       <c r="E131" s="13"/>
       <c r="F131" s="13" t="s">
-        <v>197</v>
+        <v>145</v>
       </c>
       <c r="G131" s="13" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:7">
       <c r="B132" s="13" t="s">
-        <v>50</v>
+        <v>143</v>
       </c>
       <c r="C132" s="13" t="s">
         <v>220</v>
@@ -5330,9 +5348,63 @@
       </c>
       <c r="E132" s="13"/>
       <c r="F132" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="G132" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="133" spans="2:7">
+      <c r="B133" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="C133" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D133" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E133" s="13"/>
+      <c r="F133" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G133" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="134" spans="2:7">
+      <c r="B134" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C134" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D134" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E134" s="13"/>
+      <c r="F134" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="G134" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="135" spans="2:7">
+      <c r="B135" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C135" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D135" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E135" s="13"/>
+      <c r="F135" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="G132" s="13" t="s">
+      <c r="G135" s="13" t="s">
         <v>146</v>
       </c>
     </row>
@@ -5345,7 +5417,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{EA6C777B-C12B-4DA7-8BB7-7DDC99E580DB}">
       <formula1>list.File_Loc.Users</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D45:D64 B72:B132" xr:uid="{89EA6ADA-E6CC-4F9F-8692-D86D51F6962E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D45:D64 B72:B135" xr:uid="{89EA6ADA-E6CC-4F9F-8692-D86D51F6962E}">
       <formula1>list.Files_unique</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M45:M64" xr:uid="{30B9C429-7EFE-4DEB-8979-C009F9C29D27}">
@@ -5380,24 +5452,24 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>102</v>
       </c>
@@ -5423,7 +5495,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>107</v>
       </c>
@@ -5444,7 +5516,7 @@
         <v>10102-43-9</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>202</v>
       </c>
@@ -5465,7 +5537,7 @@
         <v>10102-43-9</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:9">
       <c r="B7" t="s">
         <v>204</v>
       </c>
@@ -5486,7 +5558,7 @@
         <v>10102-44-0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>108</v>
       </c>
@@ -5505,7 +5577,7 @@
         <v>000-00-0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:9">
       <c r="B9" t="s">
         <v>128</v>
       </c>
@@ -5526,7 +5598,7 @@
         <v>7664-41-7</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9">
       <c r="B10" t="s">
         <v>129</v>
       </c>
@@ -5547,7 +5619,7 @@
         <v>14798-03-9</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9">
       <c r="B11" t="s">
         <v>109</v>
       </c>
@@ -5566,7 +5638,7 @@
         <v>000-00-0</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9">
       <c r="B12" t="s">
         <v>132</v>
       </c>
@@ -5587,7 +5659,7 @@
         <v>7446-09-5</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
         <v>135</v>
       </c>
@@ -5625,23 +5697,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1D767F-008E-40CD-A786-127BCF11776D}">
   <dimension ref="B4:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="7" max="7" width="73.109375" customWidth="1"/>
-    <col min="9" max="9" width="17.5546875" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
-    <col min="12" max="12" width="24.109375" customWidth="1"/>
-    <col min="13" max="13" width="29.109375" customWidth="1"/>
+    <col min="7" max="7" width="73.125" customWidth="1"/>
+    <col min="9" max="9" width="17.5" customWidth="1"/>
+    <col min="10" max="10" width="20.875" customWidth="1"/>
+    <col min="11" max="11" width="16.375" customWidth="1"/>
+    <col min="12" max="12" width="24.125" customWidth="1"/>
+    <col min="13" max="13" width="29.125" customWidth="1"/>
     <col min="14" max="14" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:14">
       <c r="B4" t="s">
         <v>137</v>
       </c>
@@ -5650,7 +5722,7 @@
         <v>'STM2_newEmit_Orig-Arch_test_New-Country_test', 'STM3_newEmit_Orig-Arch_test_New-Country_test_Pop2010', 'STM2_newEmit_Orig-Arch_test_split_New-Countries', 'STM2_newEmit_Orig-Arch_test_New-Countries'</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:14">
       <c r="B7" t="s">
         <v>58</v>
       </c>
@@ -5658,7 +5730,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:14">
       <c r="B8" t="s">
         <v>59</v>
       </c>
@@ -5699,7 +5771,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:14">
       <c r="B9" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM2_newEmit_Orig-Arch_test_New-Country_test</v>
@@ -5731,7 +5803,7 @@
         <v>STM2_newEmit_Orig-Arch_test_New-Country_test</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:14">
       <c r="B10" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM3_newEmit_Orig-Arch_test_New-Country_test_Pop2010</v>
@@ -5766,7 +5838,7 @@
         <v>STM3_newEmit_Orig-Arch_test_New-Country_test_Pop2010</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:14">
       <c r="B11" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM2_newEmit_Orig-Arch_test_split_New-Countries</v>
@@ -5798,7 +5870,7 @@
         <v>STM2_newEmit_Orig-Arch_test_split_New-Countries</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:14">
       <c r="B12" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM2_newEmit_Orig-Arch_test_New-Countries</v>
@@ -5862,47 +5934,47 @@
       <selection activeCell="AE24" sqref="AE24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.375" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" customWidth="1"/>
-    <col min="8" max="8" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.375" customWidth="1"/>
+    <col min="8" max="8" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.375" customWidth="1"/>
+    <col min="10" max="10" width="13.625" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="29.109375" customWidth="1"/>
-    <col min="13" max="13" width="22.109375" customWidth="1"/>
-    <col min="14" max="15" width="17.6640625" customWidth="1"/>
-    <col min="16" max="16" width="34.6640625" customWidth="1"/>
-    <col min="17" max="17" width="16.44140625" customWidth="1"/>
-    <col min="18" max="18" width="15.5546875" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="29.125" customWidth="1"/>
+    <col min="13" max="13" width="22.125" customWidth="1"/>
+    <col min="14" max="15" width="17.625" customWidth="1"/>
+    <col min="16" max="16" width="34.625" customWidth="1"/>
+    <col min="17" max="17" width="16.5" customWidth="1"/>
+    <col min="18" max="18" width="15.5" customWidth="1"/>
+    <col min="19" max="19" width="14.375" customWidth="1"/>
     <col min="20" max="20" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:24">
       <c r="X3" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:24">
       <c r="X4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:24">
       <c r="X5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:24">
       <c r="X6" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:24">
       <c r="B7" t="s">
         <v>211</v>
       </c>
@@ -5916,7 +5988,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="2:24" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:24" ht="42.75">
       <c r="B8" t="s">
         <v>206</v>
       </c>
@@ -5984,7 +6056,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:24">
       <c r="B9" t="s">
         <v>208</v>
       </c>
@@ -6049,7 +6121,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:24">
       <c r="B10" t="s">
         <v>207</v>
       </c>
@@ -6114,7 +6186,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:24">
       <c r="F11">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6170,7 +6242,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:24">
       <c r="F12">
         <f t="shared" ref="F12:F25" si="1">IFERROR($F11+1,1)</f>
         <v>4</v>
@@ -6226,7 +6298,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:24">
       <c r="F13">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -6282,7 +6354,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:24">
       <c r="F14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -6338,7 +6410,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:24">
       <c r="F15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -6394,7 +6466,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:24">
       <c r="F16">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -6450,7 +6522,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:24">
       <c r="F17">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -6506,7 +6578,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:24">
       <c r="F18">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -6564,7 +6636,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:24">
       <c r="F19">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -6622,7 +6694,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:24">
       <c r="F20">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -6680,7 +6752,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:24">
       <c r="F21">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -6732,7 +6804,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:24">
       <c r="F22">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -6784,7 +6856,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:24">
       <c r="F23">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -6836,7 +6908,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:24">
       <c r="F24">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -6888,7 +6960,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:24">
       <c r="F25">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -6940,7 +7012,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="6:24">
       <c r="F26">
         <f t="shared" ref="F26:F53" si="2">IFERROR($F25+1,1)</f>
         <v>18</v>
@@ -6992,7 +7064,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="6:24">
       <c r="F27">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -7050,7 +7122,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="6:24">
       <c r="F28">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -7108,7 +7180,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="6:24">
       <c r="F29">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -7166,7 +7238,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="6:24">
       <c r="F30">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -7218,7 +7290,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="6:24">
       <c r="F31">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -7270,7 +7342,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="6:24">
       <c r="F32">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -7322,7 +7394,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="33" spans="6:24">
       <c r="F33">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -7374,7 +7446,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="34" spans="6:24">
       <c r="F34">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -7426,7 +7498,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="35" spans="6:24">
       <c r="F35">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -7478,7 +7550,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="36" spans="6:24">
       <c r="F36">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -7536,7 +7608,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="37" spans="6:24">
       <c r="F37">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -7594,7 +7666,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="38" spans="6:24">
       <c r="F38">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -7652,7 +7724,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="39" spans="6:24">
       <c r="F39">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -7704,7 +7776,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="40" spans="6:24">
       <c r="F40">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -7756,7 +7828,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="41" spans="6:24">
       <c r="F41">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -7808,7 +7880,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="42" spans="6:24">
       <c r="F42">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -7860,7 +7932,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="43" spans="6:24">
       <c r="F43">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -7912,7 +7984,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="44" spans="6:24">
       <c r="F44">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -7964,7 +8036,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="45" spans="6:24">
       <c r="F45">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -8022,7 +8094,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="46" spans="6:24">
       <c r="F46">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -8080,7 +8152,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="47" spans="6:24">
       <c r="F47">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -8138,7 +8210,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="48" spans="6:24">
       <c r="F48">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -8190,7 +8262,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="49" spans="6:24">
       <c r="F49">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -8242,7 +8314,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="50" spans="6:24">
       <c r="F50">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -8294,7 +8366,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="51" spans="6:24">
       <c r="F51">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -8346,7 +8418,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="52" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="52" spans="6:24">
       <c r="F52">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -8398,7 +8470,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="53" spans="6:24">
       <c r="F53">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -8450,7 +8522,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="54" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="54" spans="6:24">
       <c r="F54">
         <f t="shared" ref="F54:F71" si="3">IFERROR($F53+1,1)</f>
         <v>46</v>
@@ -8508,7 +8580,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="55" spans="6:24">
       <c r="F55">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -8566,7 +8638,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="56" spans="6:24">
       <c r="F56">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -8624,7 +8696,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="57" spans="6:24">
       <c r="F57">
         <f t="shared" si="3"/>
         <v>49</v>
@@ -8676,7 +8748,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="58" spans="6:24">
       <c r="F58">
         <f t="shared" si="3"/>
         <v>50</v>
@@ -8728,7 +8800,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="59" spans="6:24">
       <c r="F59">
         <f t="shared" si="3"/>
         <v>51</v>
@@ -8780,7 +8852,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="60" spans="6:24">
       <c r="F60">
         <f t="shared" si="3"/>
         <v>52</v>
@@ -8832,7 +8904,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="61" spans="6:24">
       <c r="F61">
         <f t="shared" si="3"/>
         <v>53</v>
@@ -8884,7 +8956,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="62" spans="6:24">
       <c r="F62">
         <f t="shared" si="3"/>
         <v>54</v>
@@ -8936,7 +9008,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="63" spans="6:24">
       <c r="F63">
         <f t="shared" si="3"/>
         <v>55</v>
@@ -8994,7 +9066,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="64" spans="6:24">
       <c r="F64">
         <f t="shared" si="3"/>
         <v>56</v>
@@ -9052,7 +9124,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:24">
       <c r="F65">
         <f t="shared" si="3"/>
         <v>57</v>
@@ -9110,7 +9182,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="66" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="66" spans="6:24">
       <c r="F66">
         <f t="shared" si="3"/>
         <v>58</v>
@@ -9162,7 +9234,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="67" spans="6:24">
       <c r="F67">
         <f t="shared" si="3"/>
         <v>59</v>
@@ -9214,7 +9286,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="68" spans="6:24">
       <c r="F68">
         <f t="shared" si="3"/>
         <v>60</v>
@@ -9266,7 +9338,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="69" spans="6:24">
       <c r="F69">
         <f t="shared" si="3"/>
         <v>61</v>
@@ -9318,7 +9390,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="70" spans="6:24">
       <c r="F70">
         <f t="shared" si="3"/>
         <v>62</v>
@@ -9370,7 +9442,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="71" spans="6:24" x14ac:dyDescent="0.3">
+    <row r="71" spans="6:24">
       <c r="F71">
         <f t="shared" si="3"/>
         <v>63</v>

</xml_diff>

<commit_message>
some cleaning.  With overlay using "intersection" instead of "union", this is much faster.
</commit_message>
<xml_diff>
--- a/calc/ozone STM calc setup v00a.xlsx
+++ b/calc/ozone STM calc setup v00a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CalcDir\TRACI_ozone_stm\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83AE523C-E9A9-41D3-AC7B-67D4E10E1D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ABCD94C-9C1B-46C8-AAAF-24932CA93F1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -91,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F44" authorId="1" shapeId="0" xr:uid="{C05BA83B-E4CC-4E37-B576-FA3EC5396FF7}">
+    <comment ref="F45" authorId="1" shapeId="0" xr:uid="{C05BA83B-E4CC-4E37-B576-FA3EC5396FF7}">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1532" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1556" uniqueCount="277">
   <si>
     <t>File unique name</t>
   </si>
@@ -963,6 +963,24 @@
   </si>
   <si>
     <t>archID</t>
+  </si>
+  <si>
+    <t>ArchFullUrb2v02_prep01</t>
+  </si>
+  <si>
+    <t>repair1_holes10</t>
+  </si>
+  <si>
+    <t>all unique</t>
+  </si>
+  <si>
+    <t>with intersect</t>
+  </si>
+  <si>
+    <t>with union</t>
+  </si>
+  <si>
+    <t>minutes to multiintersect</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1115,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -1134,6 +1152,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1353,8 +1374,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3314417B-F764-4167-BACA-D8DB10DBD85A}" name="Tbl.Files" displayName="Tbl.Files" ref="B5:N37" totalsRowShown="0" headerRowDxfId="12">
-  <autoFilter ref="B5:N37" xr:uid="{3314417B-F764-4167-BACA-D8DB10DBD85A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3314417B-F764-4167-BACA-D8DB10DBD85A}" name="Tbl.Files" displayName="Tbl.Files" ref="B5:N38" totalsRowShown="0" headerRowDxfId="12">
+  <autoFilter ref="B5:N38" xr:uid="{3314417B-F764-4167-BACA-D8DB10DBD85A}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{6573F11A-0113-4248-BCA3-668BD2869F2D}" name="File unique name"/>
     <tableColumn id="6" xr3:uid="{0DD677F2-77B6-4C2B-AE61-A37A1F44E783}" name="Description"/>
@@ -1377,8 +1398,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2ED9DF3D-9218-45CC-B7DB-14E8EBAB8D85}" name="Tbl.Data" displayName="Tbl.Data" ref="B44:O64" totalsRowShown="0" headerRowDxfId="6">
-  <autoFilter ref="B44:O64" xr:uid="{2ED9DF3D-9218-45CC-B7DB-14E8EBAB8D85}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2ED9DF3D-9218-45CC-B7DB-14E8EBAB8D85}" name="Tbl.Data" displayName="Tbl.Data" ref="B45:O65" totalsRowShown="0" headerRowDxfId="6">
+  <autoFilter ref="B45:O65" xr:uid="{2ED9DF3D-9218-45CC-B7DB-14E8EBAB8D85}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{77E233E2-D46F-4939-BE1E-5F8B51BA784B}" name="Data unique name"/>
     <tableColumn id="2" xr3:uid="{F9260F16-FB5A-4EEE-9117-B235FED2A9EA}" name="Description"/>
@@ -1402,8 +1423,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8294B1BA-ABF4-4D80-9C7A-5B7B2E284256}" name="Tbl.File_Locations" displayName="Tbl.File_Locations" ref="B71:G135" totalsRowShown="0">
-  <autoFilter ref="B71:G135" xr:uid="{8294B1BA-ABF4-4D80-9C7A-5B7B2E284256}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{8294B1BA-ABF4-4D80-9C7A-5B7B2E284256}" name="Tbl.File_Locations" displayName="Tbl.File_Locations" ref="B72:G137" totalsRowShown="0">
+  <autoFilter ref="B72:G137" xr:uid="{8294B1BA-ABF4-4D80-9C7A-5B7B2E284256}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{CBD61C72-14BB-4DB4-B8FE-FFBBB16D0157}" name="File Unique Name"/>
     <tableColumn id="2" xr3:uid="{E630A020-07CA-4AA2-A57D-9F15E52AC431}" name="User"/>
@@ -1436,8 +1457,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}" name="Tbl.SpatialTransforms" displayName="Tbl.SpatialTransforms" ref="B8:N12" totalsRowShown="0">
-  <autoFilter ref="B8:N12" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}" name="Tbl.SpatialTransforms" displayName="Tbl.SpatialTransforms" ref="B10:N16" totalsRowShown="0">
+  <autoFilter ref="B10:N16" xr:uid="{DF60613B-B2E8-48B2-AE4F-B39C7018B202}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{87286839-84B9-43B8-B3CC-7A5ACD26A242}" name="STM unique name">
       <calculatedColumnFormula>Tbl.SpatialTransforms[[#This Row],[File name]]</calculatedColumnFormula>
@@ -1840,7 +1861,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F108999-1C6E-4987-A626-6DE03A70D7E6}">
-  <dimension ref="B7:V39"/>
+  <dimension ref="B7:V40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AC25" sqref="AC25"/>
@@ -1950,11 +1971,11 @@
         <v>AH_main</v>
       </c>
       <c r="L8" t="str" cm="1">
-        <f t="array" ref="L8:L39">Tbl.Files[File unique name]</f>
+        <f t="array" ref="L8:L40">Tbl.Files[File unique name]</f>
         <v>Countries</v>
       </c>
       <c r="M8" t="str" cm="1">
-        <f t="array" ref="M8:M31">_xlfn._xlws.FILTER(Tbl.Files[File unique name],Tbl.Files[File structure]=str.file_struct.geo)</f>
+        <f t="array" ref="M8:M32">_xlfn._xlws.FILTER(Tbl.Files[File unique name],Tbl.Files[File structure]=str.file_struct.geo)</f>
         <v>Countries</v>
       </c>
       <c r="N8" t="str" cm="1">
@@ -1962,7 +1983,7 @@
         <v>air_FF_NOx</v>
       </c>
       <c r="O8" t="str" cm="1">
-        <f t="array" ref="O8:O11">Tbl.SpatialTransforms[STM unique name]</f>
+        <f t="array" ref="O8:O13">Tbl.SpatialTransforms[STM unique name]</f>
         <v>STM2_newEmit_Orig-Arch_test_New-Country_test</v>
       </c>
       <c r="Q8" t="str" cm="1">
@@ -2057,16 +2078,16 @@
         <v>214</v>
       </c>
       <c r="L10" t="str">
-        <v>Arch_test_split</v>
+        <v>ArchFullUrb2v02_prep01</v>
       </c>
       <c r="M10" t="str">
-        <v>Arch_test_split</v>
+        <v>ArchFullUrb2v02_prep01</v>
       </c>
       <c r="N10" t="str">
         <v>air_FF_SOx</v>
       </c>
       <c r="O10" t="str">
-        <v>STM2_newEmit_Orig-Arch_test_split_New-Countries</v>
+        <v>STM2_newEmit_Orig-ArchFullUrb2v02_prep01_New-Country_test</v>
       </c>
       <c r="Q10" t="str">
         <v>NO2</v>
@@ -2095,16 +2116,16 @@
         <v>20</v>
       </c>
       <c r="L11" t="str">
-        <v>Arch_test</v>
+        <v>Arch_test_split</v>
       </c>
       <c r="M11" t="str">
-        <v>Arch_test</v>
+        <v>Arch_test_split</v>
       </c>
       <c r="N11" t="str">
         <v>ecoreg_EFs</v>
       </c>
       <c r="O11" t="str">
-        <v>STM2_newEmit_Orig-Arch_test_New-Countries</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Country_test_Pop2010</v>
       </c>
       <c r="Q11" t="str">
         <v>NHx</v>
@@ -2118,13 +2139,16 @@
         <v>21</v>
       </c>
       <c r="L12" t="str">
-        <v>Arch_Full_Urb2_v01</v>
+        <v>Arch_test</v>
       </c>
       <c r="M12" t="str">
-        <v>Arch_Full_Urb2_v01</v>
+        <v>Arch_test</v>
       </c>
       <c r="N12" t="str">
         <v>ecoreg_GEPs</v>
+      </c>
+      <c r="O12" t="str">
+        <v>STM2_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries</v>
       </c>
       <c r="Q12" t="str">
         <v>NH3</v>
@@ -2138,13 +2162,16 @@
         <v>45</v>
       </c>
       <c r="L13" t="str">
-        <v>Arch_Full_Urb3_v01</v>
+        <v>Arch_Full_Urb2_v01</v>
       </c>
       <c r="M13" t="str">
-        <v>Arch_Full_Urb3_v01</v>
+        <v>Arch_Full_Urb2_v01</v>
       </c>
       <c r="N13" t="str">
         <v>soil_RFs_NH4</v>
+      </c>
+      <c r="O13" t="str">
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
       </c>
       <c r="Q13" t="str">
         <v>NH4</v>
@@ -2161,10 +2188,10 @@
         <v>22</v>
       </c>
       <c r="L14" t="str">
-        <v>Arch_Full_Urb2_v02</v>
+        <v>Arch_Full_Urb3_v01</v>
       </c>
       <c r="M14" t="str">
-        <v>Arch_Full_Urb2_v02</v>
+        <v>Arch_Full_Urb3_v01</v>
       </c>
       <c r="N14" t="str">
         <v>soil_RFs_NO3</v>
@@ -2178,10 +2205,10 @@
     </row>
     <row r="15" spans="2:22">
       <c r="L15" t="str">
-        <v>Arch_Full_Urb3_v02</v>
+        <v>Arch_Full_Urb2_v02</v>
       </c>
       <c r="M15" t="str">
-        <v>Arch_Full_Urb3_v02</v>
+        <v>Arch_Full_Urb2_v02</v>
       </c>
       <c r="N15" t="str">
         <v>soil_RFs_SOx</v>
@@ -2195,10 +2222,10 @@
     </row>
     <row r="16" spans="2:22">
       <c r="L16" t="str">
-        <v>AnthroVOCs_v01_gpkg</v>
+        <v>Arch_Full_Urb3_v02</v>
       </c>
       <c r="M16" t="str">
-        <v>AnthroVOCs_v01_gpkg</v>
+        <v>Arch_Full_Urb3_v02</v>
       </c>
       <c r="N16" t="str">
         <v>AnthroVOCs_v01_gpkg</v>
@@ -2212,10 +2239,10 @@
     </row>
     <row r="17" spans="12:22">
       <c r="L17" t="str">
-        <v>AnthroVOCs_v01_tif</v>
+        <v>AnthroVOCs_v01_gpkg</v>
       </c>
       <c r="M17" t="str">
-        <v>AnthroVOCs_v01_tif</v>
+        <v>AnthroVOCs_v01_gpkg</v>
       </c>
       <c r="N17" t="str">
         <v>AnthroVOCs_v01_tif</v>
@@ -2226,10 +2253,10 @@
     </row>
     <row r="18" spans="12:22">
       <c r="L18" t="str">
-        <v>Continents</v>
+        <v>AnthroVOCs_v01_tif</v>
       </c>
       <c r="M18" t="str">
-        <v>Continents</v>
+        <v>AnthroVOCs_v01_tif</v>
       </c>
       <c r="N18" t="str">
         <v>Pop2010</v>
@@ -2240,10 +2267,10 @@
     </row>
     <row r="19" spans="12:22">
       <c r="L19" t="str">
-        <v>World</v>
+        <v>Continents</v>
       </c>
       <c r="M19" t="str">
-        <v>World</v>
+        <v>Continents</v>
       </c>
       <c r="N19" t="str">
         <v>Edgar Air Ag NH3</v>
@@ -2254,10 +2281,10 @@
     </row>
     <row r="20" spans="12:22">
       <c r="L20" t="str">
-        <v>Ecoregions</v>
+        <v>World</v>
       </c>
       <c r="M20" t="str">
-        <v>Ecoregions</v>
+        <v>World</v>
       </c>
       <c r="N20" t="str">
         <v>Edgar Air Ag NOx</v>
@@ -2265,10 +2292,10 @@
     </row>
     <row r="21" spans="12:22">
       <c r="L21" t="str">
-        <v>GeosGrid</v>
+        <v>Ecoregions</v>
       </c>
       <c r="M21" t="str">
-        <v>GeosGrid</v>
+        <v>Ecoregions</v>
       </c>
       <c r="N21" t="str">
         <v>Edgar Air Ag SO2</v>
@@ -2276,10 +2303,10 @@
     </row>
     <row r="22" spans="12:22">
       <c r="L22" t="str">
-        <v>Pop2010</v>
+        <v>GeosGrid</v>
       </c>
       <c r="M22" t="str">
-        <v>Pop2010</v>
+        <v>GeosGrid</v>
       </c>
       <c r="N22" t="str">
         <v>Edgar Air NonAg NH3</v>
@@ -2287,10 +2314,10 @@
     </row>
     <row r="23" spans="12:22">
       <c r="L23" t="str">
-        <v>EmitEdgarAgNH3</v>
+        <v>Pop2010</v>
       </c>
       <c r="M23" t="str">
-        <v>EmitEdgarAgNH3</v>
+        <v>Pop2010</v>
       </c>
       <c r="N23" t="str">
         <v>Edgar Air NonAg NOx</v>
@@ -2298,10 +2325,10 @@
     </row>
     <row r="24" spans="12:22">
       <c r="L24" t="str">
-        <v>EmitEdgarAgNOx</v>
+        <v>EmitEdgarAgNH3</v>
       </c>
       <c r="M24" t="str">
-        <v>EmitEdgarAgNOx</v>
+        <v>EmitEdgarAgNH3</v>
       </c>
       <c r="N24" t="str">
         <v>Edgar Air NonAg SO2</v>
@@ -2309,10 +2336,10 @@
     </row>
     <row r="25" spans="12:22">
       <c r="L25" t="str">
-        <v>EmitEdgarNonagNH3</v>
+        <v>EmitEdgarAgNOx</v>
       </c>
       <c r="M25" t="str">
-        <v>EmitEdgarNonagNH3</v>
+        <v>EmitEdgarAgNOx</v>
       </c>
       <c r="N25" t="str">
         <v>Edgar Air Gen NH3</v>
@@ -2320,10 +2347,10 @@
     </row>
     <row r="26" spans="12:22">
       <c r="L26" t="str">
-        <v>EmitEdgarNonagNOx</v>
+        <v>EmitEdgarNonagNH3</v>
       </c>
       <c r="M26" t="str">
-        <v>EmitEdgarNonagNOx</v>
+        <v>EmitEdgarNonagNH3</v>
       </c>
       <c r="N26" t="str">
         <v>Edgar Air Gen NOx</v>
@@ -2331,10 +2358,10 @@
     </row>
     <row r="27" spans="12:22">
       <c r="L27" t="str">
-        <v>EmitEdgarAgSO2</v>
+        <v>EmitEdgarNonagNOx</v>
       </c>
       <c r="M27" t="str">
-        <v>EmitEdgarAgSO2</v>
+        <v>EmitEdgarNonagNOx</v>
       </c>
       <c r="N27" t="str">
         <v>Edgar Air Gen SO2</v>
@@ -2342,73 +2369,81 @@
     </row>
     <row r="28" spans="12:22">
       <c r="L28" t="str">
-        <v>EmitEdgarNonagSO2</v>
+        <v>EmitEdgarAgSO2</v>
       </c>
       <c r="M28" t="str">
-        <v>EmitEdgarNonagSO2</v>
+        <v>EmitEdgarAgSO2</v>
       </c>
     </row>
     <row r="29" spans="12:22">
       <c r="L29" t="str">
-        <v>EmitEdgarGenNH3</v>
+        <v>EmitEdgarNonagSO2</v>
       </c>
       <c r="M29" t="str">
-        <v>EmitEdgarGenNH3</v>
+        <v>EmitEdgarNonagSO2</v>
       </c>
     </row>
     <row r="30" spans="12:22">
       <c r="L30" t="str">
-        <v>EmitEdgarGenNOx</v>
+        <v>EmitEdgarGenNH3</v>
       </c>
       <c r="M30" t="str">
-        <v>EmitEdgarGenNOx</v>
+        <v>EmitEdgarGenNH3</v>
       </c>
     </row>
     <row r="31" spans="12:22">
       <c r="L31" t="str">
-        <v>EmitEdgarGenSO2</v>
+        <v>EmitEdgarGenNOx</v>
       </c>
       <c r="M31" t="str">
-        <v>EmitEdgarGenSO2</v>
+        <v>EmitEdgarGenNOx</v>
       </c>
     </row>
     <row r="32" spans="12:22">
       <c r="L32" t="str">
-        <v>file_FF_NOx</v>
+        <v>EmitEdgarGenSO2</v>
+      </c>
+      <c r="M32" t="str">
+        <v>EmitEdgarGenSO2</v>
       </c>
     </row>
     <row r="33" spans="12:12">
       <c r="L33" t="str">
-        <v>file_FF_NHx</v>
+        <v>file_FF_NOx</v>
       </c>
     </row>
     <row r="34" spans="12:12">
       <c r="L34" t="str">
-        <v>file_FF_SOx</v>
+        <v>file_FF_NHx</v>
       </c>
     </row>
     <row r="35" spans="12:12">
       <c r="L35" t="str">
-        <v>ecoreg_RFs_NH4_Lebrun</v>
+        <v>file_FF_SOx</v>
       </c>
     </row>
     <row r="36" spans="12:12">
       <c r="L36" t="str">
-        <v>ecoreg_RFs_NO3_Lebrun</v>
+        <v>ecoreg_RFs_NH4_Lebrun</v>
       </c>
     </row>
     <row r="37" spans="12:12">
       <c r="L37" t="str">
-        <v>ecoreg_RFs_SO4_Lebrun</v>
+        <v>ecoreg_RFs_NO3_Lebrun</v>
       </c>
     </row>
     <row r="38" spans="12:12">
       <c r="L38" t="str">
-        <v>ecoreg_EFs_Gade</v>
+        <v>ecoreg_RFs_SO4_Lebrun</v>
       </c>
     </row>
     <row r="39" spans="12:12">
       <c r="L39" t="str">
+        <v>ecoreg_EFs_Gade</v>
+      </c>
+    </row>
+    <row r="40" spans="12:12">
+      <c r="L40" t="str">
         <v>ecoreg_GEPs</v>
       </c>
     </row>
@@ -2419,10 +2454,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2502FB-B45F-43BB-8645-D93E9F9C6CDF}">
-  <dimension ref="B2:O135"/>
+  <dimension ref="B2:O137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2595,7 +2630,7 @@
     </row>
     <row r="8" spans="2:14">
       <c r="B8" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -2610,16 +2645,16 @@
       </c>
       <c r="G8" t="str" cm="1">
         <f t="array" ref="G8">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>repair1_holes10_simplify0p05_repair2_split</v>
+        <v>repair1_holes10</v>
       </c>
       <c r="H8" t="s">
         <v>252</v>
       </c>
       <c r="I8" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="J8" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="M8" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
@@ -2628,7 +2663,7 @@
     </row>
     <row r="9" spans="2:14">
       <c r="B9" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -2643,16 +2678,16 @@
       </c>
       <c r="G9" t="str" cm="1">
         <f t="array" ref="G9">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>repair1_holes10_simplify0p05_repair2</v>
+        <v>repair1_holes10_simplify0p05_repair2_split</v>
       </c>
       <c r="H9" t="s">
         <v>252</v>
       </c>
       <c r="I9" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="J9" t="s">
-        <v>246</v>
+        <v>270</v>
       </c>
       <c r="M9" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
@@ -2661,14 +2696,14 @@
     </row>
     <row r="10" spans="2:14">
       <c r="B10" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="E10" t="str" cm="1">
         <f t="array" ref="E10">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input</v>
+        <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input</v>
       </c>
       <c r="F10" t="str" cm="1">
         <f t="array" ref="F10">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2676,648 +2711,647 @@
       </c>
       <c r="G10" t="str" cm="1">
         <f t="array" ref="G10">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>archetypes_Full_Urb2_v01</v>
+        <v>repair1_holes10_simplify0p05_repair2</v>
       </c>
       <c r="H10" t="s">
         <v>252</v>
       </c>
-      <c r="I10" t="str">
+      <c r="I10" t="s">
+        <v>263</v>
+      </c>
+      <c r="J10" t="s">
+        <v>246</v>
+      </c>
+      <c r="M10" s="10" t="str">
+        <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
+        <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
+      <c r="B11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" t="str" cm="1">
+        <f t="array" ref="E11">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input</v>
+      </c>
+      <c r="F11" t="str" cm="1">
+        <f t="array" ref="F11">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+        <v/>
+      </c>
+      <c r="G11" t="str" cm="1">
+        <f t="array" ref="G11">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+        <v>archetypes_Full_Urb2_v01</v>
+      </c>
+      <c r="H11" t="s">
+        <v>252</v>
+      </c>
+      <c r="I11" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>Arch_Full_Urb2_v01</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>246</v>
       </c>
-      <c r="M10" s="10" t="str">
+      <c r="M11" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
-      <c r="B11" t="s">
+    <row r="12" spans="2:14">
+      <c r="B12" t="s">
         <v>255</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="E11" t="str" cm="1">
-        <f t="array" ref="E11">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E12" t="str" cm="1">
+        <f t="array" ref="E12">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input</v>
       </c>
-      <c r="F11" t="str" cm="1">
-        <f t="array" ref="F11">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F12" t="str" cm="1">
+        <f t="array" ref="F12">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G11" t="str" cm="1">
-        <f t="array" ref="G11">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G12" t="str" cm="1">
+        <f t="array" ref="G12">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>archetypes_Full_Urb3_v01</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H12" t="s">
         <v>252</v>
       </c>
-      <c r="I11" t="str">
+      <c r="I12" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>Arch_Full_Urb3_v01</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J12" t="s">
         <v>246</v>
       </c>
-      <c r="M11" s="10" t="str">
+      <c r="M12" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
-      <c r="B12" t="s">
+    <row r="13" spans="2:14">
+      <c r="B13" t="s">
         <v>256</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D13" t="s">
         <v>16</v>
       </c>
-      <c r="E12" t="str" cm="1">
-        <f t="array" ref="E12">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E13" t="str" cm="1">
+        <f t="array" ref="E13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input</v>
       </c>
-      <c r="F12" t="str" cm="1">
-        <f t="array" ref="F12">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F13" t="str" cm="1">
+        <f t="array" ref="F13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G12" t="str" cm="1">
-        <f t="array" ref="G12">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G13" t="str" cm="1">
+        <f t="array" ref="G13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>archetypes_Full_Urb2_v02</v>
       </c>
-      <c r="H12" t="str" cm="1">
-        <f t="array" ref="H12">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H13" t="str" cm="1">
+        <f t="array" ref="H13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.gpkg</v>
       </c>
-      <c r="I12" t="str">
+      <c r="I13" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>Arch_Full_Urb2_v02</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J13" t="s">
         <v>246</v>
       </c>
-      <c r="M12" s="10" t="str">
+      <c r="M13" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
-      <c r="B13" t="s">
+    <row r="14" spans="2:14">
+      <c r="B14" t="s">
         <v>257</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D14" t="s">
         <v>16</v>
       </c>
-      <c r="E13" t="str" cm="1">
-        <f t="array" ref="E13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E14" t="str" cm="1">
+        <f t="array" ref="E14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input</v>
       </c>
-      <c r="F13" t="str" cm="1">
-        <f t="array" ref="F13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F14" t="str" cm="1">
+        <f t="array" ref="F14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G13" t="str" cm="1">
-        <f t="array" ref="G13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G14" t="str" cm="1">
+        <f t="array" ref="G14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>archetypes_Full_Urb3_v02</v>
       </c>
-      <c r="H13" t="str" cm="1">
-        <f t="array" ref="H13">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H14" t="str" cm="1">
+        <f t="array" ref="H14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.gpkg</v>
       </c>
-      <c r="I13" t="str">
+      <c r="I14" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>Arch_Full_Urb3_v02</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J14" t="s">
         <v>246</v>
       </c>
-      <c r="M13" s="10" t="str">
+      <c r="M14" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
-      <c r="B14" t="s">
+    <row r="15" spans="2:14">
+      <c r="B15" t="s">
         <v>250</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D15" t="s">
         <v>16</v>
       </c>
-      <c r="E14" t="str" cm="1">
-        <f t="array" ref="E14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E15" t="str" cm="1">
+        <f t="array" ref="E15">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates</v>
       </c>
-      <c r="F14" t="str" cm="1">
-        <f t="array" ref="F14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F15" t="str" cm="1">
+        <f t="array" ref="F15">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G14" t="str" cm="1">
-        <f t="array" ref="G14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G15" t="str" cm="1">
+        <f t="array" ref="G15">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>anthro_compiled_v01</v>
       </c>
-      <c r="H14" t="str" cm="1">
-        <f t="array" ref="H14">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H15" t="str" cm="1">
+        <f t="array" ref="H15">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.gpkg</v>
       </c>
-      <c r="I14" t="str">
+      <c r="I15" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>AnthroVOCs_v01_gpkg</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J15" t="s">
         <v>246</v>
       </c>
-      <c r="M14" s="10" t="str">
+      <c r="M15" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
-      <c r="B15" t="s">
+    <row r="16" spans="2:14">
+      <c r="B16" t="s">
         <v>251</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>16</v>
       </c>
-      <c r="E15" t="str" cm="1">
-        <f t="array" ref="E15">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E16" t="str" cm="1">
+        <f t="array" ref="E16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates</v>
       </c>
-      <c r="F15" t="str" cm="1">
-        <f t="array" ref="F15">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F16" t="str" cm="1">
+        <f t="array" ref="F16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G15" t="str" cm="1">
-        <f t="array" ref="G15">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G16" t="str" cm="1">
+        <f t="array" ref="G16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>anthro_compiled_v01</v>
       </c>
-      <c r="H15" t="str" cm="1">
-        <f t="array" ref="H15">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H16" t="str" cm="1">
+        <f t="array" ref="H16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.tif</v>
       </c>
-      <c r="I15" t="str">
+      <c r="I16" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>AnthroVOCs_v01_tif</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J16" t="s">
         <v>246</v>
       </c>
-      <c r="M15" s="10" t="str">
+      <c r="M16" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
-      <c r="B16" t="s">
+    <row r="17" spans="2:13">
+      <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>16</v>
       </c>
-      <c r="E16" t="str" cm="1">
-        <f t="array" ref="E16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E17" t="str" cm="1">
+        <f t="array" ref="E17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F16" t="str" cm="1">
-        <f t="array" ref="F16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F17" t="str" cm="1">
+        <f t="array" ref="F17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G16" t="str" cm="1">
-        <f t="array" ref="G16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G17" t="str" cm="1">
+        <f t="array" ref="G17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>World_Countries_2018_Continents</v>
       </c>
-      <c r="H16" t="str" cm="1">
-        <f t="array" ref="H16">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H17" t="str" cm="1">
+        <f t="array" ref="H17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I16" t="str">
+      <c r="I17" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>Continents</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J17" t="s">
         <v>66</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K17" t="s">
         <v>68</v>
       </c>
-      <c r="M16" s="9" t="str">
+      <c r="M17" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
-      <c r="B17" t="s">
+    <row r="18" spans="2:13">
+      <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>16</v>
       </c>
-      <c r="E17" t="str" cm="1">
-        <f t="array" ref="E17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E18" t="str" cm="1">
+        <f t="array" ref="E18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F17" t="str" cm="1">
-        <f t="array" ref="F17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F18" t="str" cm="1">
+        <f t="array" ref="F18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G17" t="str" cm="1">
-        <f t="array" ref="G17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G18" t="str" cm="1">
+        <f t="array" ref="G18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>World_Countries_2018_SingleShape</v>
       </c>
-      <c r="H17" t="str" cm="1">
-        <f t="array" ref="H17">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H18" t="str" cm="1">
+        <f t="array" ref="H18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I17" t="str">
+      <c r="I18" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>World</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J18" t="s">
         <v>66</v>
       </c>
-      <c r="K17" t="s">
+      <c r="K18" t="s">
         <v>217</v>
       </c>
-      <c r="L17" t="s">
+      <c r="L18" t="s">
         <v>218</v>
       </c>
-      <c r="M17" s="9" t="str">
+      <c r="M18" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
-      <c r="B18" t="s">
+    <row r="19" spans="2:13">
+      <c r="B19" t="s">
         <v>39</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D19" t="s">
         <v>16</v>
       </c>
-      <c r="E18" t="str" cm="1">
-        <f t="array" ref="E18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E19" t="str" cm="1">
+        <f t="array" ref="E19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F18" t="str" cm="1">
-        <f t="array" ref="F18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F19" t="str" cm="1">
+        <f t="array" ref="F19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G18" t="str" cm="1">
-        <f t="array" ref="G18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G19" t="str" cm="1">
+        <f t="array" ref="G19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>wwf_terr_ecos_projWCEA</v>
       </c>
-      <c r="H18" t="str" cm="1">
-        <f t="array" ref="H18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H19" t="str" cm="1">
+        <f t="array" ref="H19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I18" t="str">
+      <c r="I19" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>Ecoregions</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J19" t="s">
         <v>118</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K19" t="s">
         <v>70</v>
       </c>
-      <c r="M18" s="9" t="str">
+      <c r="M19" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="19" spans="2:13">
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="20" spans="2:13">
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" t="s">
         <v>16</v>
       </c>
-      <c r="E19" t="str" cm="1">
-        <f t="array" ref="E19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E20" t="str" cm="1">
+        <f t="array" ref="E20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F19" t="str" cm="1">
-        <f t="array" ref="F19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F20" t="str" cm="1">
+        <f t="array" ref="F20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G19" t="str" cm="1">
-        <f t="array" ref="G19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G20" t="str" cm="1">
+        <f t="array" ref="G20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>GEOS_Roy_Grid_pWCEA</v>
       </c>
-      <c r="H19" t="str" cm="1">
-        <f t="array" ref="H19">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H20" t="str" cm="1">
+        <f t="array" ref="H20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I19" t="str">
+      <c r="I20" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>GeosGrid</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J20" t="s">
         <v>69</v>
       </c>
-      <c r="M19" s="9" t="str">
+      <c r="M20" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="20" spans="2:13">
-      <c r="B20" t="s">
+    <row r="21" spans="2:13">
+      <c r="B21" t="s">
         <v>32</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D21" t="s">
         <v>16</v>
       </c>
-      <c r="E20" t="str" cm="1">
-        <f t="array" ref="E20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E21" t="str" cm="1">
+        <f t="array" ref="E21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F20" t="str" cm="1">
-        <f t="array" ref="F20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F21" t="str" cm="1">
+        <f t="array" ref="F21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G20" t="str" cm="1">
-        <f t="array" ref="G20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G21" t="str" cm="1">
+        <f t="array" ref="G21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>gpwv42010_poly_pWCEA</v>
       </c>
-      <c r="H20" t="str" cm="1">
-        <f t="array" ref="H20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H21" t="str" cm="1">
+        <f t="array" ref="H21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I20" t="str">
+      <c r="I21" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>Pop2010</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J21" t="s">
         <v>119</v>
       </c>
-      <c r="M20" s="9" t="str">
+      <c r="M21" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="21" spans="2:13">
-      <c r="B21" t="s">
+    <row r="22" spans="2:13">
+      <c r="B22" t="s">
         <v>33</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>16</v>
       </c>
-      <c r="E21" t="str" cm="1">
-        <f t="array" ref="E21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E22" t="str" cm="1">
+        <f t="array" ref="E22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F21" t="str" cm="1">
-        <f t="array" ref="F21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F22" t="str" cm="1">
+        <f t="array" ref="F22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G21" t="str" cm="1">
-        <f t="array" ref="G21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G22" t="str" cm="1">
+        <f t="array" ref="G22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>air_Edgar_agric_NH3</v>
       </c>
-      <c r="H21" t="str" cm="1">
-        <f t="array" ref="H21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H22" t="str" cm="1">
+        <f t="array" ref="H22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I21" t="str">
+      <c r="I22" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>EmitEdgarAgNH3</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J22" t="s">
         <v>119</v>
       </c>
-      <c r="M21" s="9" t="str">
+      <c r="M22" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="22" spans="2:13">
-      <c r="B22" t="s">
+    <row r="23" spans="2:13">
+      <c r="B23" t="s">
         <v>34</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>16</v>
       </c>
-      <c r="E22" t="str" cm="1">
-        <f t="array" ref="E22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E23" t="str" cm="1">
+        <f t="array" ref="E23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F22" t="str" cm="1">
-        <f t="array" ref="F22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F23" t="str" cm="1">
+        <f t="array" ref="F23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G22" t="str" cm="1">
-        <f t="array" ref="G22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G23" t="str" cm="1">
+        <f t="array" ref="G23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>air_Edgar_agric_NOx</v>
       </c>
-      <c r="H22" t="str" cm="1">
-        <f t="array" ref="H22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H23" t="str" cm="1">
+        <f t="array" ref="H23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I22" t="str">
+      <c r="I23" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>EmitEdgarAgNOx</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J23" t="s">
         <v>119</v>
       </c>
-      <c r="M22" s="9" t="str">
+      <c r="M23" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="23" spans="2:13">
-      <c r="B23" t="s">
+    <row r="24" spans="2:13">
+      <c r="B24" t="s">
         <v>35</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>16</v>
       </c>
-      <c r="E23" t="str" cm="1">
-        <f t="array" ref="E23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E24" t="str" cm="1">
+        <f t="array" ref="E24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F23" t="str" cm="1">
-        <f t="array" ref="F23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F24" t="str" cm="1">
+        <f t="array" ref="F24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G23" t="str" cm="1">
-        <f t="array" ref="G23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G24" t="str" cm="1">
+        <f t="array" ref="G24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>air_Edgar_nonagric_NH3</v>
       </c>
-      <c r="H23" t="str" cm="1">
-        <f t="array" ref="H23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H24" t="str" cm="1">
+        <f t="array" ref="H24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I23" t="str">
+      <c r="I24" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>EmitEdgarAgSO2</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J24" t="s">
         <v>119</v>
       </c>
-      <c r="M23" s="9" t="str">
+      <c r="M24" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="24" spans="2:13">
-      <c r="B24" t="s">
+    <row r="25" spans="2:13">
+      <c r="B25" t="s">
         <v>36</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>16</v>
       </c>
-      <c r="E24" t="str" cm="1">
-        <f t="array" ref="E24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E25" t="str" cm="1">
+        <f t="array" ref="E25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F24" t="str" cm="1">
-        <f t="array" ref="F24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F25" t="str" cm="1">
+        <f t="array" ref="F25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G24" t="str" cm="1">
-        <f t="array" ref="G24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G25" t="str" cm="1">
+        <f t="array" ref="G25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>air_Edgar_nonagric_NOx</v>
       </c>
-      <c r="H24" t="str" cm="1">
-        <f t="array" ref="H24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H25" t="str" cm="1">
+        <f t="array" ref="H25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I24" t="str">
+      <c r="I25" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>EmitEdgarNonagNH3</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J25" t="s">
         <v>119</v>
       </c>
-      <c r="M24" s="9" t="str">
+      <c r="M25" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="25" spans="2:13">
-      <c r="B25" t="s">
+    <row r="26" spans="2:13">
+      <c r="B26" t="s">
         <v>37</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D26" t="s">
         <v>16</v>
       </c>
-      <c r="E25" t="str" cm="1">
-        <f t="array" ref="E25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E26" t="str" cm="1">
+        <f t="array" ref="E26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F25" t="str" cm="1">
-        <f t="array" ref="F25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F26" t="str" cm="1">
+        <f t="array" ref="F26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G25" t="str" cm="1">
-        <f t="array" ref="G25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G26" t="str" cm="1">
+        <f t="array" ref="G26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>air_Edgar_agric_SO2</v>
       </c>
-      <c r="H25" t="str" cm="1">
-        <f t="array" ref="H25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H26" t="str" cm="1">
+        <f t="array" ref="H26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I25" t="str">
+      <c r="I26" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>EmitEdgarNonagNOx</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J26" t="s">
         <v>119</v>
       </c>
-      <c r="M25" s="9" t="str">
+      <c r="M26" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="26" spans="2:13">
-      <c r="B26" t="s">
+    <row r="27" spans="2:13">
+      <c r="B27" t="s">
         <v>38</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>16</v>
       </c>
-      <c r="E26" t="str" cm="1">
-        <f t="array" ref="E26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="E27" t="str" cm="1">
+        <f t="array" ref="E27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
-      <c r="F26" t="str" cm="1">
-        <f t="array" ref="F26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="F27" t="str" cm="1">
+        <f t="array" ref="F27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v/>
       </c>
-      <c r="G26" t="str" cm="1">
-        <f t="array" ref="G26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="G27" t="str" cm="1">
+        <f t="array" ref="G27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>air_Edgar_nonagric_SO2</v>
       </c>
-      <c r="H26" t="str" cm="1">
-        <f t="array" ref="H26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+      <c r="H27" t="str" cm="1">
+        <f t="array" ref="H27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
-      <c r="I26" t="str">
+      <c r="I27" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
         <v>EmitEdgarNonagSO2</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J27" t="s">
         <v>119</v>
       </c>
-      <c r="M26" s="9" t="str">
+      <c r="M27" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
-    <row r="27" spans="2:13">
-      <c r="B27" t="s">
-        <v>226</v>
-      </c>
-      <c r="D27" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" t="str" cm="1">
-        <f t="array" ref="E27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
-      </c>
-      <c r="F27" t="str" cm="1">
-        <f t="array" ref="F27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
-      </c>
-      <c r="G27" t="str" cm="1">
-        <f t="array" ref="G27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>poly_NH3_WCEA</v>
-      </c>
-      <c r="H27" t="str" cm="1">
-        <f t="array" ref="H27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>.shp</v>
-      </c>
-      <c r="I27" t="s">
-        <v>226</v>
-      </c>
-      <c r="J27" t="s">
-        <v>119</v>
-      </c>
-      <c r="M27" s="10" t="str">
-        <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
     <row r="28" spans="2:13">
       <c r="B28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D28" t="s">
         <v>16</v>
@@ -3332,14 +3366,14 @@
       </c>
       <c r="G28" t="str" cm="1">
         <f t="array" ref="G28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>poly_NOx_WCEA</v>
+        <v>poly_NH3_WCEA</v>
       </c>
       <c r="H28" t="str" cm="1">
         <f t="array" ref="H28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
       <c r="I28" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J28" t="s">
         <v>119</v>
@@ -3351,7 +3385,7 @@
     </row>
     <row r="29" spans="2:13">
       <c r="B29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D29" t="s">
         <v>16</v>
@@ -3366,14 +3400,14 @@
       </c>
       <c r="G29" t="str" cm="1">
         <f t="array" ref="G29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>poly_SO2_WCEA</v>
+        <v>poly_NOx_WCEA</v>
       </c>
       <c r="H29" t="str" cm="1">
         <f t="array" ref="H29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
         <v>.shp</v>
       </c>
       <c r="I29" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J29" t="s">
         <v>119</v>
@@ -3385,10 +3419,10 @@
     </row>
     <row r="30" spans="2:13">
       <c r="B30" t="s">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E30" t="str" cm="1">
         <f t="array" ref="E30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3400,25 +3434,26 @@
       </c>
       <c r="G30" t="str" cm="1">
         <f t="array" ref="G30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>FFairNOx</v>
+        <v>poly_SO2_WCEA</v>
       </c>
       <c r="H30" t="str" cm="1">
         <f t="array" ref="H30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>.mat</v>
-      </c>
-      <c r="I30" t="str">
-        <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
-IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
-        <v>GeosGrid</v>
-      </c>
-      <c r="M30" s="9" t="str">
+        <v>.shp</v>
+      </c>
+      <c r="I30" t="s">
+        <v>228</v>
+      </c>
+      <c r="J30" t="s">
+        <v>119</v>
+      </c>
+      <c r="M30" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="31" spans="2:13">
       <c r="B31" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D31" t="s">
         <v>17</v>
@@ -3433,7 +3468,7 @@
       </c>
       <c r="G31" t="str" cm="1">
         <f t="array" ref="G31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>FFairNHx</v>
+        <v>FFairNOx</v>
       </c>
       <c r="H31" t="str" cm="1">
         <f t="array" ref="H31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3451,7 +3486,7 @@
     </row>
     <row r="32" spans="2:13">
       <c r="B32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
@@ -3466,7 +3501,7 @@
       </c>
       <c r="G32" t="str" cm="1">
         <f t="array" ref="G32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>FFairSOx</v>
+        <v>FFairNHx</v>
       </c>
       <c r="H32" t="str" cm="1">
         <f t="array" ref="H32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3484,14 +3519,14 @@
     </row>
     <row r="33" spans="2:15">
       <c r="B33" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="D33" t="s">
-        <v>100</v>
+        <v>17</v>
       </c>
       <c r="E33" t="str" cm="1">
         <f t="array" ref="E33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F33" t="str" cm="1">
         <f t="array" ref="F33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3499,25 +3534,25 @@
       </c>
       <c r="G33" t="str" cm="1">
         <f t="array" ref="G33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>RF_no3_1_nh4_1.1_so4_1</v>
+        <v>FFairSOx</v>
       </c>
       <c r="H33" t="str" cm="1">
         <f t="array" ref="H33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>.xlsx</v>
+        <v>.mat</v>
       </c>
       <c r="I33" t="str">
         <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
 IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
-        <v>Ecoregions</v>
+        <v>GeosGrid</v>
       </c>
       <c r="M33" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="34" spans="2:15">
       <c r="B34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D34" t="s">
         <v>100</v>
@@ -3532,7 +3567,7 @@
       </c>
       <c r="G34" t="str" cm="1">
         <f t="array" ref="G34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>RF_no3_1.1_nh4_1_so4_1</v>
+        <v>RF_no3_1_nh4_1.1_so4_1</v>
       </c>
       <c r="H34" t="str" cm="1">
         <f t="array" ref="H34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3550,7 +3585,7 @@
     </row>
     <row r="35" spans="2:15">
       <c r="B35" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D35" t="s">
         <v>100</v>
@@ -3565,7 +3600,7 @@
       </c>
       <c r="G35" t="str" cm="1">
         <f t="array" ref="G35">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>RF_no3_1_nh4_1_so4_1.1</v>
+        <v>RF_no3_1.1_nh4_1_so4_1</v>
       </c>
       <c r="H35" t="str" cm="1">
         <f t="array" ref="H35">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3583,7 +3618,7 @@
     </row>
     <row r="36" spans="2:15">
       <c r="B36" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
       <c r="D36" t="s">
         <v>100</v>
@@ -3598,7 +3633,7 @@
       </c>
       <c r="G36" t="str" cm="1">
         <f t="array" ref="G36">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>EF_v02</v>
+        <v>RF_no3_1_nh4_1_so4_1.1</v>
       </c>
       <c r="H36" t="str" cm="1">
         <f t="array" ref="H36">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3616,7 +3651,7 @@
     </row>
     <row r="37" spans="2:15">
       <c r="B37" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="D37" t="s">
         <v>100</v>
@@ -3631,7 +3666,7 @@
       </c>
       <c r="G37" t="str" cm="1">
         <f t="array" ref="G37">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>VascularPlants_GEP_TEOW</v>
+        <v>EF_v02</v>
       </c>
       <c r="H37" t="str" cm="1">
         <f t="array" ref="H37">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3647,85 +3682,94 @@
         <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="43" spans="2:15">
-      <c r="B43" t="s">
+    <row r="38" spans="2:15">
+      <c r="B38" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" t="s">
+        <v>100</v>
+      </c>
+      <c r="E38" t="str" cm="1">
+        <f t="array" ref="E38">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+      </c>
+      <c r="F38" t="str" cm="1">
+        <f t="array" ref="F38">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+        <v/>
+      </c>
+      <c r="G38" t="str" cm="1">
+        <f t="array" ref="G38">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+        <v>VascularPlants_GEP_TEOW</v>
+      </c>
+      <c r="H38" t="str" cm="1">
+        <f t="array" ref="H38">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File extension]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
+        <v>.xlsx</v>
+      </c>
+      <c r="I38" t="str">
+        <f>_xlfn.LET(_xlpm.thisUniqueName, Tbl.Files[[#This Row],[File unique name]], _xlpm.thisNameUsedInData, IFERROR(_xlfn.XMATCH(_xlpm.thisUniqueName,Tbl.Data[Source file unique name],0)&gt;0, FALSE),
+IF(_xlpm.thisNameUsedInData,  _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]],Tbl.Data[Source file unique name],Tbl.Data[Associated geofile]), _xlpm.thisUniqueName))</f>
+        <v>Ecoregions</v>
+      </c>
+      <c r="M38" s="9" t="str">
+        <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15">
+      <c r="B44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="2:15">
-      <c r="B44" s="3" t="s">
+    <row r="45" spans="2:15">
+      <c r="B45" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="3" t="s">
+      <c r="C45" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D45" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="G44" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="H45" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="I44" s="3" t="s">
+      <c r="I45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J44" s="3" t="s">
+      <c r="J45" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K44" s="3" t="s">
+      <c r="K45" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L44" s="3" t="s">
+      <c r="L45" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="M44" s="3" t="s">
+      <c r="M45" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N44" s="3" t="s">
+      <c r="N45" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O44" s="3" t="s">
+      <c r="O45" s="3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="45" spans="2:15">
-      <c r="B45" t="s">
-        <v>46</v>
-      </c>
-      <c r="D45" t="s">
-        <v>191</v>
-      </c>
-      <c r="I45" t="s">
-        <v>31</v>
-      </c>
-      <c r="J45" t="s">
-        <v>19</v>
-      </c>
-      <c r="L45" t="b" cm="1">
-        <f t="array" ref="L45">_xlfn.XLOOKUP(Tbl.Data[[#This Row],[Source file unique name]],Tbl.Files[File unique name],Tbl.Files[File structure]=str.file_struct.matrix)</f>
-        <v>1</v>
-      </c>
-      <c r="M45" t="b">
-        <v>0</v>
-      </c>
-      <c r="N45" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="46" spans="2:15">
       <c r="B46" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I46" t="s">
         <v>31</v>
@@ -3741,15 +3785,15 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="47" spans="2:15">
       <c r="B47" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D47" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I47" t="s">
         <v>31</v>
@@ -3765,57 +3809,54 @@
         <v>0</v>
       </c>
       <c r="N47" t="s">
-        <v>157</v>
+        <v>96</v>
       </c>
     </row>
     <row r="48" spans="2:15">
       <c r="B48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D48" t="s">
-        <v>57</v>
-      </c>
-      <c r="E48" t="s">
-        <v>196</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>240</v>
-      </c>
-      <c r="G48" s="11" t="s">
-        <v>241</v>
+        <v>193</v>
       </c>
       <c r="I48" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="J48" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="L48" t="b" cm="1">
         <f t="array" ref="L48">_xlfn.XLOOKUP(Tbl.Data[[#This Row],[Source file unique name]],Tbl.Files[File unique name],Tbl.Files[File structure]=str.file_struct.matrix)</f>
+        <v>1</v>
+      </c>
+      <c r="M48" t="b">
         <v>0</v>
+      </c>
+      <c r="N48" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="49" spans="2:12">
       <c r="B49" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D49" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="E49" t="s">
-        <v>150</v>
+        <v>196</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>118</v>
+        <v>240</v>
       </c>
       <c r="G49" s="11" t="s">
-        <v>155</v>
+        <v>241</v>
       </c>
       <c r="I49" t="s">
         <v>39</v>
       </c>
       <c r="J49" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="L49" t="b" cm="1">
         <f t="array" ref="L49">_xlfn.XLOOKUP(Tbl.Data[[#This Row],[Source file unique name]],Tbl.Files[File unique name],Tbl.Files[File structure]=str.file_struct.matrix)</f>
@@ -3824,25 +3865,25 @@
     </row>
     <row r="50" spans="2:12">
       <c r="B50" t="s">
-        <v>151</v>
+        <v>50</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>50</v>
       </c>
       <c r="E50" t="s">
-        <v>195</v>
-      </c>
-      <c r="F50" t="s">
-        <v>156</v>
-      </c>
-      <c r="G50" t="s">
-        <v>154</v>
+        <v>150</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G50" s="11" t="s">
+        <v>155</v>
       </c>
       <c r="I50" t="s">
         <v>39</v>
       </c>
       <c r="J50" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L50" t="b" cm="1">
         <f t="array" ref="L50">_xlfn.XLOOKUP(Tbl.Data[[#This Row],[Source file unique name]],Tbl.Files[File unique name],Tbl.Files[File structure]=str.file_struct.matrix)</f>
@@ -3851,10 +3892,10 @@
     </row>
     <row r="51" spans="2:12">
       <c r="B51" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D51" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E51" t="s">
         <v>195</v>
@@ -3878,10 +3919,10 @@
     </row>
     <row r="52" spans="2:12">
       <c r="B52" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D52" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E52" t="s">
         <v>195</v>
@@ -3905,25 +3946,25 @@
     </row>
     <row r="53" spans="2:12">
       <c r="B53" t="s">
-        <v>250</v>
+        <v>153</v>
       </c>
       <c r="D53" t="s">
-        <v>250</v>
+        <v>142</v>
+      </c>
+      <c r="E53" t="s">
+        <v>195</v>
       </c>
       <c r="F53" t="s">
-        <v>246</v>
+        <v>156</v>
       </c>
       <c r="G53" t="s">
-        <v>247</v>
+        <v>154</v>
       </c>
       <c r="I53" t="s">
-        <v>250</v>
+        <v>39</v>
       </c>
       <c r="J53" t="s">
-        <v>22</v>
-      </c>
-      <c r="K53" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="L53" t="b" cm="1">
         <f t="array" ref="L53">_xlfn.XLOOKUP(Tbl.Data[[#This Row],[Source file unique name]],Tbl.Files[File unique name],Tbl.Files[File structure]=str.file_struct.matrix)</f>
@@ -3932,10 +3973,10 @@
     </row>
     <row r="54" spans="2:12">
       <c r="B54" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D54" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="F54" t="s">
         <v>246</v>
@@ -3944,7 +3985,7 @@
         <v>247</v>
       </c>
       <c r="I54" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="J54" t="s">
         <v>22</v>
@@ -3959,19 +4000,19 @@
     </row>
     <row r="55" spans="2:12">
       <c r="B55" t="s">
-        <v>32</v>
+        <v>251</v>
       </c>
       <c r="D55" t="s">
-        <v>32</v>
+        <v>251</v>
       </c>
       <c r="F55" t="s">
-        <v>119</v>
+        <v>246</v>
       </c>
       <c r="G55" t="s">
-        <v>121</v>
+        <v>247</v>
       </c>
       <c r="I55" t="s">
-        <v>32</v>
+        <v>251</v>
       </c>
       <c r="J55" t="s">
         <v>22</v>
@@ -3986,19 +4027,19 @@
     </row>
     <row r="56" spans="2:12">
       <c r="B56" t="s">
-        <v>51</v>
+        <v>32</v>
       </c>
       <c r="D56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F56" t="s">
         <v>119</v>
       </c>
       <c r="G56" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I56" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J56" t="s">
         <v>22</v>
@@ -4013,10 +4054,10 @@
     </row>
     <row r="57" spans="2:12">
       <c r="B57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F57" t="s">
         <v>119</v>
@@ -4025,7 +4066,7 @@
         <v>120</v>
       </c>
       <c r="I57" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J57" t="s">
         <v>22</v>
@@ -4040,10 +4081,10 @@
     </row>
     <row r="58" spans="2:12">
       <c r="B58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D58" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F58" t="s">
         <v>119</v>
@@ -4052,7 +4093,7 @@
         <v>120</v>
       </c>
       <c r="I58" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J58" t="s">
         <v>22</v>
@@ -4067,10 +4108,10 @@
     </row>
     <row r="59" spans="2:12">
       <c r="B59" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D59" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F59" t="s">
         <v>119</v>
@@ -4079,7 +4120,7 @@
         <v>120</v>
       </c>
       <c r="I59" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J59" t="s">
         <v>22</v>
@@ -4094,10 +4135,10 @@
     </row>
     <row r="60" spans="2:12">
       <c r="B60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F60" t="s">
         <v>119</v>
@@ -4106,7 +4147,7 @@
         <v>120</v>
       </c>
       <c r="I60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J60" t="s">
         <v>22</v>
@@ -4121,10 +4162,10 @@
     </row>
     <row r="61" spans="2:12">
       <c r="B61" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D61" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F61" t="s">
         <v>119</v>
@@ -4133,7 +4174,7 @@
         <v>120</v>
       </c>
       <c r="I61" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J61" t="s">
         <v>22</v>
@@ -4148,19 +4189,19 @@
     </row>
     <row r="62" spans="2:12">
       <c r="B62" t="s">
-        <v>223</v>
+        <v>56</v>
       </c>
       <c r="D62" t="s">
-        <v>226</v>
+        <v>38</v>
       </c>
       <c r="F62" t="s">
         <v>119</v>
       </c>
       <c r="G62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I62" t="s">
-        <v>226</v>
+        <v>38</v>
       </c>
       <c r="J62" t="s">
         <v>22</v>
@@ -4175,10 +4216,10 @@
     </row>
     <row r="63" spans="2:12">
       <c r="B63" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F63" t="s">
         <v>119</v>
@@ -4187,7 +4228,7 @@
         <v>121</v>
       </c>
       <c r="I63" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J63" t="s">
         <v>22</v>
@@ -4202,10 +4243,10 @@
     </row>
     <row r="64" spans="2:12">
       <c r="B64" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F64" t="s">
         <v>119</v>
@@ -4214,7 +4255,7 @@
         <v>121</v>
       </c>
       <c r="I64" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J64" t="s">
         <v>22</v>
@@ -4227,71 +4268,81 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:7">
-      <c r="B70" t="s">
+    <row r="65" spans="2:12">
+      <c r="B65" t="s">
+        <v>224</v>
+      </c>
+      <c r="D65" t="s">
+        <v>228</v>
+      </c>
+      <c r="F65" t="s">
+        <v>119</v>
+      </c>
+      <c r="G65" t="s">
+        <v>121</v>
+      </c>
+      <c r="I65" t="s">
+        <v>228</v>
+      </c>
+      <c r="J65" t="s">
+        <v>22</v>
+      </c>
+      <c r="K65" t="s">
+        <v>26</v>
+      </c>
+      <c r="L65" t="b" cm="1">
+        <f t="array" ref="L65">_xlfn.XLOOKUP(Tbl.Data[[#This Row],[Source file unique name]],Tbl.Files[File unique name],Tbl.Files[File structure]=str.file_struct.matrix)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:12">
+      <c r="B71" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="71" spans="2:7">
-      <c r="B71" t="s">
+    <row r="72" spans="2:12">
+      <c r="B72" t="s">
         <v>71</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C72" t="s">
         <v>72</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D72" t="s">
         <v>8</v>
       </c>
-      <c r="E71" t="s">
+      <c r="E72" t="s">
         <v>9</v>
       </c>
-      <c r="F71" t="s">
+      <c r="F72" t="s">
         <v>5</v>
       </c>
-      <c r="G71" t="s">
+      <c r="G72" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="2:7">
-      <c r="B72" t="s">
+    <row r="73" spans="2:12">
+      <c r="B73" t="s">
         <v>28</v>
-      </c>
-      <c r="C72" t="s">
-        <v>94</v>
-      </c>
-      <c r="D72" t="s">
-        <v>77</v>
-      </c>
-      <c r="E72" t="s">
-        <v>78</v>
-      </c>
-      <c r="F72" t="s">
-        <v>79</v>
-      </c>
-      <c r="G72" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="73" spans="2:7">
-      <c r="B73" t="s">
-        <v>266</v>
       </c>
       <c r="C73" t="s">
         <v>94</v>
       </c>
       <c r="D73" t="s">
-        <v>264</v>
+        <v>77</v>
+      </c>
+      <c r="E73" t="s">
+        <v>78</v>
       </c>
       <c r="F73" t="s">
-        <v>267</v>
+        <v>79</v>
       </c>
       <c r="G73" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="74" spans="2:7">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="2:12">
       <c r="B74" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C74" t="s">
         <v>94</v>
@@ -4300,15 +4351,15 @@
         <v>264</v>
       </c>
       <c r="F74" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G74" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="75" spans="2:7">
+    <row r="75" spans="2:12">
       <c r="B75" t="s">
-        <v>263</v>
+        <v>268</v>
       </c>
       <c r="C75" t="s">
         <v>94</v>
@@ -4317,32 +4368,32 @@
         <v>264</v>
       </c>
       <c r="F75" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="G75" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="76" spans="2:7">
+    <row r="76" spans="2:12">
       <c r="B76" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="C76" t="s">
         <v>94</v>
       </c>
       <c r="D76" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="F76" t="s">
-        <v>259</v>
+        <v>265</v>
       </c>
       <c r="G76" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="77" spans="2:7">
+    <row r="77" spans="2:12">
       <c r="B77" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C77" t="s">
         <v>94</v>
@@ -4351,15 +4402,15 @@
         <v>258</v>
       </c>
       <c r="F77" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G77" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="2:7">
+    <row r="78" spans="2:12">
       <c r="B78" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C78" t="s">
         <v>94</v>
@@ -4368,15 +4419,15 @@
         <v>258</v>
       </c>
       <c r="F78" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G78" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="79" spans="2:7">
+    <row r="79" spans="2:12">
       <c r="B79" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C79" t="s">
         <v>94</v>
@@ -4385,27 +4436,24 @@
         <v>258</v>
       </c>
       <c r="F79" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G79" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="80" spans="2:7">
+    <row r="80" spans="2:12">
       <c r="B80" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="C80" t="s">
         <v>94</v>
       </c>
       <c r="D80" t="s">
-        <v>248</v>
-      </c>
-      <c r="E80" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="F80" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="G80" t="s">
         <v>252</v>
@@ -4413,7 +4461,7 @@
     </row>
     <row r="81" spans="2:7">
       <c r="B81" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C81" t="s">
         <v>94</v>
@@ -4421,36 +4469,36 @@
       <c r="D81" t="s">
         <v>248</v>
       </c>
+      <c r="E81" t="s">
+        <v>249</v>
+      </c>
       <c r="F81" t="s">
         <v>249</v>
       </c>
       <c r="G81" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="82" spans="2:7">
       <c r="B82" t="s">
-        <v>29</v>
+        <v>251</v>
       </c>
       <c r="C82" t="s">
         <v>94</v>
       </c>
       <c r="D82" t="s">
-        <v>77</v>
-      </c>
-      <c r="E82" t="s">
-        <v>78</v>
+        <v>248</v>
       </c>
       <c r="F82" t="s">
-        <v>80</v>
+        <v>249</v>
       </c>
       <c r="G82" t="s">
-        <v>76</v>
+        <v>253</v>
       </c>
     </row>
     <row r="83" spans="2:7">
       <c r="B83" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C83" t="s">
         <v>94</v>
@@ -4462,7 +4510,7 @@
         <v>78</v>
       </c>
       <c r="F83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G83" t="s">
         <v>76</v>
@@ -4470,16 +4518,19 @@
     </row>
     <row r="84" spans="2:7">
       <c r="B84" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C84" t="s">
         <v>94</v>
       </c>
       <c r="D84" t="s">
-        <v>74</v>
+        <v>77</v>
+      </c>
+      <c r="E84" t="s">
+        <v>78</v>
       </c>
       <c r="F84" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="G84" t="s">
         <v>76</v>
@@ -4487,19 +4538,16 @@
     </row>
     <row r="85" spans="2:7">
       <c r="B85" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="C85" t="s">
         <v>94</v>
       </c>
       <c r="D85" t="s">
-        <v>77</v>
-      </c>
-      <c r="E85" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F85" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G85" t="s">
         <v>76</v>
@@ -4507,7 +4555,7 @@
     </row>
     <row r="86" spans="2:7">
       <c r="B86" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C86" t="s">
         <v>94</v>
@@ -4518,8 +4566,8 @@
       <c r="E86" t="s">
         <v>78</v>
       </c>
-      <c r="F86" s="4" t="s">
-        <v>83</v>
+      <c r="F86" t="s">
+        <v>82</v>
       </c>
       <c r="G86" t="s">
         <v>76</v>
@@ -4527,7 +4575,7 @@
     </row>
     <row r="87" spans="2:7">
       <c r="B87" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C87" t="s">
         <v>94</v>
@@ -4539,7 +4587,7 @@
         <v>78</v>
       </c>
       <c r="F87" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G87" t="s">
         <v>76</v>
@@ -4547,7 +4595,7 @@
     </row>
     <row r="88" spans="2:7">
       <c r="B88" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C88" t="s">
         <v>94</v>
@@ -4559,7 +4607,7 @@
         <v>78</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G88" t="s">
         <v>76</v>
@@ -4567,7 +4615,7 @@
     </row>
     <row r="89" spans="2:7">
       <c r="B89" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C89" t="s">
         <v>94</v>
@@ -4579,7 +4627,7 @@
         <v>78</v>
       </c>
       <c r="F89" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G89" t="s">
         <v>76</v>
@@ -4587,7 +4635,7 @@
     </row>
     <row r="90" spans="2:7">
       <c r="B90" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C90" t="s">
         <v>94</v>
@@ -4599,7 +4647,7 @@
         <v>78</v>
       </c>
       <c r="F90" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G90" t="s">
         <v>76</v>
@@ -4607,19 +4655,19 @@
     </row>
     <row r="91" spans="2:7">
       <c r="B91" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C91" t="s">
         <v>94</v>
       </c>
       <c r="D91" t="s">
-        <v>138</v>
+        <v>77</v>
       </c>
       <c r="E91" t="s">
         <v>78</v>
       </c>
-      <c r="F91" t="s">
-        <v>88</v>
+      <c r="F91" s="4" t="s">
+        <v>87</v>
       </c>
       <c r="G91" t="s">
         <v>76</v>
@@ -4627,7 +4675,7 @@
     </row>
     <row r="92" spans="2:7">
       <c r="B92" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C92" t="s">
         <v>94</v>
@@ -4639,7 +4687,7 @@
         <v>78</v>
       </c>
       <c r="F92" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G92" t="s">
         <v>76</v>
@@ -4647,16 +4695,19 @@
     </row>
     <row r="93" spans="2:7">
       <c r="B93" t="s">
-        <v>226</v>
+        <v>38</v>
       </c>
       <c r="C93" t="s">
         <v>94</v>
       </c>
       <c r="D93" t="s">
-        <v>232</v>
+        <v>138</v>
+      </c>
+      <c r="E93" t="s">
+        <v>78</v>
       </c>
       <c r="F93" t="s">
-        <v>229</v>
+        <v>89</v>
       </c>
       <c r="G93" t="s">
         <v>76</v>
@@ -4664,7 +4715,7 @@
     </row>
     <row r="94" spans="2:7">
       <c r="B94" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C94" t="s">
         <v>94</v>
@@ -4673,7 +4724,7 @@
         <v>232</v>
       </c>
       <c r="F94" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G94" t="s">
         <v>76</v>
@@ -4681,7 +4732,7 @@
     </row>
     <row r="95" spans="2:7">
       <c r="B95" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C95" t="s">
         <v>94</v>
@@ -4690,7 +4741,7 @@
         <v>232</v>
       </c>
       <c r="F95" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G95" t="s">
         <v>76</v>
@@ -4698,24 +4749,24 @@
     </row>
     <row r="96" spans="2:7">
       <c r="B96" t="s">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="C96" t="s">
         <v>94</v>
       </c>
       <c r="D96" t="s">
-        <v>139</v>
+        <v>232</v>
       </c>
       <c r="F96" t="s">
-        <v>91</v>
+        <v>231</v>
       </c>
       <c r="G96" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="97" spans="2:7">
       <c r="B97" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C97" t="s">
         <v>94</v>
@@ -4724,7 +4775,7 @@
         <v>139</v>
       </c>
       <c r="F97" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G97" t="s">
         <v>92</v>
@@ -4732,7 +4783,7 @@
     </row>
     <row r="98" spans="2:7">
       <c r="B98" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C98" t="s">
         <v>94</v>
@@ -4741,7 +4792,7 @@
         <v>139</v>
       </c>
       <c r="F98" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="G98" t="s">
         <v>92</v>
@@ -4749,24 +4800,24 @@
     </row>
     <row r="99" spans="2:7">
       <c r="B99" t="s">
-        <v>141</v>
+        <v>193</v>
       </c>
       <c r="C99" t="s">
         <v>94</v>
       </c>
       <c r="D99" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="F99" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="G99" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
     </row>
     <row r="100" spans="2:7">
       <c r="B100" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C100" t="s">
         <v>94</v>
@@ -4775,7 +4826,7 @@
         <v>144</v>
       </c>
       <c r="F100" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G100" t="s">
         <v>146</v>
@@ -4783,7 +4834,7 @@
     </row>
     <row r="101" spans="2:7">
       <c r="B101" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C101" t="s">
         <v>94</v>
@@ -4792,7 +4843,7 @@
         <v>144</v>
       </c>
       <c r="F101" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G101" t="s">
         <v>146</v>
@@ -4800,7 +4851,7 @@
     </row>
     <row r="102" spans="2:7">
       <c r="B102" t="s">
-        <v>57</v>
+        <v>142</v>
       </c>
       <c r="C102" t="s">
         <v>94</v>
@@ -4809,7 +4860,7 @@
         <v>144</v>
       </c>
       <c r="F102" t="s">
-        <v>197</v>
+        <v>148</v>
       </c>
       <c r="G102" t="s">
         <v>146</v>
@@ -4817,7 +4868,7 @@
     </row>
     <row r="103" spans="2:7">
       <c r="B103" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C103" t="s">
         <v>94</v>
@@ -4826,51 +4877,50 @@
         <v>144</v>
       </c>
       <c r="F103" t="s">
-        <v>150</v>
+        <v>197</v>
       </c>
       <c r="G103" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="104" spans="2:7">
-      <c r="B104" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C104" s="13" t="s">
-        <v>220</v>
-      </c>
-      <c r="D104" s="13" t="s">
-        <v>221</v>
-      </c>
-      <c r="E104" s="13"/>
-      <c r="F104" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G104" s="13" t="s">
-        <v>76</v>
+      <c r="B104" t="s">
+        <v>50</v>
+      </c>
+      <c r="C104" t="s">
+        <v>94</v>
+      </c>
+      <c r="D104" t="s">
+        <v>144</v>
+      </c>
+      <c r="F104" t="s">
+        <v>150</v>
+      </c>
+      <c r="G104" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="105" spans="2:7">
       <c r="B105" s="13" t="s">
-        <v>266</v>
+        <v>28</v>
       </c>
       <c r="C105" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D105" s="13" t="s">
-        <v>264</v>
+        <v>221</v>
       </c>
       <c r="E105" s="13"/>
       <c r="F105" s="13" t="s">
-        <v>267</v>
+        <v>79</v>
       </c>
       <c r="G105" s="13" t="s">
-        <v>252</v>
+        <v>76</v>
       </c>
     </row>
     <row r="106" spans="2:7">
       <c r="B106" s="13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C106" s="13" t="s">
         <v>220</v>
@@ -4880,7 +4930,7 @@
       </c>
       <c r="E106" s="13"/>
       <c r="F106" s="13" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G106" s="13" t="s">
         <v>252</v>
@@ -4888,7 +4938,7 @@
     </row>
     <row r="107" spans="2:7">
       <c r="B107" s="13" t="s">
-        <v>263</v>
+        <v>271</v>
       </c>
       <c r="C107" s="13" t="s">
         <v>220</v>
@@ -4898,7 +4948,7 @@
       </c>
       <c r="E107" s="13"/>
       <c r="F107" s="13" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="G107" s="13" t="s">
         <v>252</v>
@@ -4906,17 +4956,17 @@
     </row>
     <row r="108" spans="2:7">
       <c r="B108" s="13" t="s">
-        <v>254</v>
+        <v>268</v>
       </c>
       <c r="C108" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D108" s="13" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E108" s="13"/>
       <c r="F108" s="13" t="s">
-        <v>259</v>
+        <v>269</v>
       </c>
       <c r="G108" s="13" t="s">
         <v>252</v>
@@ -4924,17 +4974,17 @@
     </row>
     <row r="109" spans="2:7">
       <c r="B109" s="13" t="s">
-        <v>255</v>
+        <v>263</v>
       </c>
       <c r="C109" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D109" s="13" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E109" s="13"/>
       <c r="F109" s="13" t="s">
-        <v>260</v>
+        <v>265</v>
       </c>
       <c r="G109" s="13" t="s">
         <v>252</v>
@@ -4942,7 +4992,7 @@
     </row>
     <row r="110" spans="2:7">
       <c r="B110" s="13" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C110" s="13" t="s">
         <v>220</v>
@@ -4952,7 +5002,7 @@
       </c>
       <c r="E110" s="13"/>
       <c r="F110" s="13" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="G110" s="13" t="s">
         <v>252</v>
@@ -4960,7 +5010,7 @@
     </row>
     <row r="111" spans="2:7">
       <c r="B111" s="13" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C111" s="13" t="s">
         <v>220</v>
@@ -4970,7 +5020,7 @@
       </c>
       <c r="E111" s="13"/>
       <c r="F111" s="13" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="G111" s="13" t="s">
         <v>252</v>
@@ -4978,17 +5028,17 @@
     </row>
     <row r="112" spans="2:7">
       <c r="B112" s="13" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="C112" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D112" s="13" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="E112" s="13"/>
       <c r="F112" s="13" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="G112" s="13" t="s">
         <v>252</v>
@@ -4996,61 +5046,61 @@
     </row>
     <row r="113" spans="2:7">
       <c r="B113" s="13" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="C113" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D113" s="13" t="s">
-        <v>248</v>
+        <v>258</v>
       </c>
       <c r="E113" s="13"/>
       <c r="F113" s="13" t="s">
-        <v>249</v>
+        <v>262</v>
       </c>
       <c r="G113" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" spans="2:7">
       <c r="B114" s="13" t="s">
-        <v>29</v>
+        <v>250</v>
       </c>
       <c r="C114" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D114" s="13" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="E114" s="13"/>
       <c r="F114" s="13" t="s">
-        <v>80</v>
+        <v>249</v>
       </c>
       <c r="G114" s="13" t="s">
-        <v>76</v>
+        <v>252</v>
       </c>
     </row>
     <row r="115" spans="2:7">
       <c r="B115" s="13" t="s">
-        <v>30</v>
+        <v>251</v>
       </c>
       <c r="C115" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D115" s="13" t="s">
-        <v>221</v>
+        <v>248</v>
       </c>
       <c r="E115" s="13"/>
       <c r="F115" s="13" t="s">
-        <v>81</v>
+        <v>249</v>
       </c>
       <c r="G115" s="13" t="s">
-        <v>76</v>
+        <v>253</v>
       </c>
     </row>
     <row r="116" spans="2:7">
       <c r="B116" s="13" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C116" s="13" t="s">
         <v>220</v>
@@ -5060,7 +5110,7 @@
       </c>
       <c r="E116" s="13"/>
       <c r="F116" s="13" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="G116" s="13" t="s">
         <v>76</v>
@@ -5068,7 +5118,7 @@
     </row>
     <row r="117" spans="2:7">
       <c r="B117" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C117" s="13" t="s">
         <v>220</v>
@@ -5078,7 +5128,7 @@
       </c>
       <c r="E117" s="13"/>
       <c r="F117" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G117" s="13" t="s">
         <v>76</v>
@@ -5086,7 +5136,7 @@
     </row>
     <row r="118" spans="2:7">
       <c r="B118" s="13" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C118" s="13" t="s">
         <v>220</v>
@@ -5096,7 +5146,7 @@
       </c>
       <c r="E118" s="13"/>
       <c r="F118" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="G118" s="13" t="s">
         <v>76</v>
@@ -5104,7 +5154,7 @@
     </row>
     <row r="119" spans="2:7">
       <c r="B119" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C119" s="13" t="s">
         <v>220</v>
@@ -5114,7 +5164,7 @@
       </c>
       <c r="E119" s="13"/>
       <c r="F119" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G119" s="13" t="s">
         <v>76</v>
@@ -5122,7 +5172,7 @@
     </row>
     <row r="120" spans="2:7">
       <c r="B120" s="13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C120" s="13" t="s">
         <v>220</v>
@@ -5132,7 +5182,7 @@
       </c>
       <c r="E120" s="13"/>
       <c r="F120" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G120" s="13" t="s">
         <v>76</v>
@@ -5140,7 +5190,7 @@
     </row>
     <row r="121" spans="2:7">
       <c r="B121" s="13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C121" s="13" t="s">
         <v>220</v>
@@ -5150,7 +5200,7 @@
       </c>
       <c r="E121" s="13"/>
       <c r="F121" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="G121" s="13" t="s">
         <v>76</v>
@@ -5158,7 +5208,7 @@
     </row>
     <row r="122" spans="2:7">
       <c r="B122" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C122" s="13" t="s">
         <v>220</v>
@@ -5168,7 +5218,7 @@
       </c>
       <c r="E122" s="13"/>
       <c r="F122" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G122" s="13" t="s">
         <v>76</v>
@@ -5176,7 +5226,7 @@
     </row>
     <row r="123" spans="2:7">
       <c r="B123" s="13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C123" s="13" t="s">
         <v>220</v>
@@ -5186,7 +5236,7 @@
       </c>
       <c r="E123" s="13"/>
       <c r="F123" s="13" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G123" s="13" t="s">
         <v>76</v>
@@ -5194,7 +5244,7 @@
     </row>
     <row r="124" spans="2:7">
       <c r="B124" s="13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C124" s="13" t="s">
         <v>220</v>
@@ -5204,7 +5254,7 @@
       </c>
       <c r="E124" s="13"/>
       <c r="F124" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G124" s="13" t="s">
         <v>76</v>
@@ -5212,7 +5262,7 @@
     </row>
     <row r="125" spans="2:7">
       <c r="B125" s="13" t="s">
-        <v>226</v>
+        <v>37</v>
       </c>
       <c r="C125" s="13" t="s">
         <v>220</v>
@@ -5222,7 +5272,7 @@
       </c>
       <c r="E125" s="13"/>
       <c r="F125" s="13" t="s">
-        <v>229</v>
+        <v>88</v>
       </c>
       <c r="G125" s="13" t="s">
         <v>76</v>
@@ -5230,7 +5280,7 @@
     </row>
     <row r="126" spans="2:7">
       <c r="B126" s="13" t="s">
-        <v>227</v>
+        <v>38</v>
       </c>
       <c r="C126" s="13" t="s">
         <v>220</v>
@@ -5240,7 +5290,7 @@
       </c>
       <c r="E126" s="13"/>
       <c r="F126" s="13" t="s">
-        <v>230</v>
+        <v>89</v>
       </c>
       <c r="G126" s="13" t="s">
         <v>76</v>
@@ -5248,7 +5298,7 @@
     </row>
     <row r="127" spans="2:7">
       <c r="B127" s="13" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C127" s="13" t="s">
         <v>220</v>
@@ -5258,7 +5308,7 @@
       </c>
       <c r="E127" s="13"/>
       <c r="F127" s="13" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="G127" s="13" t="s">
         <v>76</v>
@@ -5266,7 +5316,7 @@
     </row>
     <row r="128" spans="2:7">
       <c r="B128" s="13" t="s">
-        <v>191</v>
+        <v>227</v>
       </c>
       <c r="C128" s="13" t="s">
         <v>220</v>
@@ -5276,15 +5326,15 @@
       </c>
       <c r="E128" s="13"/>
       <c r="F128" s="13" t="s">
-        <v>91</v>
+        <v>230</v>
       </c>
       <c r="G128" s="13" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="129" spans="2:7">
       <c r="B129" s="13" t="s">
-        <v>192</v>
+        <v>228</v>
       </c>
       <c r="C129" s="13" t="s">
         <v>220</v>
@@ -5294,15 +5344,15 @@
       </c>
       <c r="E129" s="13"/>
       <c r="F129" s="13" t="s">
-        <v>90</v>
+        <v>231</v>
       </c>
       <c r="G129" s="13" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
     </row>
     <row r="130" spans="2:7">
       <c r="B130" s="13" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C130" s="13" t="s">
         <v>220</v>
@@ -5312,7 +5362,7 @@
       </c>
       <c r="E130" s="13"/>
       <c r="F130" s="13" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
       <c r="G130" s="13" t="s">
         <v>92</v>
@@ -5320,43 +5370,43 @@
     </row>
     <row r="131" spans="2:7">
       <c r="B131" s="13" t="s">
-        <v>141</v>
+        <v>192</v>
       </c>
       <c r="C131" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D131" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E131" s="13"/>
       <c r="F131" s="13" t="s">
-        <v>145</v>
+        <v>90</v>
       </c>
       <c r="G131" s="13" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
     </row>
     <row r="132" spans="2:7">
       <c r="B132" s="13" t="s">
-        <v>143</v>
+        <v>193</v>
       </c>
       <c r="C132" s="13" t="s">
         <v>220</v>
       </c>
       <c r="D132" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E132" s="13"/>
       <c r="F132" s="13" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="G132" s="13" t="s">
-        <v>146</v>
+        <v>92</v>
       </c>
     </row>
     <row r="133" spans="2:7">
       <c r="B133" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C133" s="13" t="s">
         <v>220</v>
@@ -5366,7 +5416,7 @@
       </c>
       <c r="E133" s="13"/>
       <c r="F133" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G133" s="13" t="s">
         <v>146</v>
@@ -5374,7 +5424,7 @@
     </row>
     <row r="134" spans="2:7">
       <c r="B134" s="13" t="s">
-        <v>57</v>
+        <v>143</v>
       </c>
       <c r="C134" s="13" t="s">
         <v>220</v>
@@ -5384,7 +5434,7 @@
       </c>
       <c r="E134" s="13"/>
       <c r="F134" s="13" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="G134" s="13" t="s">
         <v>146</v>
@@ -5392,7 +5442,7 @@
     </row>
     <row r="135" spans="2:7">
       <c r="B135" s="13" t="s">
-        <v>50</v>
+        <v>142</v>
       </c>
       <c r="C135" s="13" t="s">
         <v>220</v>
@@ -5402,34 +5452,70 @@
       </c>
       <c r="E135" s="13"/>
       <c r="F135" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="G135" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="136" spans="2:7">
+      <c r="B136" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="C136" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D136" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E136" s="13"/>
+      <c r="F136" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="G136" s="13" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="137" spans="2:7">
+      <c r="B137" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C137" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D137" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E137" s="13"/>
+      <c r="F137" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="G135" s="13" t="s">
+      <c r="G137" s="13" t="s">
         <v>146</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I45:I64 I6:I37" xr:uid="{3AF342F9-C154-4566-A6D6-DF321DDA9F17}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I46:I65 I6:I38" xr:uid="{3AF342F9-C154-4566-A6D6-DF321DDA9F17}">
       <formula1>list.Files_geo_unique</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{EA6C777B-C12B-4DA7-8BB7-7DDC99E580DB}">
       <formula1>list.File_Loc.Users</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D45:D64 B72:B135" xr:uid="{89EA6ADA-E6CC-4F9F-8692-D86D51F6962E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D46:D65 B73:B137" xr:uid="{89EA6ADA-E6CC-4F9F-8692-D86D51F6962E}">
       <formula1>list.Files_unique</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M45:M64" xr:uid="{30B9C429-7EFE-4DEB-8979-C009F9C29D27}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M46:M65" xr:uid="{30B9C429-7EFE-4DEB-8979-C009F9C29D27}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J45:J64" xr:uid="{5A7219B4-496A-4564-B050-1C5EC592B3C4}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J46:J65" xr:uid="{5A7219B4-496A-4564-B050-1C5EC592B3C4}">
       <formula1>list.Data_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K45:K64" xr:uid="{F772E2DB-4630-467B-AA9F-63204FD4B8D8}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K46:K65" xr:uid="{F772E2DB-4630-467B-AA9F-63204FD4B8D8}">
       <formula1>list.Weight_type</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D37" xr:uid="{53F75F56-0961-4D59-9F5F-5CC227CBB16D}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D6:D38" xr:uid="{53F75F56-0961-4D59-9F5F-5CC227CBB16D}">
       <formula1>list.File_structures</formula1>
     </dataValidation>
   </dataValidations>
@@ -5695,10 +5781,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1D767F-008E-40CD-A786-127BCF11776D}">
-  <dimension ref="B4:N12"/>
+  <dimension ref="B4:Q16"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -5711,210 +5797,326 @@
     <col min="12" max="12" width="24.125" customWidth="1"/>
     <col min="13" max="13" width="29.125" customWidth="1"/>
     <col min="14" max="14" width="45" customWidth="1"/>
+    <col min="16" max="16" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:17">
       <c r="B4" t="s">
         <v>137</v>
       </c>
       <c r="C4" t="str" cm="1">
-        <f t="array" ref="C4">_xlfn.TEXTJOIN(", ",TRUE, "'"&amp;B9:B12&amp;"'")</f>
-        <v>'STM2_newEmit_Orig-Arch_test_New-Country_test', 'STM3_newEmit_Orig-Arch_test_New-Country_test_Pop2010', 'STM2_newEmit_Orig-Arch_test_split_New-Countries', 'STM2_newEmit_Orig-Arch_test_New-Countries'</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14">
-      <c r="B7" t="s">
+        <f t="array" ref="C4">_xlfn.TEXTJOIN(", ",TRUE, "'"&amp;B11:B16&amp;"'")</f>
+        <v>'STM2_newEmit_Orig-Arch_test_New-Country_test', 'STM3_newEmit_Orig-Arch_test_New-Country_test_Pop2010', 'STM2_newEmit_Orig-ArchFullUrb2v02_prep01_New-Country_test', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Country_test_Pop2010', 'STM2_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010'</v>
+      </c>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="B6" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" t="b">
+        <f>ROWS(_xlfn.UNIQUE(Tbl.SpatialTransforms[STM unique name]))=ROWS(Tbl.SpatialTransforms[STM unique name])</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="B9" t="s">
         <v>58</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E9" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="8" spans="2:14">
-      <c r="B8" t="s">
+      <c r="P9" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" t="s">
         <v>59</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C10" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D10" t="s">
         <v>111</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E10" t="s">
         <v>8</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F10" t="s">
         <v>9</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G10" t="s">
         <v>5</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H10" t="s">
         <v>10</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I10" t="s">
         <v>64</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J10" t="s">
         <v>122</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K10" t="s">
         <v>123</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L10" t="s">
         <v>124</v>
       </c>
-      <c r="M8" t="s">
+      <c r="M10" t="s">
         <v>114</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="9" spans="2:14">
-      <c r="B9" t="str">
+      <c r="P10" t="s">
+        <v>274</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM2_newEmit_Orig-Arch_test_New-Country_test</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G9" t="str">
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
         <v>STM2_newEmit_Orig-Arch_test_New-Country_test</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H11" t="s">
         <v>194</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I11" t="s">
         <v>117</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J11" t="s">
         <v>263</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K11" t="s">
         <v>266</v>
       </c>
-      <c r="M9" t="b">
+      <c r="M11" t="b">
         <v>1</v>
       </c>
-      <c r="N9" t="str">
+      <c r="N11" t="str">
         <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
         <v>STM2_newEmit_Orig-Arch_test_New-Country_test</v>
       </c>
-    </row>
-    <row r="10" spans="2:14">
-      <c r="B10" t="str">
+      <c r="P11">
+        <f>15/60</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="B12" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM3_newEmit_Orig-Arch_test_New-Country_test_Pop2010</v>
       </c>
-      <c r="D10" t="b">
-        <v>1</v>
-      </c>
-      <c r="G10" t="str">
+      <c r="D12" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
         <v>STM3_newEmit_Orig-Arch_test_New-Country_test_Pop2010</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H12" t="s">
         <v>194</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I12" t="s">
         <v>117</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J12" t="s">
         <v>263</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K12" t="s">
         <v>266</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L12" t="s">
         <v>32</v>
       </c>
-      <c r="M10" t="b">
+      <c r="M12" t="b">
         <v>1</v>
       </c>
-      <c r="N10" t="str">
+      <c r="N12" t="str">
         <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
         <v>STM3_newEmit_Orig-Arch_test_New-Country_test_Pop2010</v>
       </c>
-    </row>
-    <row r="11" spans="2:14">
-      <c r="B11" t="str">
+      <c r="P12">
+        <f>24/60</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="B13" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM2_newEmit_Orig-Arch_test_split_New-Countries</v>
-      </c>
-      <c r="D11" t="b">
+        <v>STM2_newEmit_Orig-ArchFullUrb2v02_prep01_New-Country_test</v>
+      </c>
+      <c r="D13" t="b">
         <v>0</v>
       </c>
-      <c r="G11" t="str">
+      <c r="G13" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM2_newEmit_Orig-Arch_test_split_New-Countries</v>
-      </c>
-      <c r="H11" t="s">
+        <v>STM2_newEmit_Orig-ArchFullUrb2v02_prep01_New-Country_test</v>
+      </c>
+      <c r="H13" t="s">
         <v>194</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I13" t="s">
         <v>117</v>
       </c>
-      <c r="J11" t="s">
-        <v>268</v>
-      </c>
-      <c r="K11" t="s">
+      <c r="J13" t="s">
+        <v>271</v>
+      </c>
+      <c r="K13" t="s">
+        <v>266</v>
+      </c>
+      <c r="M13" t="b">
+        <v>1</v>
+      </c>
+      <c r="N13" t="str">
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM2_newEmit_Orig-ArchFullUrb2v02_prep01_New-Country_test</v>
+      </c>
+      <c r="P13">
+        <f>25/60</f>
+        <v>0.41666666666666669</v>
+      </c>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="B14" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Country_test_Pop2010</v>
+      </c>
+      <c r="D14" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Country_test_Pop2010</v>
+      </c>
+      <c r="H14" t="s">
+        <v>194</v>
+      </c>
+      <c r="I14" t="s">
+        <v>117</v>
+      </c>
+      <c r="J14" t="s">
+        <v>271</v>
+      </c>
+      <c r="K14" t="s">
+        <v>266</v>
+      </c>
+      <c r="L14" t="s">
+        <v>32</v>
+      </c>
+      <c r="M14" t="b">
+        <v>1</v>
+      </c>
+      <c r="N14" s="14" t="str">
+        <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Country_test_Pop2010</v>
+      </c>
+      <c r="P14">
+        <f>46/60</f>
+        <v>0.76666666666666672</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="B15" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
+        <v>STM2_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries</v>
+      </c>
+      <c r="D15" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" t="str">
+        <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
+        <v>STM2_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries</v>
+      </c>
+      <c r="H15" t="s">
+        <v>194</v>
+      </c>
+      <c r="I15" t="s">
+        <v>117</v>
+      </c>
+      <c r="J15" t="s">
+        <v>271</v>
+      </c>
+      <c r="K15" t="s">
         <v>28</v>
       </c>
-      <c r="M11" t="b">
+      <c r="M15" t="b">
         <v>1</v>
       </c>
-      <c r="N11" t="str">
+      <c r="N15" t="str">
         <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM2_newEmit_Orig-Arch_test_split_New-Countries</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14">
-      <c r="B12" t="str">
+        <v>STM2_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries</v>
+      </c>
+      <c r="P15">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="B16" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM2_newEmit_Orig-Arch_test_New-Countries</v>
-      </c>
-      <c r="D12" t="b">
-        <v>0</v>
-      </c>
-      <c r="G12" t="str">
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+      </c>
+      <c r="D16" t="b">
+        <v>1</v>
+      </c>
+      <c r="G16" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM2_newEmit_Orig-Arch_test_New-Countries</v>
-      </c>
-      <c r="H12" t="s">
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+      </c>
+      <c r="H16" t="s">
         <v>194</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I16" t="s">
         <v>117</v>
       </c>
-      <c r="J12" t="s">
-        <v>263</v>
-      </c>
-      <c r="K12" t="s">
+      <c r="J16" t="s">
+        <v>271</v>
+      </c>
+      <c r="K16" t="s">
         <v>28</v>
       </c>
-      <c r="M12" t="b">
+      <c r="L16" t="s">
+        <v>32</v>
+      </c>
+      <c r="M16" t="b">
         <v>1</v>
       </c>
-      <c r="N12" t="str">
+      <c r="N16" t="str">
         <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM2_newEmit_Orig-Arch_test_New-Countries</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+      </c>
+      <c r="P16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q16">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I12" xr:uid="{E821405C-6957-4A9F-8765-11FEDC830D01}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I11:I16" xr:uid="{E821405C-6957-4A9F-8765-11FEDC830D01}">
       <formula1>list.STM_types</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L9:L12" xr:uid="{5BDCD423-46E4-4A7B-8628-5C9344A21620}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L11:L16" xr:uid="{5BDCD423-46E4-4A7B-8628-5C9344A21620}">
       <formula1>list.Data_unique</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M12" xr:uid="{30B9C429-7EFE-4DEB-8979-C009F9C29D27}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M11:M16" xr:uid="{30B9C429-7EFE-4DEB-8979-C009F9C29D27}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J9:K12" xr:uid="{3AF342F9-C154-4566-A6D6-DF321DDA9F17}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11:K16" xr:uid="{3AF342F9-C154-4566-A6D6-DF321DDA9F17}">
       <formula1>list.Files_geo_unique</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Fix indexing Check to see if colID provided first; if not, then force addition.  If index is fid, then increment it by 1 (to match the geopackage).
</commit_message>
<xml_diff>
--- a/calc/ozone STM calc setup v00a.xlsx
+++ b/calc/ozone STM calc setup v00a.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CalcDir\TRACI_ozone_stm\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0016937-6612-46AD-8014-F7C5890FD976}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06E5A53-82BD-4CF9-83C6-B00B56B7A562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -1177,10 +1177,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1482,7 +1482,7 @@
     <tableColumn id="5" xr3:uid="{AE90259D-C343-4380-B54E-4F5CB63A2684}" name="New Geofile"/>
     <tableColumn id="6" xr3:uid="{0517F68E-B086-4B29-BCBB-FD080B95A1FD}" name="Weight Data"/>
     <tableColumn id="13" xr3:uid="{941AE024-63C8-477F-9C19-AB394C4E3067}" name="Use Existing"/>
-    <tableColumn id="7" xr3:uid="{DC381ACA-0C61-4D84-BCD2-331C1153758A}" name="Auto file name" dataDxfId="0">
+    <tableColumn id="7" xr3:uid="{DC381ACA-0C61-4D84-BCD2-331C1153758A}" name="Auto file name" dataDxfId="2">
       <calculatedColumnFormula>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1491,7 +1491,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B44F7711-2BBD-4E1B-B88E-ED6C45B7E8A5}" name="Tbl.Calc" displayName="Tbl.Calc" ref="F8:X71" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B44F7711-2BBD-4E1B-B88E-ED6C45B7E8A5}" name="Tbl.Calc" displayName="Tbl.Calc" ref="F8:X71" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="F8:X71" xr:uid="{B44F7711-2BBD-4E1B-B88E-ED6C45B7E8A5}"/>
   <tableColumns count="19">
     <tableColumn id="15" xr3:uid="{63913522-0BFE-4696-873E-B4148EA4C495}" name="Calc Num">
@@ -1506,7 +1506,7 @@
     <tableColumn id="10" xr3:uid="{31E957E8-AA7D-475B-A9F0-F044834548C3}" name="New Emit Resolution"/>
     <tableColumn id="17" xr3:uid="{F66257FA-C678-4EEC-9987-2015AAF1A0EA}" name="Emit Weighting Sector"/>
     <tableColumn id="5" xr3:uid="{C53E261C-C2AC-4E59-9C17-4E9BD692BE8E}" name="Emit Weighting Data"/>
-    <tableColumn id="12" xr3:uid="{BE306CBD-148A-461F-B1D9-7302AAC03FDC}" name="Emit STM" dataDxfId="1">
+    <tableColumn id="12" xr3:uid="{BE306CBD-148A-461F-B1D9-7302AAC03FDC}" name="Emit STM" dataDxfId="0">
       <calculatedColumnFormula array="1">IF(Tbl.Calc[[#This Row],[Orig Emit Resolution]]=Tbl.Calc[[#This Row],[New Emit Resolution]], "",
 _xlfn._xlws.FILTER(Tbl.SpatialTransforms[STM unique name],(Tbl.SpatialTransforms[STM type]=str.stm_type.NewEmit)*(Tbl.Calc[[#This Row],[Orig Emit Resolution]]=Tbl.SpatialTransforms[Orig Geofile])*(Tbl.Calc[[#This Row],[New Emit Resolution]]=Tbl.SpatialTransforms[New Geofile])*(Tbl.Calc[[#This Row],[Emit Weighting Data]]=Tbl.SpatialTransforms[Weight Data]))
 )</calculatedColumnFormula>
@@ -2480,8 +2480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2502FB-B45F-43BB-8645-D93E9F9C6CDF}">
   <dimension ref="B2:O147"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2522,7 +2522,7 @@
         <v>93</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>94</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="2:14">
@@ -2580,11 +2580,11 @@
       </c>
       <c r="E6" t="str" cm="1">
         <f t="array" ref="E6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F6" t="str" cm="1">
         <f t="array" ref="F6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G6" t="str" cm="1">
         <f t="array" ref="G6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2610,7 +2610,7 @@
       </c>
       <c r="M6" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="7" spans="2:14">
@@ -3005,7 +3005,7 @@
       </c>
       <c r="F18" t="str" cm="1">
         <f t="array" ref="F18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>anthro_compiled_v01</v>
+        <v/>
       </c>
       <c r="G18" t="str" cm="1">
         <f t="array" ref="G18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="M18" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\anthro_compiled_v01</v>
+        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
       </c>
     </row>
     <row r="19" spans="2:13">
@@ -3073,11 +3073,11 @@
       </c>
       <c r="E20" t="str" cm="1">
         <f t="array" ref="E20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F20" t="str" cm="1">
         <f t="array" ref="F20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G20" t="str" cm="1">
         <f t="array" ref="G20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3100,7 +3100,7 @@
       </c>
       <c r="M20" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="21" spans="2:13">
@@ -3112,11 +3112,11 @@
       </c>
       <c r="E21" t="str" cm="1">
         <f t="array" ref="E21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F21" t="str" cm="1">
         <f t="array" ref="F21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G21" t="str" cm="1">
         <f t="array" ref="G21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3142,7 +3142,7 @@
       </c>
       <c r="M21" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="22" spans="2:13">
@@ -3154,7 +3154,7 @@
       </c>
       <c r="E22" t="str" cm="1">
         <f t="array" ref="E22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>W:\data\geo\ecoregions_teow\Olson_2012\official</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F22" t="str" cm="1">
         <f t="array" ref="F22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3181,7 +3181,7 @@
       </c>
       <c r="M22" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>W:\data\geo\ecoregions_teow\Olson_2012\official\</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="23" spans="2:13">
@@ -3193,11 +3193,11 @@
       </c>
       <c r="E23" t="str" cm="1">
         <f t="array" ref="E23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F23" t="str" cm="1">
         <f t="array" ref="F23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G23" t="str" cm="1">
         <f t="array" ref="G23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3217,7 +3217,7 @@
       </c>
       <c r="M23" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="24" spans="2:13">
@@ -3229,11 +3229,11 @@
       </c>
       <c r="E24" t="str" cm="1">
         <f t="array" ref="E24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F24" t="str" cm="1">
         <f t="array" ref="F24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G24" t="str" cm="1">
         <f t="array" ref="G24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3253,7 +3253,7 @@
       </c>
       <c r="M24" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="25" spans="2:13">
@@ -3265,11 +3265,11 @@
       </c>
       <c r="E25" t="str" cm="1">
         <f t="array" ref="E25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F25" t="str" cm="1">
         <f t="array" ref="F25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G25" t="str" cm="1">
         <f t="array" ref="G25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3289,7 +3289,7 @@
       </c>
       <c r="M25" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="26" spans="2:13">
@@ -3301,11 +3301,11 @@
       </c>
       <c r="E26" t="str" cm="1">
         <f t="array" ref="E26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F26" t="str" cm="1">
         <f t="array" ref="F26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G26" t="str" cm="1">
         <f t="array" ref="G26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3325,7 +3325,7 @@
       </c>
       <c r="M26" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="27" spans="2:13">
@@ -3337,11 +3337,11 @@
       </c>
       <c r="E27" t="str" cm="1">
         <f t="array" ref="E27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F27" t="str" cm="1">
         <f t="array" ref="F27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G27" t="str" cm="1">
         <f t="array" ref="G27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="M27" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="28" spans="2:13">
@@ -3373,11 +3373,11 @@
       </c>
       <c r="E28" t="str" cm="1">
         <f t="array" ref="E28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F28" t="str" cm="1">
         <f t="array" ref="F28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G28" t="str" cm="1">
         <f t="array" ref="G28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3397,7 +3397,7 @@
       </c>
       <c r="M28" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="29" spans="2:13">
@@ -3409,11 +3409,11 @@
       </c>
       <c r="E29" t="str" cm="1">
         <f t="array" ref="E29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F29" t="str" cm="1">
         <f t="array" ref="F29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G29" t="str" cm="1">
         <f t="array" ref="G29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3433,7 +3433,7 @@
       </c>
       <c r="M29" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="30" spans="2:13">
@@ -3445,11 +3445,11 @@
       </c>
       <c r="E30" t="str" cm="1">
         <f t="array" ref="E30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F30" t="str" cm="1">
         <f t="array" ref="F30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G30" t="str" cm="1">
         <f t="array" ref="G30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3469,7 +3469,7 @@
       </c>
       <c r="M30" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="31" spans="2:13">
@@ -3481,7 +3481,7 @@
       </c>
       <c r="E31" t="str" cm="1">
         <f t="array" ref="E31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F31" t="str" cm="1">
         <f t="array" ref="F31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3503,7 +3503,7 @@
       </c>
       <c r="M31" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="32" spans="2:13">
@@ -3515,7 +3515,7 @@
       </c>
       <c r="E32" t="str" cm="1">
         <f t="array" ref="E32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F32" t="str" cm="1">
         <f t="array" ref="F32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3537,7 +3537,7 @@
       </c>
       <c r="M32" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="33" spans="2:15">
@@ -3549,7 +3549,7 @@
       </c>
       <c r="E33" t="str" cm="1">
         <f t="array" ref="E33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F33" t="str" cm="1">
         <f t="array" ref="F33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3571,7 +3571,7 @@
       </c>
       <c r="M33" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="34" spans="2:15">
@@ -3583,7 +3583,7 @@
       </c>
       <c r="E34" t="str" cm="1">
         <f t="array" ref="E34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F34" t="str" cm="1">
         <f t="array" ref="F34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3604,7 +3604,7 @@
       </c>
       <c r="M34" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="35" spans="2:15">
@@ -3616,7 +3616,7 @@
       </c>
       <c r="E35" t="str" cm="1">
         <f t="array" ref="E35">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F35" t="str" cm="1">
         <f t="array" ref="F35">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3637,7 +3637,7 @@
       </c>
       <c r="M35" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="36" spans="2:15">
@@ -3649,7 +3649,7 @@
       </c>
       <c r="E36" t="str" cm="1">
         <f t="array" ref="E36">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F36" t="str" cm="1">
         <f t="array" ref="F36">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3670,7 +3670,7 @@
       </c>
       <c r="M36" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
       </c>
     </row>
     <row r="37" spans="2:15">
@@ -3682,7 +3682,7 @@
       </c>
       <c r="E37" t="str" cm="1">
         <f t="array" ref="E37">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F37" t="str" cm="1">
         <f t="array" ref="F37">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3703,7 +3703,7 @@
       </c>
       <c r="M37" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
       </c>
     </row>
     <row r="38" spans="2:15">
@@ -3715,7 +3715,7 @@
       </c>
       <c r="E38" t="str" cm="1">
         <f t="array" ref="E38">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F38" t="str" cm="1">
         <f t="array" ref="F38">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3736,7 +3736,7 @@
       </c>
       <c r="M38" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
       </c>
     </row>
     <row r="39" spans="2:15">
@@ -3748,7 +3748,7 @@
       </c>
       <c r="E39" t="str" cm="1">
         <f t="array" ref="E39">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F39" t="str" cm="1">
         <f t="array" ref="F39">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3769,7 +3769,7 @@
       </c>
       <c r="M39" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
       </c>
     </row>
     <row r="40" spans="2:15">
@@ -3781,7 +3781,7 @@
       </c>
       <c r="E40" t="str" cm="1">
         <f t="array" ref="E40">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F40" t="str" cm="1">
         <f t="array" ref="F40">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="M40" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
       </c>
     </row>
     <row r="41" spans="2:15">
@@ -3814,7 +3814,7 @@
       </c>
       <c r="E41" t="str" cm="1">
         <f t="array" ref="E41">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F41" t="str" cm="1">
         <f t="array" ref="F41">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3835,7 +3835,7 @@
       </c>
       <c r="M41" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
       </c>
     </row>
     <row r="47" spans="2:15">
@@ -6028,7 +6028,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1D767F-008E-40CD-A786-127BCF11776D}">
   <dimension ref="B4:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
use archID_num: update gpkg from v01 to have archID_num and _text. Clean up the files used for testing the repair, holes, and simplification.
</commit_message>
<xml_diff>
--- a/calc/ozone STM calc setup v00a.xlsx
+++ b/calc/ozone STM calc setup v00a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CalcDir\TRACI_ozone_stm\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A06E5A53-82BD-4CF9-83C6-B00B56B7A562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391E455D-690B-4C03-92EF-8F79D76BC172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -75,37 +75,19 @@
   <commentList>
     <comment ref="I5" authorId="0" shapeId="0" xr:uid="{C3F9C59B-D4CD-4335-8367-A9C7977F41DA}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t xml:space="preserve">[Threaded comment]
+        <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This could be done in python, but it is calculated here.  Needed because the function fix_data_ids uses the path/file/extension to get the associated geofile.
 </t>
-        </r>
       </text>
     </comment>
     <comment ref="F48" authorId="1" shapeId="0" xr:uid="{C05BA83B-E4CC-4E37-B576-FA3EC5396FF7}">
       <text>
-        <r>
-          <rPr>
-            <sz val="11"/>
-            <color theme="1"/>
-            <rFont val="Aptos Narrow"/>
-            <family val="2"/>
-            <scheme val="minor"/>
-          </rPr>
-          <t>[Threaded comment]
+        <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This is redundant for the GIS files.  However, it's necessary in case the others come from an excel file (e.g.) with a different ID name than what is used in the associated geofile.</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -150,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="280">
   <si>
     <t>File unique name</t>
   </si>
@@ -965,9 +947,6 @@
     <t>ArchFullUrb2v02_prep01</t>
   </si>
   <si>
-    <t>repair1_holes10</t>
-  </si>
-  <si>
     <t>all unique</t>
   </si>
   <si>
@@ -987,6 +966,12 @@
   </si>
   <si>
     <t>archUrb2v01_repair1_holes10_urban</t>
+  </si>
+  <si>
+    <t>archUrb2v02_repair1_holes10</t>
+  </si>
+  <si>
+    <t>archID_num</t>
   </si>
 </sst>
 </file>
@@ -996,7 +981,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#000\-00\-0"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1121,7 +1106,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -1158,9 +1143,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1322,7 +1304,7 @@
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <global>
     <keyFlags>
       <key name="_Self">
@@ -1859,7 +1841,7 @@
     <text xml:space="preserve">This could be done in python, but it is calculated here.  Needed because the function fix_data_ids uses the path/file/extension to get the associated geofile.
 </text>
   </threadedComment>
-  <threadedComment ref="F46" dT="2024-03-27T18:27:30.51" personId="{6027BF47-3954-4784-9D7C-EBFA15F39BC9}" id="{C05BA83B-E4CC-4E37-B576-FA3EC5396FF7}">
+  <threadedComment ref="F48" dT="2024-03-27T18:27:30.51" personId="{6027BF47-3954-4784-9D7C-EBFA15F39BC9}" id="{C05BA83B-E4CC-4E37-B576-FA3EC5396FF7}">
     <text>This is redundant for the GIS files.  However, it's necessary in case the others come from an excel file (e.g.) with a different ID name than what is used in the associated geofile.</text>
   </threadedComment>
 </ThreadedComments>
@@ -1873,29 +1855,29 @@
       <selection activeCell="AC25" sqref="AC25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.875" customWidth="1"/>
-    <col min="3" max="3" width="19.625" customWidth="1"/>
-    <col min="4" max="4" width="23.375" customWidth="1"/>
-    <col min="5" max="5" width="24.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.625" customWidth="1"/>
-    <col min="7" max="7" width="23.375" customWidth="1"/>
-    <col min="8" max="8" width="20.625" customWidth="1"/>
-    <col min="9" max="9" width="15.375" customWidth="1"/>
-    <col min="10" max="10" width="20.625" customWidth="1"/>
-    <col min="12" max="13" width="30.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="43.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" customWidth="1"/>
+    <col min="12" max="13" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:22" ht="30">
+    <row r="7" spans="2:22" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1947,7 +1929,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="2:22">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>61</v>
       </c>
@@ -1990,7 +1972,7 @@
       </c>
       <c r="O8" t="str" cm="1">
         <f t="array" ref="O8:O11">Tbl.SpatialTransforms[STM unique name]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
       </c>
       <c r="Q8" t="str" cm="1">
         <f t="array" ref="Q8:Q16">Tbl.Flows[Flow unique Name]</f>
@@ -2017,7 +1999,7 @@
         <v>AnthroVOCs_v01_gpkg</v>
       </c>
     </row>
-    <row r="9" spans="2:22">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>100</v>
       </c>
@@ -2052,7 +2034,7 @@
         <v>air_FF_NHx</v>
       </c>
       <c r="O9" t="str">
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
       </c>
       <c r="Q9" t="str">
         <v>NO</v>
@@ -2067,7 +2049,7 @@
         <v>AnthroVOCs_v01_tif</v>
       </c>
     </row>
-    <row r="10" spans="2:22">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>159</v>
       </c>
@@ -2108,7 +2090,7 @@
         <v>Pop2010</v>
       </c>
     </row>
-    <row r="11" spans="2:22">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>115</v>
       </c>
@@ -2140,7 +2122,7 @@
         <v>Edgar Air Ag NH3</v>
       </c>
     </row>
-    <row r="12" spans="2:22">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
         <v>21</v>
       </c>
@@ -2160,7 +2142,7 @@
         <v>Edgar Air Ag NOx</v>
       </c>
     </row>
-    <row r="13" spans="2:22">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
         <v>45</v>
       </c>
@@ -2180,7 +2162,7 @@
         <v>Edgar Air Ag SO2</v>
       </c>
     </row>
-    <row r="14" spans="2:22">
+    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
         <v>172</v>
       </c>
@@ -2203,7 +2185,7 @@
         <v>Edgar Air NonAg NH3</v>
       </c>
     </row>
-    <row r="15" spans="2:22">
+    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L15" t="str">
         <v>Arch_test</v>
       </c>
@@ -2220,7 +2202,7 @@
         <v>Edgar Air NonAg NOx</v>
       </c>
     </row>
-    <row r="16" spans="2:22">
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
       <c r="L16" t="str">
         <v>Arch_Full_Urb2_v01</v>
       </c>
@@ -2237,7 +2219,7 @@
         <v>Edgar Air NonAg SO2</v>
       </c>
     </row>
-    <row r="17" spans="12:22">
+    <row r="17" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L17" t="str">
         <v>Arch_Full_Urb3_v01</v>
       </c>
@@ -2251,7 +2233,7 @@
         <v>Edgar Air Gen NH3</v>
       </c>
     </row>
-    <row r="18" spans="12:22">
+    <row r="18" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L18" t="str">
         <v>Arch_Full_Urb2_v02</v>
       </c>
@@ -2265,7 +2247,7 @@
         <v>Edgar Air Gen NOx</v>
       </c>
     </row>
-    <row r="19" spans="12:22">
+    <row r="19" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L19" t="str">
         <v>Arch_Full_Urb3_v02</v>
       </c>
@@ -2279,7 +2261,7 @@
         <v>Edgar Air Gen SO2</v>
       </c>
     </row>
-    <row r="20" spans="12:22">
+    <row r="20" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L20" t="str">
         <v>AnthroVOCs_v01_gpkg</v>
       </c>
@@ -2290,7 +2272,7 @@
         <v>Edgar Air Ag NOx</v>
       </c>
     </row>
-    <row r="21" spans="12:22">
+    <row r="21" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L21" t="str">
         <v>AnthroVOCs_v01_tif</v>
       </c>
@@ -2301,7 +2283,7 @@
         <v>Edgar Air Ag SO2</v>
       </c>
     </row>
-    <row r="22" spans="12:22">
+    <row r="22" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L22" t="str">
         <v>Continents</v>
       </c>
@@ -2312,7 +2294,7 @@
         <v>Edgar Air NonAg NH3</v>
       </c>
     </row>
-    <row r="23" spans="12:22">
+    <row r="23" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L23" t="str">
         <v>World</v>
       </c>
@@ -2323,7 +2305,7 @@
         <v>Edgar Air NonAg NOx</v>
       </c>
     </row>
-    <row r="24" spans="12:22">
+    <row r="24" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L24" t="str">
         <v>Ecoregions</v>
       </c>
@@ -2334,7 +2316,7 @@
         <v>Edgar Air NonAg SO2</v>
       </c>
     </row>
-    <row r="25" spans="12:22">
+    <row r="25" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L25" t="str">
         <v>GeosGrid</v>
       </c>
@@ -2345,7 +2327,7 @@
         <v>Edgar Air Gen NH3</v>
       </c>
     </row>
-    <row r="26" spans="12:22">
+    <row r="26" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L26" t="str">
         <v>Pop2010</v>
       </c>
@@ -2356,7 +2338,7 @@
         <v>Edgar Air Gen NOx</v>
       </c>
     </row>
-    <row r="27" spans="12:22">
+    <row r="27" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L27" t="str">
         <v>EmitEdgarAgNH3</v>
       </c>
@@ -2367,7 +2349,7 @@
         <v>Edgar Air Gen SO2</v>
       </c>
     </row>
-    <row r="28" spans="12:22">
+    <row r="28" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L28" t="str">
         <v>EmitEdgarAgNOx</v>
       </c>
@@ -2375,7 +2357,7 @@
         <v>EmitEdgarAgNOx</v>
       </c>
     </row>
-    <row r="29" spans="12:22">
+    <row r="29" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L29" t="str">
         <v>EmitEdgarNonagNH3</v>
       </c>
@@ -2383,7 +2365,7 @@
         <v>EmitEdgarNonagNH3</v>
       </c>
     </row>
-    <row r="30" spans="12:22">
+    <row r="30" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L30" t="str">
         <v>EmitEdgarNonagNOx</v>
       </c>
@@ -2391,7 +2373,7 @@
         <v>EmitEdgarNonagNOx</v>
       </c>
     </row>
-    <row r="31" spans="12:22">
+    <row r="31" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L31" t="str">
         <v>EmitEdgarAgSO2</v>
       </c>
@@ -2399,7 +2381,7 @@
         <v>EmitEdgarAgSO2</v>
       </c>
     </row>
-    <row r="32" spans="12:22">
+    <row r="32" spans="12:22" x14ac:dyDescent="0.25">
       <c r="L32" t="str">
         <v>EmitEdgarNonagSO2</v>
       </c>
@@ -2407,7 +2389,7 @@
         <v>EmitEdgarNonagSO2</v>
       </c>
     </row>
-    <row r="33" spans="12:13">
+    <row r="33" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L33" t="str">
         <v>EmitEdgarGenNH3</v>
       </c>
@@ -2415,7 +2397,7 @@
         <v>EmitEdgarGenNH3</v>
       </c>
     </row>
-    <row r="34" spans="12:13">
+    <row r="34" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L34" t="str">
         <v>EmitEdgarGenNOx</v>
       </c>
@@ -2423,7 +2405,7 @@
         <v>EmitEdgarGenNOx</v>
       </c>
     </row>
-    <row r="35" spans="12:13">
+    <row r="35" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L35" t="str">
         <v>EmitEdgarGenSO2</v>
       </c>
@@ -2431,42 +2413,42 @@
         <v>EmitEdgarGenSO2</v>
       </c>
     </row>
-    <row r="36" spans="12:13">
+    <row r="36" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L36" t="str">
         <v>file_FF_NOx</v>
       </c>
     </row>
-    <row r="37" spans="12:13">
+    <row r="37" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L37" t="str">
         <v>file_FF_NHx</v>
       </c>
     </row>
-    <row r="38" spans="12:13">
+    <row r="38" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L38" t="str">
         <v>file_FF_SOx</v>
       </c>
     </row>
-    <row r="39" spans="12:13">
+    <row r="39" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L39" t="str">
         <v>ecoreg_RFs_NH4_Lebrun</v>
       </c>
     </row>
-    <row r="40" spans="12:13">
+    <row r="40" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L40" t="str">
         <v>ecoreg_RFs_NO3_Lebrun</v>
       </c>
     </row>
-    <row r="41" spans="12:13">
+    <row r="41" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L41" t="str">
         <v>ecoreg_RFs_SO4_Lebrun</v>
       </c>
     </row>
-    <row r="42" spans="12:13">
+    <row r="42" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L42" t="str">
         <v>ecoreg_EFs_Gade</v>
       </c>
     </row>
-    <row r="43" spans="12:13">
+    <row r="43" spans="12:13" x14ac:dyDescent="0.25">
       <c r="L43" t="str">
         <v>ecoreg_GEPs</v>
       </c>
@@ -2481,56 +2463,56 @@
   <dimension ref="B2:O147"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="42.125" customWidth="1"/>
-    <col min="3" max="3" width="26.375" customWidth="1"/>
-    <col min="4" max="4" width="44.625" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
     <col min="5" max="5" width="58" customWidth="1"/>
-    <col min="6" max="6" width="31.375" customWidth="1"/>
-    <col min="7" max="7" width="68.375" customWidth="1"/>
-    <col min="8" max="8" width="18.625" customWidth="1"/>
-    <col min="9" max="9" width="30.625" customWidth="1"/>
-    <col min="10" max="10" width="22.875" customWidth="1"/>
-    <col min="11" max="11" width="32.375" customWidth="1"/>
-    <col min="12" max="12" width="21.375" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="7" max="7" width="68.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="32.42578125" customWidth="1"/>
+    <col min="12" max="12" width="21.42578125" customWidth="1"/>
     <col min="13" max="13" width="28" customWidth="1"/>
-    <col min="14" max="14" width="37.375" customWidth="1"/>
-    <col min="15" max="15" width="11.875" customWidth="1"/>
-    <col min="16" max="16" width="16.875" customWidth="1"/>
-    <col min="17" max="17" width="19.625" customWidth="1"/>
+    <col min="14" max="14" width="37.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.85546875" customWidth="1"/>
+    <col min="16" max="16" width="16.85546875" customWidth="1"/>
+    <col min="17" max="17" width="19.5703125" customWidth="1"/>
     <col min="18" max="22" width="18" customWidth="1"/>
-    <col min="23" max="23" width="14.875" customWidth="1"/>
-    <col min="24" max="24" width="19.375" customWidth="1"/>
-    <col min="25" max="26" width="23.375" customWidth="1"/>
-    <col min="27" max="28" width="20.125" customWidth="1"/>
-    <col min="29" max="29" width="10.375" customWidth="1"/>
-    <col min="31" max="31" width="14.875" customWidth="1"/>
-    <col min="32" max="32" width="18.375" customWidth="1"/>
-    <col min="33" max="33" width="11.875" customWidth="1"/>
-    <col min="34" max="34" width="15.375" customWidth="1"/>
-    <col min="35" max="35" width="23.375" customWidth="1"/>
-    <col min="36" max="36" width="23.875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.375" customWidth="1"/>
+    <col min="23" max="23" width="14.85546875" customWidth="1"/>
+    <col min="24" max="24" width="19.42578125" customWidth="1"/>
+    <col min="25" max="26" width="23.42578125" customWidth="1"/>
+    <col min="27" max="28" width="20.140625" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" customWidth="1"/>
+    <col min="31" max="31" width="14.85546875" customWidth="1"/>
+    <col min="32" max="32" width="18.42578125" customWidth="1"/>
+    <col min="33" max="33" width="11.85546875" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" customWidth="1"/>
+    <col min="35" max="35" width="23.42578125" customWidth="1"/>
+    <col min="36" max="36" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E2" t="s">
         <v>93</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:14">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2571,7 +2553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:14">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -2580,11 +2562,11 @@
       </c>
       <c r="E6" t="str" cm="1">
         <f t="array" ref="E6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F6" t="str" cm="1">
         <f t="array" ref="F6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G6" t="str" cm="1">
         <f t="array" ref="G6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2610,10 +2592,10 @@
       </c>
       <c r="M6" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>266</v>
       </c>
@@ -2652,9 +2634,9 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="8" spans="2:14">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
@@ -2675,19 +2657,19 @@
         <v>252</v>
       </c>
       <c r="I8" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="J8" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="M8" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -2708,17 +2690,17 @@
         <v>252</v>
       </c>
       <c r="I9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="J9" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="M9" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>270</v>
       </c>
@@ -2735,7 +2717,7 @@
       </c>
       <c r="G10" t="str" cm="1">
         <f t="array" ref="G10">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>repair1_holes10</v>
+        <v>archUrb2v02_repair1_holes10</v>
       </c>
       <c r="H10" t="s">
         <v>252</v>
@@ -2744,16 +2726,16 @@
         <v>270</v>
       </c>
       <c r="J10" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="M10" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
@@ -2774,17 +2756,17 @@
         <v>252</v>
       </c>
       <c r="I11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J11" t="s">
-        <v>246</v>
+        <v>279</v>
       </c>
       <c r="M11" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="12" spans="2:14">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>268</v>
       </c>
@@ -2817,7 +2799,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="13" spans="2:14">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>263</v>
       </c>
@@ -2850,7 +2832,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>254</v>
       </c>
@@ -2885,7 +2867,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>255</v>
       </c>
@@ -2920,7 +2902,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="16" spans="2:14">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>256</v>
       </c>
@@ -2956,7 +2938,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="17" spans="2:13">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>257</v>
       </c>
@@ -2992,7 +2974,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="18" spans="2:13">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>250</v>
       </c>
@@ -3005,7 +2987,7 @@
       </c>
       <c r="F18" t="str" cm="1">
         <f t="array" ref="F18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>anthro_compiled_v01</v>
       </c>
       <c r="G18" t="str" cm="1">
         <f t="array" ref="G18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3025,10 +3007,10 @@
       </c>
       <c r="M18" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13">
+        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\anthro_compiled_v01</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>251</v>
       </c>
@@ -3064,7 +3046,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
       </c>
     </row>
-    <row r="20" spans="2:13">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>29</v>
       </c>
@@ -3073,11 +3055,11 @@
       </c>
       <c r="E20" t="str" cm="1">
         <f t="array" ref="E20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F20" t="str" cm="1">
         <f t="array" ref="F20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G20" t="str" cm="1">
         <f t="array" ref="G20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3100,10 +3082,10 @@
       </c>
       <c r="M20" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>30</v>
       </c>
@@ -3112,11 +3094,11 @@
       </c>
       <c r="E21" t="str" cm="1">
         <f t="array" ref="E21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F21" t="str" cm="1">
         <f t="array" ref="F21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G21" t="str" cm="1">
         <f t="array" ref="G21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3142,10 +3124,10 @@
       </c>
       <c r="M21" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -3154,7 +3136,7 @@
       </c>
       <c r="E22" t="str" cm="1">
         <f t="array" ref="E22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>W:\data\geo\ecoregions_teow\Olson_2012\official</v>
       </c>
       <c r="F22" t="str" cm="1">
         <f t="array" ref="F22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3181,10 +3163,10 @@
       </c>
       <c r="M22" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13">
+        <v>W:\data\geo\ecoregions_teow\Olson_2012\official\</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>31</v>
       </c>
@@ -3193,11 +3175,11 @@
       </c>
       <c r="E23" t="str" cm="1">
         <f t="array" ref="E23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F23" t="str" cm="1">
         <f t="array" ref="F23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G23" t="str" cm="1">
         <f t="array" ref="G23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3217,10 +3199,10 @@
       </c>
       <c r="M23" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>32</v>
       </c>
@@ -3229,11 +3211,11 @@
       </c>
       <c r="E24" t="str" cm="1">
         <f t="array" ref="E24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F24" t="str" cm="1">
         <f t="array" ref="F24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G24" t="str" cm="1">
         <f t="array" ref="G24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3253,10 +3235,10 @@
       </c>
       <c r="M24" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>33</v>
       </c>
@@ -3265,11 +3247,11 @@
       </c>
       <c r="E25" t="str" cm="1">
         <f t="array" ref="E25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F25" t="str" cm="1">
         <f t="array" ref="F25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G25" t="str" cm="1">
         <f t="array" ref="G25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3289,10 +3271,10 @@
       </c>
       <c r="M25" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>34</v>
       </c>
@@ -3301,11 +3283,11 @@
       </c>
       <c r="E26" t="str" cm="1">
         <f t="array" ref="E26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F26" t="str" cm="1">
         <f t="array" ref="F26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G26" t="str" cm="1">
         <f t="array" ref="G26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3325,10 +3307,10 @@
       </c>
       <c r="M26" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>35</v>
       </c>
@@ -3337,11 +3319,11 @@
       </c>
       <c r="E27" t="str" cm="1">
         <f t="array" ref="E27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F27" t="str" cm="1">
         <f t="array" ref="F27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G27" t="str" cm="1">
         <f t="array" ref="G27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3361,10 +3343,10 @@
       </c>
       <c r="M27" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>36</v>
       </c>
@@ -3373,11 +3355,11 @@
       </c>
       <c r="E28" t="str" cm="1">
         <f t="array" ref="E28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
       </c>
       <c r="F28" t="str" cm="1">
         <f t="array" ref="F28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G28" t="str" cm="1">
         <f t="array" ref="G28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3397,10 +3379,10 @@
       </c>
       <c r="M28" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>37</v>
       </c>
@@ -3409,11 +3391,11 @@
       </c>
       <c r="E29" t="str" cm="1">
         <f t="array" ref="E29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input</v>
       </c>
       <c r="F29" t="str" cm="1">
         <f t="array" ref="F29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G29" t="str" cm="1">
         <f t="array" ref="G29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3433,10 +3415,10 @@
       </c>
       <c r="M29" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>38</v>
       </c>
@@ -3445,11 +3427,11 @@
       </c>
       <c r="E30" t="str" cm="1">
         <f t="array" ref="E30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input</v>
       </c>
       <c r="F30" t="str" cm="1">
         <f t="array" ref="F30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v/>
+        <v>Shapefiles</v>
       </c>
       <c r="G30" t="str" cm="1">
         <f t="array" ref="G30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3469,10 +3451,10 @@
       </c>
       <c r="M30" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13">
+        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input\Shapefiles</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>226</v>
       </c>
@@ -3481,7 +3463,7 @@
       </c>
       <c r="E31" t="str" cm="1">
         <f t="array" ref="E31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
       </c>
       <c r="F31" t="str" cm="1">
         <f t="array" ref="F31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3503,10 +3485,10 @@
       </c>
       <c r="M31" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13">
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>227</v>
       </c>
@@ -3515,7 +3497,7 @@
       </c>
       <c r="E32" t="str" cm="1">
         <f t="array" ref="E32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
       </c>
       <c r="F32" t="str" cm="1">
         <f t="array" ref="F32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3537,10 +3519,10 @@
       </c>
       <c r="M32" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15">
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>228</v>
       </c>
@@ -3549,7 +3531,7 @@
       </c>
       <c r="E33" t="str" cm="1">
         <f t="array" ref="E33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
       </c>
       <c r="F33" t="str" cm="1">
         <f t="array" ref="F33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3571,10 +3553,10 @@
       </c>
       <c r="M33" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15">
+        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>191</v>
       </c>
@@ -3583,7 +3565,7 @@
       </c>
       <c r="E34" t="str" cm="1">
         <f t="array" ref="E34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
       </c>
       <c r="F34" t="str" cm="1">
         <f t="array" ref="F34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3604,10 +3586,10 @@
       </c>
       <c r="M34" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15">
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>192</v>
       </c>
@@ -3616,7 +3598,7 @@
       </c>
       <c r="E35" t="str" cm="1">
         <f t="array" ref="E35">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
       </c>
       <c r="F35" t="str" cm="1">
         <f t="array" ref="F35">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3637,10 +3619,10 @@
       </c>
       <c r="M35" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15">
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>193</v>
       </c>
@@ -3649,7 +3631,7 @@
       </c>
       <c r="E36" t="str" cm="1">
         <f t="array" ref="E36">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
       </c>
       <c r="F36" t="str" cm="1">
         <f t="array" ref="F36">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3670,10 +3652,10 @@
       </c>
       <c r="M36" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="37" spans="2:15">
+        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>141</v>
       </c>
@@ -3682,7 +3664,7 @@
       </c>
       <c r="E37" t="str" cm="1">
         <f t="array" ref="E37">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
       </c>
       <c r="F37" t="str" cm="1">
         <f t="array" ref="F37">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3703,10 +3685,10 @@
       </c>
       <c r="M37" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="38" spans="2:15">
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>143</v>
       </c>
@@ -3715,7 +3697,7 @@
       </c>
       <c r="E38" t="str" cm="1">
         <f t="array" ref="E38">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
       </c>
       <c r="F38" t="str" cm="1">
         <f t="array" ref="F38">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3736,10 +3718,10 @@
       </c>
       <c r="M38" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="39" spans="2:15">
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>142</v>
       </c>
@@ -3748,7 +3730,7 @@
       </c>
       <c r="E39" t="str" cm="1">
         <f t="array" ref="E39">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
       </c>
       <c r="F39" t="str" cm="1">
         <f t="array" ref="F39">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3769,10 +3751,10 @@
       </c>
       <c r="M39" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="40" spans="2:15">
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>57</v>
       </c>
@@ -3781,7 +3763,7 @@
       </c>
       <c r="E40" t="str" cm="1">
         <f t="array" ref="E40">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
       </c>
       <c r="F40" t="str" cm="1">
         <f t="array" ref="F40">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3802,10 +3784,10 @@
       </c>
       <c r="M40" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="41" spans="2:15">
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>50</v>
       </c>
@@ -3814,7 +3796,7 @@
       </c>
       <c r="E41" t="str" cm="1">
         <f t="array" ref="E41">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
       </c>
       <c r="F41" t="str" cm="1">
         <f t="array" ref="F41">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3835,15 +3817,15 @@
       </c>
       <c r="M41" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="47" spans="2:15">
+        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="2:15">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B48" s="3" t="s">
         <v>42</v>
       </c>
@@ -3887,7 +3869,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="2:14">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>46</v>
       </c>
@@ -3911,7 +3893,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="2:14">
+    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>47</v>
       </c>
@@ -3935,7 +3917,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="2:14">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>48</v>
       </c>
@@ -3959,7 +3941,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="2:14">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>49</v>
       </c>
@@ -3986,7 +3968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:14">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>50</v>
       </c>
@@ -4013,7 +3995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:14">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>151</v>
       </c>
@@ -4040,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:14">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>152</v>
       </c>
@@ -4067,7 +4049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:14">
+    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>153</v>
       </c>
@@ -4094,7 +4076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:14">
+    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>250</v>
       </c>
@@ -4121,7 +4103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:14">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>251</v>
       </c>
@@ -4148,7 +4130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:14">
+    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>32</v>
       </c>
@@ -4175,7 +4157,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:14">
+    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>51</v>
       </c>
@@ -4202,7 +4184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:14">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
         <v>52</v>
       </c>
@@ -4229,7 +4211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:14">
+    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
         <v>53</v>
       </c>
@@ -4256,7 +4238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:14">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
         <v>54</v>
       </c>
@@ -4283,7 +4265,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:14">
+    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>55</v>
       </c>
@@ -4310,7 +4292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:12">
+    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>56</v>
       </c>
@@ -4337,7 +4319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:12">
+    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
         <v>223</v>
       </c>
@@ -4364,7 +4346,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:12">
+    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
         <v>225</v>
       </c>
@@ -4391,7 +4373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:12">
+    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>224</v>
       </c>
@@ -4418,12 +4400,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:12">
+    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="2:12">
+    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>71</v>
       </c>
@@ -4443,7 +4425,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="2:12">
+    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>28</v>
       </c>
@@ -4463,7 +4445,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="2:12">
+    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>266</v>
       </c>
@@ -4480,9 +4462,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="2:12">
+    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C78" t="s">
         <v>94</v>
@@ -4491,13 +4473,13 @@
         <v>264</v>
       </c>
       <c r="F78" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G78" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="79" spans="2:12">
+    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>270</v>
       </c>
@@ -4508,15 +4490,15 @@
         <v>264</v>
       </c>
       <c r="F79" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="G79" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="80" spans="2:12">
+    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C80" t="s">
         <v>94</v>
@@ -4525,15 +4507,15 @@
         <v>264</v>
       </c>
       <c r="F80" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G80" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="81" spans="2:7">
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C81" t="s">
         <v>94</v>
@@ -4542,13 +4524,13 @@
         <v>264</v>
       </c>
       <c r="F81" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G81" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="82" spans="2:7">
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>268</v>
       </c>
@@ -4565,7 +4547,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="83" spans="2:7">
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>263</v>
       </c>
@@ -4582,7 +4564,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="84" spans="2:7">
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>254</v>
       </c>
@@ -4599,7 +4581,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="85" spans="2:7">
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>255</v>
       </c>
@@ -4616,7 +4598,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="86" spans="2:7">
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>256</v>
       </c>
@@ -4633,7 +4615,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="87" spans="2:7">
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>257</v>
       </c>
@@ -4650,7 +4632,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="88" spans="2:7">
+    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>250</v>
       </c>
@@ -4670,7 +4652,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="89" spans="2:7">
+    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>251</v>
       </c>
@@ -4687,7 +4669,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="90" spans="2:7">
+    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>29</v>
       </c>
@@ -4707,7 +4689,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="2:7">
+    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>30</v>
       </c>
@@ -4727,7 +4709,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="2:7">
+    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>39</v>
       </c>
@@ -4744,7 +4726,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="93" spans="2:7">
+    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>31</v>
       </c>
@@ -4764,7 +4746,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="94" spans="2:7">
+    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>32</v>
       </c>
@@ -4784,7 +4766,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="95" spans="2:7">
+    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
         <v>33</v>
       </c>
@@ -4804,7 +4786,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="2:7">
+    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
         <v>34</v>
       </c>
@@ -4824,7 +4806,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="97" spans="2:7">
+    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
         <v>35</v>
       </c>
@@ -4844,7 +4826,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="2:7">
+    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
         <v>36</v>
       </c>
@@ -4864,7 +4846,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="2:7">
+    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
         <v>37</v>
       </c>
@@ -4884,7 +4866,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="2:7">
+    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
         <v>38</v>
       </c>
@@ -4904,7 +4886,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="101" spans="2:7">
+    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
         <v>226</v>
       </c>
@@ -4921,7 +4903,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="2:7">
+    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B102" t="s">
         <v>227</v>
       </c>
@@ -4938,7 +4920,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="103" spans="2:7">
+    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B103" t="s">
         <v>228</v>
       </c>
@@ -4955,7 +4937,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="104" spans="2:7">
+    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
         <v>191</v>
       </c>
@@ -4972,7 +4954,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="2:7">
+    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>192</v>
       </c>
@@ -4989,7 +4971,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="2:7">
+    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
         <v>193</v>
       </c>
@@ -5006,7 +4988,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="107" spans="2:7">
+    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B107" t="s">
         <v>141</v>
       </c>
@@ -5023,7 +5005,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="108" spans="2:7">
+    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
         <v>143</v>
       </c>
@@ -5040,7 +5022,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="109" spans="2:7">
+    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
         <v>142</v>
       </c>
@@ -5057,7 +5039,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="110" spans="2:7">
+    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B110" t="s">
         <v>57</v>
       </c>
@@ -5074,7 +5056,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="111" spans="2:7">
+    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B111" t="s">
         <v>50</v>
       </c>
@@ -5091,7 +5073,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="112" spans="2:7">
+    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B112" s="13" t="s">
         <v>28</v>
       </c>
@@ -5109,7 +5091,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="113" spans="2:7">
+    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B113" s="13" t="s">
         <v>266</v>
       </c>
@@ -5127,9 +5109,9 @@
         <v>252</v>
       </c>
     </row>
-    <row r="114" spans="2:7">
+    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B114" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C114" s="13" t="s">
         <v>220</v>
@@ -5139,13 +5121,13 @@
       </c>
       <c r="E114" s="13"/>
       <c r="F114" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G114" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="115" spans="2:7">
+    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B115" s="13" t="s">
         <v>270</v>
       </c>
@@ -5157,15 +5139,15 @@
       </c>
       <c r="E115" s="13"/>
       <c r="F115" s="13" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="G115" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="2:7">
+    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B116" s="13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C116" s="13" t="s">
         <v>220</v>
@@ -5175,15 +5157,15 @@
       </c>
       <c r="E116" s="13"/>
       <c r="F116" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G116" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="117" spans="2:7">
+    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B117" s="13" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C117" s="13" t="s">
         <v>220</v>
@@ -5193,13 +5175,13 @@
       </c>
       <c r="E117" s="13"/>
       <c r="F117" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G117" s="13" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="118" spans="2:7">
+    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B118" s="13" t="s">
         <v>268</v>
       </c>
@@ -5217,7 +5199,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="119" spans="2:7">
+    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B119" s="13" t="s">
         <v>263</v>
       </c>
@@ -5235,7 +5217,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="120" spans="2:7">
+    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B120" s="13" t="s">
         <v>254</v>
       </c>
@@ -5253,7 +5235,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="121" spans="2:7">
+    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B121" s="13" t="s">
         <v>255</v>
       </c>
@@ -5271,7 +5253,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="122" spans="2:7">
+    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B122" s="13" t="s">
         <v>256</v>
       </c>
@@ -5289,7 +5271,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="123" spans="2:7">
+    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B123" s="13" t="s">
         <v>257</v>
       </c>
@@ -5307,7 +5289,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="124" spans="2:7">
+    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B124" s="13" t="s">
         <v>250</v>
       </c>
@@ -5325,7 +5307,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="2:7">
+    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B125" s="13" t="s">
         <v>251</v>
       </c>
@@ -5343,7 +5325,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="126" spans="2:7">
+    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B126" s="13" t="s">
         <v>29</v>
       </c>
@@ -5361,7 +5343,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="127" spans="2:7">
+    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B127" s="13" t="s">
         <v>30</v>
       </c>
@@ -5379,7 +5361,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="128" spans="2:7">
+    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B128" s="13" t="s">
         <v>39</v>
       </c>
@@ -5397,7 +5379,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="129" spans="2:7">
+    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B129" s="13" t="s">
         <v>31</v>
       </c>
@@ -5415,7 +5397,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="130" spans="2:7">
+    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B130" s="13" t="s">
         <v>32</v>
       </c>
@@ -5433,7 +5415,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="131" spans="2:7">
+    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B131" s="13" t="s">
         <v>33</v>
       </c>
@@ -5451,7 +5433,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="132" spans="2:7">
+    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B132" s="13" t="s">
         <v>34</v>
       </c>
@@ -5469,7 +5451,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="133" spans="2:7">
+    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B133" s="13" t="s">
         <v>35</v>
       </c>
@@ -5487,7 +5469,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="134" spans="2:7">
+    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B134" s="13" t="s">
         <v>36</v>
       </c>
@@ -5505,7 +5487,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="135" spans="2:7">
+    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B135" s="13" t="s">
         <v>37</v>
       </c>
@@ -5523,7 +5505,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="136" spans="2:7">
+    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B136" s="13" t="s">
         <v>38</v>
       </c>
@@ -5541,7 +5523,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="137" spans="2:7">
+    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B137" s="13" t="s">
         <v>226</v>
       </c>
@@ -5559,7 +5541,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="138" spans="2:7">
+    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B138" s="13" t="s">
         <v>227</v>
       </c>
@@ -5577,7 +5559,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="139" spans="2:7">
+    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B139" s="13" t="s">
         <v>228</v>
       </c>
@@ -5595,7 +5577,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="140" spans="2:7">
+    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B140" s="13" t="s">
         <v>191</v>
       </c>
@@ -5613,7 +5595,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="141" spans="2:7">
+    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B141" s="13" t="s">
         <v>192</v>
       </c>
@@ -5631,7 +5613,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="142" spans="2:7">
+    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B142" s="13" t="s">
         <v>193</v>
       </c>
@@ -5649,7 +5631,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="143" spans="2:7">
+    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B143" s="13" t="s">
         <v>141</v>
       </c>
@@ -5667,7 +5649,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="144" spans="2:7">
+    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B144" s="13" t="s">
         <v>143</v>
       </c>
@@ -5685,7 +5667,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="145" spans="2:7">
+    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B145" s="13" t="s">
         <v>142</v>
       </c>
@@ -5703,7 +5685,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="146" spans="2:7">
+    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B146" s="13" t="s">
         <v>57</v>
       </c>
@@ -5721,7 +5703,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147" spans="2:7">
+    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B147" s="13" t="s">
         <v>50</v>
       </c>
@@ -5783,24 +5765,24 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="2:9">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>102</v>
       </c>
@@ -5826,7 +5808,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="2:9">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>107</v>
       </c>
@@ -5847,7 +5829,7 @@
         <v>10102-43-9</v>
       </c>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>202</v>
       </c>
@@ -5868,7 +5850,7 @@
         <v>10102-43-9</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>204</v>
       </c>
@@ -5889,7 +5871,7 @@
         <v>10102-44-0</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>108</v>
       </c>
@@ -5908,7 +5890,7 @@
         <v>000-00-0</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>128</v>
       </c>
@@ -5929,7 +5911,7 @@
         <v>7664-41-7</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>129</v>
       </c>
@@ -5950,7 +5932,7 @@
         <v>14798-03-9</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>109</v>
       </c>
@@ -5969,7 +5951,7 @@
         <v>000-00-0</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>132</v>
       </c>
@@ -5990,7 +5972,7 @@
         <v>7446-09-5</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>135</v>
       </c>
@@ -6029,43 +6011,43 @@
   <dimension ref="B4:N14"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="7" max="7" width="73.125" customWidth="1"/>
-    <col min="9" max="9" width="17.375" customWidth="1"/>
+    <col min="7" max="7" width="73.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" customWidth="1"/>
     <col min="10" max="10" width="28" customWidth="1"/>
-    <col min="11" max="11" width="16.375" customWidth="1"/>
-    <col min="12" max="12" width="16.75" customWidth="1"/>
-    <col min="13" max="13" width="15.375" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.42578125" customWidth="1"/>
     <col min="14" max="14" width="45" customWidth="1"/>
-    <col min="16" max="16" width="15.25" customWidth="1"/>
+    <col min="16" max="16" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>137</v>
       </c>
       <c r="C4" t="str" cm="1">
         <f t="array" ref="C4">_xlfn.TEXTJOIN(", ",TRUE, "'"&amp;B11:B14&amp;"'")</f>
-        <v>'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010'</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14">
+        <v>'STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010'</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B7" t="b">
         <f>ROWS(_xlfn.UNIQUE(Tbl.SpatialTransforms[STM unique name]))=ROWS(Tbl.SpatialTransforms[STM unique name])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:14">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>58</v>
       </c>
@@ -6073,7 +6055,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="2:14">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>59</v>
       </c>
@@ -6114,17 +6096,17 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="2:14">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="G11" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
       </c>
       <c r="H11" t="s">
         <v>194</v>
@@ -6133,7 +6115,7 @@
         <v>117</v>
       </c>
       <c r="J11" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="K11" t="s">
         <v>28</v>
@@ -6146,20 +6128,20 @@
       </c>
       <c r="N11" t="str">
         <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
-      </c>
-    </row>
-    <row r="12" spans="2:14">
+        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="G12" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
       </c>
       <c r="H12" t="s">
         <v>194</v>
@@ -6168,7 +6150,7 @@
         <v>117</v>
       </c>
       <c r="J12" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="K12" t="s">
         <v>28</v>
@@ -6181,10 +6163,10 @@
       </c>
       <c r="N12" t="str">
         <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
-        <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
-      </c>
-    </row>
-    <row r="13" spans="2:14">
+        <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010</v>
@@ -6203,7 +6185,7 @@
         <v>117</v>
       </c>
       <c r="J13" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="K13" t="s">
         <v>28</v>
@@ -6214,12 +6196,12 @@
       <c r="M13" t="b">
         <v>1</v>
       </c>
-      <c r="N13" s="14" t="str">
+      <c r="N13" t="str">
         <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
         <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010</v>
       </c>
     </row>
-    <row r="14" spans="2:14">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010</v>
@@ -6238,7 +6220,7 @@
         <v>117</v>
       </c>
       <c r="J14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="K14" t="s">
         <v>28</v>
@@ -6249,7 +6231,7 @@
       <c r="M14" t="b">
         <v>1</v>
       </c>
-      <c r="N14" s="14" t="str">
+      <c r="N14" t="str">
         <f>"STM"&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),2,3)&amp;"_"&amp;Tbl.SpatialTransforms[[#This Row],[STM type]]&amp;"_Orig-"&amp;Tbl.SpatialTransforms[[#This Row],[Orig Geofile]]&amp;"_New-"&amp;Tbl.SpatialTransforms[[#This Row],[New Geofile]]&amp;IF(ISBLANK(Tbl.SpatialTransforms[[#This Row],[Weight Data]]),"","_"&amp;Tbl.SpatialTransforms[[#This Row],[Weight Data]])</f>
         <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010</v>
       </c>
@@ -6286,47 +6268,47 @@
       <selection activeCell="AE24" sqref="AE24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.375" customWidth="1"/>
-    <col min="3" max="3" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="4" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.375" customWidth="1"/>
-    <col min="8" max="8" width="22.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.375" customWidth="1"/>
-    <col min="10" max="10" width="13.625" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="29.125" customWidth="1"/>
-    <col min="13" max="13" width="22.125" customWidth="1"/>
-    <col min="14" max="15" width="17.625" customWidth="1"/>
-    <col min="16" max="16" width="34.625" customWidth="1"/>
-    <col min="17" max="17" width="16.375" customWidth="1"/>
-    <col min="18" max="18" width="15.375" customWidth="1"/>
-    <col min="19" max="19" width="14.375" customWidth="1"/>
+    <col min="12" max="12" width="29.140625" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" customWidth="1"/>
+    <col min="14" max="15" width="17.5703125" customWidth="1"/>
+    <col min="16" max="16" width="34.5703125" customWidth="1"/>
+    <col min="17" max="17" width="16.42578125" customWidth="1"/>
+    <col min="18" max="18" width="15.42578125" customWidth="1"/>
+    <col min="19" max="19" width="14.42578125" customWidth="1"/>
     <col min="20" max="20" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:24">
+    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X3" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="2:24">
+    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="2:24">
+    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="2:24">
+    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
       <c r="X6" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:24">
+    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>211</v>
       </c>
@@ -6340,7 +6322,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="2:24" ht="42.75">
+    <row r="8" spans="2:24" ht="45" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>206</v>
       </c>
@@ -6408,7 +6390,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="2:24">
+    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>208</v>
       </c>
@@ -6473,7 +6455,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="2:24">
+    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>207</v>
       </c>
@@ -6538,7 +6520,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="2:24">
+    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F11">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6594,7 +6576,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="2:24">
+    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F12">
         <f t="shared" ref="F12:F25" si="1">IFERROR($F11+1,1)</f>
         <v>4</v>
@@ -6650,7 +6632,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="2:24">
+    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F13">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -6706,7 +6688,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="2:24">
+    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -6762,7 +6744,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="2:24">
+    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -6818,7 +6800,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="2:24">
+    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
       <c r="F16">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -6874,7 +6856,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="6:24">
+    <row r="17" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F17">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -6930,7 +6912,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="6:24">
+    <row r="18" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F18">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -6988,7 +6970,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="6:24">
+    <row r="19" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F19">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -7046,7 +7028,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="6:24">
+    <row r="20" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F20">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -7104,7 +7086,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="6:24">
+    <row r="21" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F21">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -7156,7 +7138,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="6:24">
+    <row r="22" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F22">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -7208,7 +7190,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="6:24">
+    <row r="23" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F23">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -7260,7 +7242,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="6:24">
+    <row r="24" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F24">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -7312,7 +7294,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="6:24">
+    <row r="25" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F25">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -7364,7 +7346,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="6:24">
+    <row r="26" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F26">
         <f t="shared" ref="F26:F53" si="2">IFERROR($F25+1,1)</f>
         <v>18</v>
@@ -7416,7 +7398,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="6:24">
+    <row r="27" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F27">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -7474,7 +7456,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="6:24">
+    <row r="28" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F28">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -7532,7 +7514,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="6:24">
+    <row r="29" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F29">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -7590,7 +7572,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="6:24">
+    <row r="30" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F30">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -7642,7 +7624,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="6:24">
+    <row r="31" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F31">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -7694,7 +7676,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="6:24">
+    <row r="32" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F32">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -7746,7 +7728,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="6:24">
+    <row r="33" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F33">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -7798,7 +7780,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="6:24">
+    <row r="34" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F34">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -7850,7 +7832,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="6:24">
+    <row r="35" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F35">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -7902,7 +7884,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="6:24">
+    <row r="36" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F36">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -7960,7 +7942,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="6:24">
+    <row r="37" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F37">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -8018,7 +8000,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="6:24">
+    <row r="38" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F38">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -8076,7 +8058,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="6:24">
+    <row r="39" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F39">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -8128,7 +8110,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="6:24">
+    <row r="40" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F40">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -8180,7 +8162,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="6:24">
+    <row r="41" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F41">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -8232,7 +8214,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="6:24">
+    <row r="42" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F42">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -8284,7 +8266,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="6:24">
+    <row r="43" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F43">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -8336,7 +8318,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="6:24">
+    <row r="44" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F44">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -8388,7 +8370,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="6:24">
+    <row r="45" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F45">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -8446,7 +8428,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="6:24">
+    <row r="46" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F46">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -8504,7 +8486,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="6:24">
+    <row r="47" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F47">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -8562,7 +8544,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="6:24">
+    <row r="48" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F48">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -8614,7 +8596,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="6:24">
+    <row r="49" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F49">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -8666,7 +8648,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="6:24">
+    <row r="50" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F50">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -8718,7 +8700,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="6:24">
+    <row r="51" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F51">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -8770,7 +8752,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="52" spans="6:24">
+    <row r="52" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F52">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -8822,7 +8804,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="6:24">
+    <row r="53" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F53">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -8874,7 +8856,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="54" spans="6:24">
+    <row r="54" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F54">
         <f t="shared" ref="F54:F71" si="3">IFERROR($F53+1,1)</f>
         <v>46</v>
@@ -8932,7 +8914,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="6:24">
+    <row r="55" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F55">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -8990,7 +8972,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="6:24">
+    <row r="56" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F56">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -9048,7 +9030,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="6:24">
+    <row r="57" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F57">
         <f t="shared" si="3"/>
         <v>49</v>
@@ -9100,7 +9082,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="6:24">
+    <row r="58" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F58">
         <f t="shared" si="3"/>
         <v>50</v>
@@ -9152,7 +9134,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="6:24">
+    <row r="59" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F59">
         <f t="shared" si="3"/>
         <v>51</v>
@@ -9204,7 +9186,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="6:24">
+    <row r="60" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F60">
         <f t="shared" si="3"/>
         <v>52</v>
@@ -9256,7 +9238,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="6:24">
+    <row r="61" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F61">
         <f t="shared" si="3"/>
         <v>53</v>
@@ -9308,7 +9290,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="6:24">
+    <row r="62" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F62">
         <f t="shared" si="3"/>
         <v>54</v>
@@ -9360,7 +9342,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="6:24">
+    <row r="63" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F63">
         <f t="shared" si="3"/>
         <v>55</v>
@@ -9418,7 +9400,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="6:24">
+    <row r="64" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F64">
         <f t="shared" si="3"/>
         <v>56</v>
@@ -9476,7 +9458,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="6:24">
+    <row r="65" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F65">
         <f t="shared" si="3"/>
         <v>57</v>
@@ -9534,7 +9516,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="66" spans="6:24">
+    <row r="66" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F66">
         <f t="shared" si="3"/>
         <v>58</v>
@@ -9586,7 +9568,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="6:24">
+    <row r="67" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F67">
         <f t="shared" si="3"/>
         <v>59</v>
@@ -9638,7 +9620,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="6:24">
+    <row r="68" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F68">
         <f t="shared" si="3"/>
         <v>60</v>
@@ -9690,7 +9672,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="6:24">
+    <row r="69" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F69">
         <f t="shared" si="3"/>
         <v>61</v>
@@ -9742,7 +9724,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="6:24">
+    <row r="70" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F70">
         <f t="shared" si="3"/>
         <v>62</v>
@@ -9794,7 +9776,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="71" spans="6:24">
+    <row r="71" spans="6:24" x14ac:dyDescent="0.25">
       <c r="F71">
         <f t="shared" si="3"/>
         <v>63</v>

</xml_diff>

<commit_message>
fix capitalization in gpkg fields: archID_num -> ArchID_num Also excel crashed, so updated calc file to v0b.
</commit_message>
<xml_diff>
--- a/calc/ozone STM calc setup v00a.xlsx
+++ b/calc/ozone STM calc setup v00a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CalcDir\TRACI_ozone_stm\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD12E993-2967-476B-9F9F-EC487D59525C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565D6DF3-2A62-4C67-BA45-252592D6FB85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{BD39A979-CEB5-421F-A893-2A15417D7C3E}"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="2" r:id="rId1"/>
@@ -75,19 +75,37 @@
   <commentList>
     <comment ref="I5" authorId="0" shapeId="0" xr:uid="{C3F9C59B-D4CD-4335-8367-A9C7977F41DA}">
       <text>
-        <t xml:space="preserve">[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This could be done in python, but it is calculated here.  Needed because the function fix_data_ids uses the path/file/extension to get the associated geofile.
 </t>
+        </r>
       </text>
     </comment>
     <comment ref="F48" authorId="1" shapeId="0" xr:uid="{C05BA83B-E4CC-4E37-B576-FA3EC5396FF7}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Aptos Narrow"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     This is redundant for the GIS files.  However, it's necessary in case the others come from an excel file (e.g.) with a different ID name than what is used in the associated geofile.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -981,7 +999,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#000\-00\-0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1304,7 +1322,7 @@
 </file>
 
 <file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
-<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2">
   <global>
     <keyFlags>
       <key name="_Self">
@@ -1855,29 +1873,29 @@
       <selection activeCell="AC25" sqref="AC25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="23.42578125" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" customWidth="1"/>
-    <col min="12" max="13" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="29.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="19.625" customWidth="1"/>
+    <col min="4" max="4" width="23.375" customWidth="1"/>
+    <col min="5" max="5" width="24.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.625" customWidth="1"/>
+    <col min="7" max="7" width="23.375" customWidth="1"/>
+    <col min="8" max="8" width="20.625" customWidth="1"/>
+    <col min="9" max="9" width="15.375" customWidth="1"/>
+    <col min="10" max="10" width="20.625" customWidth="1"/>
+    <col min="12" max="13" width="30.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="29.875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="43.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="2:22" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" ht="30">
       <c r="C7" s="1" t="s">
         <v>15</v>
       </c>
@@ -1929,7 +1947,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22">
       <c r="B8" t="s">
         <v>61</v>
       </c>
@@ -1999,7 +2017,7 @@
         <v>AnthroVOCs_v01_gpkg</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22">
       <c r="C9" t="s">
         <v>100</v>
       </c>
@@ -2049,7 +2067,7 @@
         <v>AnthroVOCs_v01_tif</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22">
       <c r="B10" t="s">
         <v>159</v>
       </c>
@@ -2090,7 +2108,7 @@
         <v>Pop2010</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22">
       <c r="B11" t="s">
         <v>115</v>
       </c>
@@ -2122,7 +2140,7 @@
         <v>Edgar Air Ag NH3</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22">
       <c r="E12" t="s">
         <v>21</v>
       </c>
@@ -2142,7 +2160,7 @@
         <v>Edgar Air Ag NOx</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22">
       <c r="E13" t="s">
         <v>45</v>
       </c>
@@ -2162,7 +2180,7 @@
         <v>Edgar Air Ag SO2</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22">
       <c r="D14" t="s">
         <v>172</v>
       </c>
@@ -2185,7 +2203,7 @@
         <v>Edgar Air NonAg NH3</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:22">
       <c r="L15" t="str">
         <v>Arch_test</v>
       </c>
@@ -2202,7 +2220,7 @@
         <v>Edgar Air NonAg NOx</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22">
       <c r="L16" t="str">
         <v>Arch_Full_Urb2_v01</v>
       </c>
@@ -2219,7 +2237,7 @@
         <v>Edgar Air NonAg SO2</v>
       </c>
     </row>
-    <row r="17" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="12:22">
       <c r="L17" t="str">
         <v>Arch_Full_Urb3_v01</v>
       </c>
@@ -2233,7 +2251,7 @@
         <v>Edgar Air Gen NH3</v>
       </c>
     </row>
-    <row r="18" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="12:22">
       <c r="L18" t="str">
         <v>Arch_Full_Urb2_v02</v>
       </c>
@@ -2247,7 +2265,7 @@
         <v>Edgar Air Gen NOx</v>
       </c>
     </row>
-    <row r="19" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="12:22">
       <c r="L19" t="str">
         <v>Arch_Full_Urb3_v02</v>
       </c>
@@ -2261,7 +2279,7 @@
         <v>Edgar Air Gen SO2</v>
       </c>
     </row>
-    <row r="20" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="12:22">
       <c r="L20" t="str">
         <v>AnthroVOCs_v01_gpkg</v>
       </c>
@@ -2272,7 +2290,7 @@
         <v>Edgar Air Ag NOx</v>
       </c>
     </row>
-    <row r="21" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="12:22">
       <c r="L21" t="str">
         <v>AnthroVOCs_v01_tif</v>
       </c>
@@ -2283,7 +2301,7 @@
         <v>Edgar Air Ag SO2</v>
       </c>
     </row>
-    <row r="22" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="12:22">
       <c r="L22" t="str">
         <v>Continents</v>
       </c>
@@ -2294,7 +2312,7 @@
         <v>Edgar Air NonAg NH3</v>
       </c>
     </row>
-    <row r="23" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="12:22">
       <c r="L23" t="str">
         <v>World</v>
       </c>
@@ -2305,7 +2323,7 @@
         <v>Edgar Air NonAg NOx</v>
       </c>
     </row>
-    <row r="24" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="12:22">
       <c r="L24" t="str">
         <v>Ecoregions</v>
       </c>
@@ -2316,7 +2334,7 @@
         <v>Edgar Air NonAg SO2</v>
       </c>
     </row>
-    <row r="25" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="12:22">
       <c r="L25" t="str">
         <v>GeosGrid</v>
       </c>
@@ -2327,7 +2345,7 @@
         <v>Edgar Air Gen NH3</v>
       </c>
     </row>
-    <row r="26" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="12:22">
       <c r="L26" t="str">
         <v>Pop2010</v>
       </c>
@@ -2338,7 +2356,7 @@
         <v>Edgar Air Gen NOx</v>
       </c>
     </row>
-    <row r="27" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="12:22">
       <c r="L27" t="str">
         <v>EmitEdgarAgNH3</v>
       </c>
@@ -2349,7 +2367,7 @@
         <v>Edgar Air Gen SO2</v>
       </c>
     </row>
-    <row r="28" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="12:22">
       <c r="L28" t="str">
         <v>EmitEdgarAgNOx</v>
       </c>
@@ -2357,7 +2375,7 @@
         <v>EmitEdgarAgNOx</v>
       </c>
     </row>
-    <row r="29" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="12:22">
       <c r="L29" t="str">
         <v>EmitEdgarNonagNH3</v>
       </c>
@@ -2365,7 +2383,7 @@
         <v>EmitEdgarNonagNH3</v>
       </c>
     </row>
-    <row r="30" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="12:22">
       <c r="L30" t="str">
         <v>EmitEdgarNonagNOx</v>
       </c>
@@ -2373,7 +2391,7 @@
         <v>EmitEdgarNonagNOx</v>
       </c>
     </row>
-    <row r="31" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="12:22">
       <c r="L31" t="str">
         <v>EmitEdgarAgSO2</v>
       </c>
@@ -2381,7 +2399,7 @@
         <v>EmitEdgarAgSO2</v>
       </c>
     </row>
-    <row r="32" spans="12:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="12:22">
       <c r="L32" t="str">
         <v>EmitEdgarNonagSO2</v>
       </c>
@@ -2389,7 +2407,7 @@
         <v>EmitEdgarNonagSO2</v>
       </c>
     </row>
-    <row r="33" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="12:13">
       <c r="L33" t="str">
         <v>EmitEdgarGenNH3</v>
       </c>
@@ -2397,7 +2415,7 @@
         <v>EmitEdgarGenNH3</v>
       </c>
     </row>
-    <row r="34" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="12:13">
       <c r="L34" t="str">
         <v>EmitEdgarGenNOx</v>
       </c>
@@ -2405,7 +2423,7 @@
         <v>EmitEdgarGenNOx</v>
       </c>
     </row>
-    <row r="35" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="12:13">
       <c r="L35" t="str">
         <v>EmitEdgarGenSO2</v>
       </c>
@@ -2413,42 +2431,42 @@
         <v>EmitEdgarGenSO2</v>
       </c>
     </row>
-    <row r="36" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="12:13">
       <c r="L36" t="str">
         <v>file_FF_NOx</v>
       </c>
     </row>
-    <row r="37" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="12:13">
       <c r="L37" t="str">
         <v>file_FF_NHx</v>
       </c>
     </row>
-    <row r="38" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="12:13">
       <c r="L38" t="str">
         <v>file_FF_SOx</v>
       </c>
     </row>
-    <row r="39" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="12:13">
       <c r="L39" t="str">
         <v>ecoreg_RFs_NH4_Lebrun</v>
       </c>
     </row>
-    <row r="40" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="12:13">
       <c r="L40" t="str">
         <v>ecoreg_RFs_NO3_Lebrun</v>
       </c>
     </row>
-    <row r="41" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="12:13">
       <c r="L41" t="str">
         <v>ecoreg_RFs_SO4_Lebrun</v>
       </c>
     </row>
-    <row r="42" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="12:13">
       <c r="L42" t="str">
         <v>ecoreg_EFs_Gade</v>
       </c>
     </row>
-    <row r="43" spans="12:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="12:13">
       <c r="L43" t="str">
         <v>ecoreg_GEPs</v>
       </c>
@@ -2462,57 +2480,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E2502FB-B45F-43BB-8645-D93E9F9C6CDF}">
   <dimension ref="B2:O147"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+    <col min="2" max="2" width="42.125" customWidth="1"/>
+    <col min="3" max="3" width="26.375" customWidth="1"/>
+    <col min="4" max="4" width="44.625" customWidth="1"/>
     <col min="5" max="5" width="58" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" customWidth="1"/>
-    <col min="7" max="7" width="68.42578125" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="11" width="32.42578125" customWidth="1"/>
-    <col min="12" max="12" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="31.375" customWidth="1"/>
+    <col min="7" max="7" width="68.375" customWidth="1"/>
+    <col min="8" max="8" width="18.625" customWidth="1"/>
+    <col min="9" max="9" width="30.625" customWidth="1"/>
+    <col min="10" max="10" width="22.875" customWidth="1"/>
+    <col min="11" max="11" width="32.375" customWidth="1"/>
+    <col min="12" max="12" width="21.375" customWidth="1"/>
     <col min="13" max="13" width="28" customWidth="1"/>
-    <col min="14" max="14" width="37.42578125" customWidth="1"/>
-    <col min="15" max="15" width="11.85546875" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" customWidth="1"/>
-    <col min="17" max="17" width="19.5703125" customWidth="1"/>
+    <col min="14" max="14" width="37.375" customWidth="1"/>
+    <col min="15" max="15" width="11.875" customWidth="1"/>
+    <col min="16" max="16" width="16.875" customWidth="1"/>
+    <col min="17" max="17" width="19.625" customWidth="1"/>
     <col min="18" max="22" width="18" customWidth="1"/>
-    <col min="23" max="23" width="14.85546875" customWidth="1"/>
-    <col min="24" max="24" width="19.42578125" customWidth="1"/>
-    <col min="25" max="26" width="23.42578125" customWidth="1"/>
-    <col min="27" max="28" width="20.140625" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" customWidth="1"/>
-    <col min="31" max="31" width="14.85546875" customWidth="1"/>
-    <col min="32" max="32" width="18.42578125" customWidth="1"/>
-    <col min="33" max="33" width="11.85546875" customWidth="1"/>
-    <col min="34" max="34" width="15.42578125" customWidth="1"/>
-    <col min="35" max="35" width="23.42578125" customWidth="1"/>
-    <col min="36" max="36" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="15.42578125" customWidth="1"/>
+    <col min="23" max="23" width="14.875" customWidth="1"/>
+    <col min="24" max="24" width="19.375" customWidth="1"/>
+    <col min="25" max="26" width="23.375" customWidth="1"/>
+    <col min="27" max="28" width="20.125" customWidth="1"/>
+    <col min="29" max="29" width="10.375" customWidth="1"/>
+    <col min="31" max="31" width="14.875" customWidth="1"/>
+    <col min="32" max="32" width="18.375" customWidth="1"/>
+    <col min="33" max="33" width="11.875" customWidth="1"/>
+    <col min="34" max="34" width="15.375" customWidth="1"/>
+    <col min="35" max="35" width="23.375" customWidth="1"/>
+    <col min="36" max="36" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14">
       <c r="E2" t="s">
         <v>93</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14">
       <c r="B4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -2553,7 +2571,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" t="s">
         <v>28</v>
       </c>
@@ -2562,11 +2580,11 @@
       </c>
       <c r="E6" t="str" cm="1">
         <f t="array" ref="E6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F6" t="str" cm="1">
         <f t="array" ref="F6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G6" t="str" cm="1">
         <f t="array" ref="G6">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -2592,10 +2610,10 @@
       </c>
       <c r="M6" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
       <c r="B7" t="s">
         <v>266</v>
       </c>
@@ -2634,7 +2652,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14">
       <c r="B8" t="s">
         <v>272</v>
       </c>
@@ -2667,7 +2685,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="B9" t="s">
         <v>274</v>
       </c>
@@ -2700,7 +2718,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14">
       <c r="B10" t="s">
         <v>270</v>
       </c>
@@ -2733,7 +2751,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14">
       <c r="B11" t="s">
         <v>275</v>
       </c>
@@ -2766,7 +2784,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" t="s">
         <v>268</v>
       </c>
@@ -2799,7 +2817,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" t="s">
         <v>263</v>
       </c>
@@ -2832,7 +2850,7 @@
         <v>C:\CalcDir\TRACI_ozone_stm\calc\datasets\Input\</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="B14" t="s">
         <v>254</v>
       </c>
@@ -2867,7 +2885,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14">
       <c r="B15" t="s">
         <v>255</v>
       </c>
@@ -2902,7 +2920,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14">
       <c r="B16" t="s">
         <v>256</v>
       </c>
@@ -2938,7 +2956,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:13">
       <c r="B17" t="s">
         <v>257</v>
       </c>
@@ -2974,7 +2992,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\data_input\</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:13">
       <c r="B18" t="s">
         <v>250</v>
       </c>
@@ -2987,7 +3005,7 @@
       </c>
       <c r="F18" t="str" cm="1">
         <f t="array" ref="F18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>anthro_compiled_v01</v>
+        <v/>
       </c>
       <c r="G18" t="str" cm="1">
         <f t="array" ref="G18">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3007,10 +3025,10 @@
       </c>
       <c r="M18" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\anthro_compiled_v01</v>
-      </c>
-    </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13">
       <c r="B19" t="s">
         <v>251</v>
       </c>
@@ -3046,7 +3064,7 @@
         <v>C:\CalcDir\TRACI_ozone\TRACI_ozone\intermediates\</v>
       </c>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:13">
       <c r="B20" t="s">
         <v>29</v>
       </c>
@@ -3055,11 +3073,11 @@
       </c>
       <c r="E20" t="str" cm="1">
         <f t="array" ref="E20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F20" t="str" cm="1">
         <f t="array" ref="F20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G20" t="str" cm="1">
         <f t="array" ref="G20">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3082,10 +3100,10 @@
       </c>
       <c r="M20" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13">
       <c r="B21" t="s">
         <v>30</v>
       </c>
@@ -3094,11 +3112,11 @@
       </c>
       <c r="E21" t="str" cm="1">
         <f t="array" ref="E21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F21" t="str" cm="1">
         <f t="array" ref="F21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G21" t="str" cm="1">
         <f t="array" ref="G21">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3124,10 +3142,10 @@
       </c>
       <c r="M21" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13">
       <c r="B22" t="s">
         <v>39</v>
       </c>
@@ -3136,7 +3154,7 @@
       </c>
       <c r="E22" t="str" cm="1">
         <f t="array" ref="E22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>W:\data\geo\ecoregions_teow\Olson_2012\official</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F22" t="str" cm="1">
         <f t="array" ref="F22">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3163,10 +3181,10 @@
       </c>
       <c r="M22" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>W:\data\geo\ecoregions_teow\Olson_2012\official\</v>
-      </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13">
       <c r="B23" t="s">
         <v>31</v>
       </c>
@@ -3175,11 +3193,11 @@
       </c>
       <c r="E23" t="str" cm="1">
         <f t="array" ref="E23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F23" t="str" cm="1">
         <f t="array" ref="F23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G23" t="str" cm="1">
         <f t="array" ref="G23">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3199,10 +3217,10 @@
       </c>
       <c r="M23" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13">
       <c r="B24" t="s">
         <v>32</v>
       </c>
@@ -3211,11 +3229,11 @@
       </c>
       <c r="E24" t="str" cm="1">
         <f t="array" ref="E24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F24" t="str" cm="1">
         <f t="array" ref="F24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G24" t="str" cm="1">
         <f t="array" ref="G24">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3235,10 +3253,10 @@
       </c>
       <c r="M24" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13">
       <c r="B25" t="s">
         <v>33</v>
       </c>
@@ -3247,11 +3265,11 @@
       </c>
       <c r="E25" t="str" cm="1">
         <f t="array" ref="E25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F25" t="str" cm="1">
         <f t="array" ref="F25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G25" t="str" cm="1">
         <f t="array" ref="G25">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3271,10 +3289,10 @@
       </c>
       <c r="M25" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13">
       <c r="B26" t="s">
         <v>34</v>
       </c>
@@ -3283,11 +3301,11 @@
       </c>
       <c r="E26" t="str" cm="1">
         <f t="array" ref="E26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F26" t="str" cm="1">
         <f t="array" ref="F26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G26" t="str" cm="1">
         <f t="array" ref="G26">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3307,10 +3325,10 @@
       </c>
       <c r="M26" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13">
       <c r="B27" t="s">
         <v>35</v>
       </c>
@@ -3319,11 +3337,11 @@
       </c>
       <c r="E27" t="str" cm="1">
         <f t="array" ref="E27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F27" t="str" cm="1">
         <f t="array" ref="F27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G27" t="str" cm="1">
         <f t="array" ref="G27">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3343,10 +3361,10 @@
       </c>
       <c r="M27" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13">
       <c r="B28" t="s">
         <v>36</v>
       </c>
@@ -3355,11 +3373,11 @@
       </c>
       <c r="E28" t="str" cm="1">
         <f t="array" ref="E28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F28" t="str" cm="1">
         <f t="array" ref="F28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G28" t="str" cm="1">
         <f t="array" ref="G28">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3379,10 +3397,10 @@
       </c>
       <c r="M28" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs_GLAM3\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13">
       <c r="B29" t="s">
         <v>37</v>
       </c>
@@ -3391,11 +3409,11 @@
       </c>
       <c r="E29" t="str" cm="1">
         <f t="array" ref="E29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F29" t="str" cm="1">
         <f t="array" ref="F29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G29" t="str" cm="1">
         <f t="array" ref="G29">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3415,10 +3433,10 @@
       </c>
       <c r="M29" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13">
       <c r="B30" t="s">
         <v>38</v>
       </c>
@@ -3427,11 +3445,11 @@
       </c>
       <c r="E30" t="str" cm="1">
         <f t="array" ref="E30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F30" t="str" cm="1">
         <f t="array" ref="F30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>Shapefiles</v>
+        <v/>
       </c>
       <c r="G30" t="str" cm="1">
         <f t="array" ref="G30">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File name]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3451,10 +3469,10 @@
       </c>
       <c r="M30" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\CalcCFs\calc\datasets\Input\Shapefiles</v>
-      </c>
-    </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13">
       <c r="B31" t="s">
         <v>226</v>
       </c>
@@ -3463,7 +3481,7 @@
       </c>
       <c r="E31" t="str" cm="1">
         <f t="array" ref="E31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F31" t="str" cm="1">
         <f t="array" ref="F31">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3485,10 +3503,10 @@
       </c>
       <c r="M31" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13">
       <c r="B32" t="s">
         <v>227</v>
       </c>
@@ -3497,7 +3515,7 @@
       </c>
       <c r="E32" t="str" cm="1">
         <f t="array" ref="E32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F32" t="str" cm="1">
         <f t="array" ref="F32">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3519,10 +3537,10 @@
       </c>
       <c r="M32" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15">
       <c r="B33" t="s">
         <v>228</v>
       </c>
@@ -3531,7 +3549,7 @@
       </c>
       <c r="E33" t="str" cm="1">
         <f t="array" ref="E33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F33" t="str" cm="1">
         <f t="array" ref="F33">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3553,10 +3571,10 @@
       </c>
       <c r="M33" s="10" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\temp\FFsCFs\Intermed\Shapefiles\</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15">
       <c r="B34" t="s">
         <v>191</v>
       </c>
@@ -3565,7 +3583,7 @@
       </c>
       <c r="E34" t="str" cm="1">
         <f t="array" ref="E34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F34" t="str" cm="1">
         <f t="array" ref="F34">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3586,10 +3604,10 @@
       </c>
       <c r="M34" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
-      </c>
-    </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15">
       <c r="B35" t="s">
         <v>192</v>
       </c>
@@ -3598,7 +3616,7 @@
       </c>
       <c r="E35" t="str" cm="1">
         <f t="array" ref="E35">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F35" t="str" cm="1">
         <f t="array" ref="F35">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3619,10 +3637,10 @@
       </c>
       <c r="M35" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15">
       <c r="B36" t="s">
         <v>193</v>
       </c>
@@ -3631,7 +3649,7 @@
       </c>
       <c r="E36" t="str" cm="1">
         <f t="array" ref="E36">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all</v>
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles</v>
       </c>
       <c r="F36" t="str" cm="1">
         <f t="array" ref="F36">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3652,10 +3670,10 @@
       </c>
       <c r="M36" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\FF_Roy\DepositionAirborne\2024-03-28_create_all\</v>
-      </c>
-    </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrAcid_Inputs\Shapefiles\</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15">
       <c r="B37" t="s">
         <v>141</v>
       </c>
@@ -3664,7 +3682,7 @@
       </c>
       <c r="E37" t="str" cm="1">
         <f t="array" ref="E37">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F37" t="str" cm="1">
         <f t="array" ref="F37">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3685,10 +3703,10 @@
       </c>
       <c r="M37" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15">
       <c r="B38" t="s">
         <v>143</v>
       </c>
@@ -3697,7 +3715,7 @@
       </c>
       <c r="E38" t="str" cm="1">
         <f t="array" ref="E38">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F38" t="str" cm="1">
         <f t="array" ref="F38">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3718,10 +3736,10 @@
       </c>
       <c r="M38" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15">
       <c r="B39" t="s">
         <v>142</v>
       </c>
@@ -3730,7 +3748,7 @@
       </c>
       <c r="E39" t="str" cm="1">
         <f t="array" ref="E39">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F39" t="str" cm="1">
         <f t="array" ref="F39">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3751,10 +3769,10 @@
       </c>
       <c r="M39" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15">
       <c r="B40" t="s">
         <v>57</v>
       </c>
@@ -3763,7 +3781,7 @@
       </c>
       <c r="E40" t="str" cm="1">
         <f t="array" ref="E40">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F40" t="str" cm="1">
         <f t="array" ref="F40">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3784,10 +3802,10 @@
       </c>
       <c r="M40" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15">
       <c r="B41" t="s">
         <v>50</v>
       </c>
@@ -3796,7 +3814,7 @@
       </c>
       <c r="E41" t="str" cm="1">
         <f t="array" ref="E41">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory main]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input</v>
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input</v>
       </c>
       <c r="F41" t="str" cm="1">
         <f t="array" ref="F41">_xlfn.LET(_xlpm.the_user, $F$2, _xlpm.big_tbl, Tbl.File_Locations[], _xlpm.user_col, _xlfn.XMATCH("User",Tbl.File_Locations[#Headers],0), _xlpm.data_col, _xlfn.XMATCH(Tbl.Files[[#Headers],[File directory subfolder]], Tbl.File_Locations[#Headers]), _xlpm.filtered_table, _xlfn._xlws.FILTER(_xlpm.big_tbl, INDEX(_xlpm.big_tbl, ,_xlpm.user_col)=_xlpm.the_user), _xlpm.result, _xlfn.XLOOKUP(Tbl.Files[[#This Row],[File unique name]:[File unique name]], INDEX(_xlpm.filtered_table,,1), INDEX(_xlpm.filtered_table, ,_xlpm.data_col)), IF(_xlpm.result=0,"",_xlpm.result))</f>
@@ -3817,15 +3835,15 @@
       </c>
       <c r="M41" s="9" t="str">
         <f>HYPERLINK(Tbl.Files[[#This Row],[File directory main]]&amp;IF(ISBLANK(Tbl.Files[[#This Row],[File directory subfolder]]),"","\"&amp;Tbl.Files[[#This Row],[File directory subfolder]]))</f>
-        <v>C:\CalcDir\Python\Code_FFtoCF_v2\calc\datasets\Input\</v>
-      </c>
-    </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+        <v>C:\CalcDir\TerrestrialAcidificationCFs\calc\datasets\Input\</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15">
       <c r="B47" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:15">
       <c r="B48" s="3" t="s">
         <v>42</v>
       </c>
@@ -3869,7 +3887,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:14">
       <c r="B49" t="s">
         <v>46</v>
       </c>
@@ -3893,7 +3911,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:14">
       <c r="B50" t="s">
         <v>47</v>
       </c>
@@ -3917,7 +3935,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:14">
       <c r="B51" t="s">
         <v>48</v>
       </c>
@@ -3941,7 +3959,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:14">
       <c r="B52" t="s">
         <v>49</v>
       </c>
@@ -3968,7 +3986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:14">
       <c r="B53" t="s">
         <v>50</v>
       </c>
@@ -3995,7 +4013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:14">
       <c r="B54" t="s">
         <v>151</v>
       </c>
@@ -4022,7 +4040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:14">
       <c r="B55" t="s">
         <v>152</v>
       </c>
@@ -4049,7 +4067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:14">
       <c r="B56" t="s">
         <v>153</v>
       </c>
@@ -4076,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:14">
       <c r="B57" t="s">
         <v>250</v>
       </c>
@@ -4103,7 +4121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:14">
       <c r="B58" t="s">
         <v>251</v>
       </c>
@@ -4130,7 +4148,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:14">
       <c r="B59" t="s">
         <v>32</v>
       </c>
@@ -4157,7 +4175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:14">
       <c r="B60" t="s">
         <v>51</v>
       </c>
@@ -4184,7 +4202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:14">
       <c r="B61" t="s">
         <v>52</v>
       </c>
@@ -4211,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:14">
       <c r="B62" t="s">
         <v>53</v>
       </c>
@@ -4238,7 +4256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:14">
       <c r="B63" t="s">
         <v>54</v>
       </c>
@@ -4265,7 +4283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:14">
       <c r="B64" t="s">
         <v>55</v>
       </c>
@@ -4292,7 +4310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:12">
       <c r="B65" t="s">
         <v>56</v>
       </c>
@@ -4319,7 +4337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:12">
       <c r="B66" t="s">
         <v>223</v>
       </c>
@@ -4346,7 +4364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:12">
       <c r="B67" t="s">
         <v>225</v>
       </c>
@@ -4373,7 +4391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:12">
       <c r="B68" t="s">
         <v>224</v>
       </c>
@@ -4400,12 +4418,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:12">
       <c r="B74" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="75" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:12">
       <c r="B75" t="s">
         <v>71</v>
       </c>
@@ -4425,7 +4443,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="76" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:12">
       <c r="B76" t="s">
         <v>28</v>
       </c>
@@ -4445,7 +4463,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="77" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:12">
       <c r="B77" t="s">
         <v>266</v>
       </c>
@@ -4462,7 +4480,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:12">
       <c r="B78" t="s">
         <v>272</v>
       </c>
@@ -4479,7 +4497,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="79" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:12">
       <c r="B79" t="s">
         <v>270</v>
       </c>
@@ -4496,7 +4514,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="80" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:12">
       <c r="B80" t="s">
         <v>274</v>
       </c>
@@ -4513,7 +4531,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:7">
       <c r="B81" t="s">
         <v>275</v>
       </c>
@@ -4530,7 +4548,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:7">
       <c r="B82" t="s">
         <v>268</v>
       </c>
@@ -4547,7 +4565,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:7">
       <c r="B83" t="s">
         <v>263</v>
       </c>
@@ -4564,7 +4582,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:7">
       <c r="B84" t="s">
         <v>254</v>
       </c>
@@ -4581,7 +4599,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:7">
       <c r="B85" t="s">
         <v>255</v>
       </c>
@@ -4598,7 +4616,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:7">
       <c r="B86" t="s">
         <v>256</v>
       </c>
@@ -4615,7 +4633,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:7">
       <c r="B87" t="s">
         <v>257</v>
       </c>
@@ -4632,7 +4650,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:7">
       <c r="B88" t="s">
         <v>250</v>
       </c>
@@ -4652,7 +4670,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:7">
       <c r="B89" t="s">
         <v>251</v>
       </c>
@@ -4669,7 +4687,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:7">
       <c r="B90" t="s">
         <v>29</v>
       </c>
@@ -4689,7 +4707,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:7">
       <c r="B91" t="s">
         <v>30</v>
       </c>
@@ -4709,7 +4727,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:7">
       <c r="B92" t="s">
         <v>39</v>
       </c>
@@ -4726,7 +4744,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:7">
       <c r="B93" t="s">
         <v>31</v>
       </c>
@@ -4746,7 +4764,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:7">
       <c r="B94" t="s">
         <v>32</v>
       </c>
@@ -4766,7 +4784,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:7">
       <c r="B95" t="s">
         <v>33</v>
       </c>
@@ -4786,7 +4804,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:7">
       <c r="B96" t="s">
         <v>34</v>
       </c>
@@ -4806,7 +4824,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:7">
       <c r="B97" t="s">
         <v>35</v>
       </c>
@@ -4826,7 +4844,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:7">
       <c r="B98" t="s">
         <v>36</v>
       </c>
@@ -4846,7 +4864,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:7">
       <c r="B99" t="s">
         <v>37</v>
       </c>
@@ -4866,7 +4884,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:7">
       <c r="B100" t="s">
         <v>38</v>
       </c>
@@ -4886,7 +4904,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:7">
       <c r="B101" t="s">
         <v>226</v>
       </c>
@@ -4903,7 +4921,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:7">
       <c r="B102" t="s">
         <v>227</v>
       </c>
@@ -4920,7 +4938,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:7">
       <c r="B103" t="s">
         <v>228</v>
       </c>
@@ -4937,7 +4955,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:7">
       <c r="B104" t="s">
         <v>191</v>
       </c>
@@ -4954,7 +4972,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:7">
       <c r="B105" t="s">
         <v>192</v>
       </c>
@@ -4971,7 +4989,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:7">
       <c r="B106" t="s">
         <v>193</v>
       </c>
@@ -4988,7 +5006,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:7">
       <c r="B107" t="s">
         <v>141</v>
       </c>
@@ -5005,7 +5023,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:7">
       <c r="B108" t="s">
         <v>143</v>
       </c>
@@ -5022,7 +5040,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:7">
       <c r="B109" t="s">
         <v>142</v>
       </c>
@@ -5039,7 +5057,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:7">
       <c r="B110" t="s">
         <v>57</v>
       </c>
@@ -5056,7 +5074,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:7">
       <c r="B111" t="s">
         <v>50</v>
       </c>
@@ -5073,7 +5091,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:7">
       <c r="B112" s="13" t="s">
         <v>28</v>
       </c>
@@ -5091,7 +5109,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:7">
       <c r="B113" s="13" t="s">
         <v>266</v>
       </c>
@@ -5109,7 +5127,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:7">
       <c r="B114" s="13" t="s">
         <v>272</v>
       </c>
@@ -5127,7 +5145,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:7">
       <c r="B115" s="13" t="s">
         <v>270</v>
       </c>
@@ -5145,7 +5163,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:7">
       <c r="B116" s="13" t="s">
         <v>274</v>
       </c>
@@ -5163,7 +5181,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:7">
       <c r="B117" s="13" t="s">
         <v>275</v>
       </c>
@@ -5181,7 +5199,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:7">
       <c r="B118" s="13" t="s">
         <v>268</v>
       </c>
@@ -5199,7 +5217,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:7">
       <c r="B119" s="13" t="s">
         <v>263</v>
       </c>
@@ -5217,7 +5235,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:7">
       <c r="B120" s="13" t="s">
         <v>254</v>
       </c>
@@ -5235,7 +5253,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:7">
       <c r="B121" s="13" t="s">
         <v>255</v>
       </c>
@@ -5253,7 +5271,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:7">
       <c r="B122" s="13" t="s">
         <v>256</v>
       </c>
@@ -5271,7 +5289,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:7">
       <c r="B123" s="13" t="s">
         <v>257</v>
       </c>
@@ -5289,7 +5307,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:7">
       <c r="B124" s="13" t="s">
         <v>250</v>
       </c>
@@ -5307,7 +5325,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:7">
       <c r="B125" s="13" t="s">
         <v>251</v>
       </c>
@@ -5325,7 +5343,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:7">
       <c r="B126" s="13" t="s">
         <v>29</v>
       </c>
@@ -5343,7 +5361,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:7">
       <c r="B127" s="13" t="s">
         <v>30</v>
       </c>
@@ -5361,7 +5379,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:7">
       <c r="B128" s="13" t="s">
         <v>39</v>
       </c>
@@ -5379,7 +5397,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:7">
       <c r="B129" s="13" t="s">
         <v>31</v>
       </c>
@@ -5397,7 +5415,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:7">
       <c r="B130" s="13" t="s">
         <v>32</v>
       </c>
@@ -5415,7 +5433,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:7">
       <c r="B131" s="13" t="s">
         <v>33</v>
       </c>
@@ -5433,7 +5451,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:7">
       <c r="B132" s="13" t="s">
         <v>34</v>
       </c>
@@ -5451,7 +5469,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:7">
       <c r="B133" s="13" t="s">
         <v>35</v>
       </c>
@@ -5469,7 +5487,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:7">
       <c r="B134" s="13" t="s">
         <v>36</v>
       </c>
@@ -5487,7 +5505,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:7">
       <c r="B135" s="13" t="s">
         <v>37</v>
       </c>
@@ -5505,7 +5523,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:7">
       <c r="B136" s="13" t="s">
         <v>38</v>
       </c>
@@ -5523,7 +5541,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:7">
       <c r="B137" s="13" t="s">
         <v>226</v>
       </c>
@@ -5541,7 +5559,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:7">
       <c r="B138" s="13" t="s">
         <v>227</v>
       </c>
@@ -5559,7 +5577,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:7">
       <c r="B139" s="13" t="s">
         <v>228</v>
       </c>
@@ -5577,7 +5595,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:7">
       <c r="B140" s="13" t="s">
         <v>191</v>
       </c>
@@ -5595,7 +5613,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:7">
       <c r="B141" s="13" t="s">
         <v>192</v>
       </c>
@@ -5613,7 +5631,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:7">
       <c r="B142" s="13" t="s">
         <v>193</v>
       </c>
@@ -5631,7 +5649,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:7">
       <c r="B143" s="13" t="s">
         <v>141</v>
       </c>
@@ -5649,7 +5667,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:7">
       <c r="B144" s="13" t="s">
         <v>143</v>
       </c>
@@ -5667,7 +5685,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:7">
       <c r="B145" s="13" t="s">
         <v>142</v>
       </c>
@@ -5685,7 +5703,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:7">
       <c r="B146" s="13" t="s">
         <v>57</v>
       </c>
@@ -5703,7 +5721,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:7">
       <c r="B147" s="13" t="s">
         <v>50</v>
       </c>
@@ -5765,24 +5783,24 @@
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9">
       <c r="B3" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9">
       <c r="B4" t="s">
         <v>102</v>
       </c>
@@ -5808,7 +5826,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9">
       <c r="B5" t="s">
         <v>107</v>
       </c>
@@ -5829,7 +5847,7 @@
         <v>10102-43-9</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9">
       <c r="B6" t="s">
         <v>202</v>
       </c>
@@ -5850,7 +5868,7 @@
         <v>10102-43-9</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9">
       <c r="B7" t="s">
         <v>204</v>
       </c>
@@ -5871,7 +5889,7 @@
         <v>10102-44-0</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9">
       <c r="B8" t="s">
         <v>108</v>
       </c>
@@ -5890,7 +5908,7 @@
         <v>000-00-0</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9">
       <c r="B9" t="s">
         <v>128</v>
       </c>
@@ -5911,7 +5929,7 @@
         <v>7664-41-7</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9">
       <c r="B10" t="s">
         <v>129</v>
       </c>
@@ -5932,7 +5950,7 @@
         <v>14798-03-9</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9">
       <c r="B11" t="s">
         <v>109</v>
       </c>
@@ -5951,7 +5969,7 @@
         <v>000-00-0</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9">
       <c r="B12" t="s">
         <v>132</v>
       </c>
@@ -5972,7 +5990,7 @@
         <v>7446-09-5</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:9">
       <c r="B13" t="s">
         <v>135</v>
       </c>
@@ -6010,24 +6028,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD1D767F-008E-40CD-A786-127BCF11776D}">
   <dimension ref="B4:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="70" customWidth="1"/>
-    <col min="7" max="7" width="73.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" customWidth="1"/>
+    <col min="7" max="7" width="73.125" customWidth="1"/>
+    <col min="9" max="9" width="17.375" customWidth="1"/>
     <col min="10" max="10" width="28" customWidth="1"/>
-    <col min="11" max="11" width="16.42578125" customWidth="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
+    <col min="11" max="11" width="16.375" customWidth="1"/>
+    <col min="12" max="12" width="16.75" customWidth="1"/>
+    <col min="13" max="13" width="15.375" customWidth="1"/>
     <col min="14" max="14" width="45" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14">
       <c r="B4" t="s">
         <v>137</v>
       </c>
@@ -6036,18 +6054,18 @@
         <v>'STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010', 'STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010'</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14">
       <c r="B6" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14">
       <c r="B7" t="b">
         <f>ROWS(_xlfn.UNIQUE(Tbl.SpatialTransforms[STM unique name]))=ROWS(Tbl.SpatialTransforms[STM unique name])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14">
       <c r="B9" t="s">
         <v>58</v>
       </c>
@@ -6055,7 +6073,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14">
       <c r="B10" t="s">
         <v>59</v>
       </c>
@@ -6096,13 +6114,13 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14">
       <c r="B11" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G11" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[Auto file name]]</f>
@@ -6131,7 +6149,7 @@
         <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_New-Countries_Pop2010</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14">
       <c r="B12" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
@@ -6166,7 +6184,7 @@
         <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_New-Countries_Pop2010</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14">
       <c r="B13" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010</v>
@@ -6201,7 +6219,7 @@
         <v>STM3_newEmit_Orig-ArchFullUrb2v01_prep01_urb_New-Countries_Pop2010</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14">
       <c r="B14" t="str">
         <f>Tbl.SpatialTransforms[[#This Row],[File name]]</f>
         <v>STM3_newEmit_Orig-ArchFullUrb2v02_prep01_urb_New-Countries_Pop2010</v>
@@ -6268,47 +6286,47 @@
       <selection activeCell="AE24" sqref="AE24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.375" customWidth="1"/>
+    <col min="3" max="3" width="17.375" customWidth="1"/>
     <col min="4" max="6" width="17" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" customWidth="1"/>
-    <col min="8" max="8" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
+    <col min="7" max="7" width="15.375" customWidth="1"/>
+    <col min="8" max="8" width="22.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.375" customWidth="1"/>
+    <col min="10" max="10" width="13.625" customWidth="1"/>
     <col min="11" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="29.140625" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" customWidth="1"/>
-    <col min="14" max="15" width="17.5703125" customWidth="1"/>
-    <col min="16" max="16" width="34.5703125" customWidth="1"/>
-    <col min="17" max="17" width="16.42578125" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" customWidth="1"/>
+    <col min="12" max="12" width="29.125" customWidth="1"/>
+    <col min="13" max="13" width="22.125" customWidth="1"/>
+    <col min="14" max="15" width="17.625" customWidth="1"/>
+    <col min="16" max="16" width="34.625" customWidth="1"/>
+    <col min="17" max="17" width="16.375" customWidth="1"/>
+    <col min="18" max="18" width="15.375" customWidth="1"/>
+    <col min="19" max="19" width="14.375" customWidth="1"/>
     <col min="20" max="20" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:24">
       <c r="X3" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:24">
       <c r="X4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="5" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:24">
       <c r="X5" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:24">
       <c r="X6" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="7" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:24">
       <c r="B7" t="s">
         <v>211</v>
       </c>
@@ -6322,7 +6340,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="8" spans="2:24" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:24" ht="42.75">
       <c r="B8" t="s">
         <v>206</v>
       </c>
@@ -6390,7 +6408,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:24">
       <c r="B9" t="s">
         <v>208</v>
       </c>
@@ -6455,7 +6473,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:24">
       <c r="B10" t="s">
         <v>207</v>
       </c>
@@ -6520,7 +6538,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="11" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:24">
       <c r="F11">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -6576,7 +6594,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="12" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:24">
       <c r="F12">
         <f t="shared" ref="F12:F25" si="1">IFERROR($F11+1,1)</f>
         <v>4</v>
@@ -6632,7 +6650,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:24">
       <c r="F13">
         <f t="shared" si="1"/>
         <v>5</v>
@@ -6688,7 +6706,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="14" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:24">
       <c r="F14">
         <f t="shared" si="1"/>
         <v>6</v>
@@ -6744,7 +6762,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="15" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:24">
       <c r="F15">
         <f t="shared" si="1"/>
         <v>7</v>
@@ -6800,7 +6818,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="16" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:24">
       <c r="F16">
         <f t="shared" si="1"/>
         <v>8</v>
@@ -6856,7 +6874,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="17" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:24">
       <c r="F17">
         <f t="shared" si="1"/>
         <v>9</v>
@@ -6912,7 +6930,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="18" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:24">
       <c r="F18">
         <f t="shared" si="1"/>
         <v>10</v>
@@ -6970,7 +6988,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:24">
       <c r="F19">
         <f t="shared" si="1"/>
         <v>11</v>
@@ -7028,7 +7046,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="20" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:24">
       <c r="F20">
         <f t="shared" si="1"/>
         <v>12</v>
@@ -7086,7 +7104,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="21" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:24">
       <c r="F21">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -7138,7 +7156,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="22" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:24">
       <c r="F22">
         <f t="shared" si="1"/>
         <v>14</v>
@@ -7190,7 +7208,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="23" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:24">
       <c r="F23">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -7242,7 +7260,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="24" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="6:24">
       <c r="F24">
         <f t="shared" si="1"/>
         <v>16</v>
@@ -7294,7 +7312,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="25" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="6:24">
       <c r="F25">
         <f t="shared" si="1"/>
         <v>17</v>
@@ -7346,7 +7364,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="26" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="6:24">
       <c r="F26">
         <f t="shared" ref="F26:F53" si="2">IFERROR($F25+1,1)</f>
         <v>18</v>
@@ -7398,7 +7416,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="27" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="6:24">
       <c r="F27">
         <f t="shared" si="2"/>
         <v>19</v>
@@ -7456,7 +7474,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="6:24">
       <c r="F28">
         <f t="shared" si="2"/>
         <v>20</v>
@@ -7514,7 +7532,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="29" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="6:24">
       <c r="F29">
         <f t="shared" si="2"/>
         <v>21</v>
@@ -7572,7 +7590,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="6:24">
       <c r="F30">
         <f t="shared" si="2"/>
         <v>22</v>
@@ -7624,7 +7642,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="31" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="6:24">
       <c r="F31">
         <f t="shared" si="2"/>
         <v>23</v>
@@ -7676,7 +7694,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="6:24">
       <c r="F32">
         <f t="shared" si="2"/>
         <v>24</v>
@@ -7728,7 +7746,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="33" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="6:24">
       <c r="F33">
         <f t="shared" si="2"/>
         <v>25</v>
@@ -7780,7 +7798,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="34" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="6:24">
       <c r="F34">
         <f t="shared" si="2"/>
         <v>26</v>
@@ -7832,7 +7850,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="6:24">
       <c r="F35">
         <f t="shared" si="2"/>
         <v>27</v>
@@ -7884,7 +7902,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="36" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="6:24">
       <c r="F36">
         <f t="shared" si="2"/>
         <v>28</v>
@@ -7942,7 +7960,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="37" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="6:24">
       <c r="F37">
         <f t="shared" si="2"/>
         <v>29</v>
@@ -8000,7 +8018,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="38" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="6:24">
       <c r="F38">
         <f t="shared" si="2"/>
         <v>30</v>
@@ -8058,7 +8076,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="39" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="6:24">
       <c r="F39">
         <f t="shared" si="2"/>
         <v>31</v>
@@ -8110,7 +8128,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="6:24">
       <c r="F40">
         <f t="shared" si="2"/>
         <v>32</v>
@@ -8162,7 +8180,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="41" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="6:24">
       <c r="F41">
         <f t="shared" si="2"/>
         <v>33</v>
@@ -8214,7 +8232,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="42" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="42" spans="6:24">
       <c r="F42">
         <f t="shared" si="2"/>
         <v>34</v>
@@ -8266,7 +8284,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="6:24">
       <c r="F43">
         <f t="shared" si="2"/>
         <v>35</v>
@@ -8318,7 +8336,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="44" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="6:24">
       <c r="F44">
         <f t="shared" si="2"/>
         <v>36</v>
@@ -8370,7 +8388,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="45" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="6:24">
       <c r="F45">
         <f t="shared" si="2"/>
         <v>37</v>
@@ -8428,7 +8446,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="6:24">
       <c r="F46">
         <f t="shared" si="2"/>
         <v>38</v>
@@ -8486,7 +8504,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="6:24">
       <c r="F47">
         <f t="shared" si="2"/>
         <v>39</v>
@@ -8544,7 +8562,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="48" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="6:24">
       <c r="F48">
         <f t="shared" si="2"/>
         <v>40</v>
@@ -8596,7 +8614,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="49" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:24">
       <c r="F49">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -8648,7 +8666,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="50" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="50" spans="6:24">
       <c r="F50">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -8700,7 +8718,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="51" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="6:24">
       <c r="F51">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -8752,7 +8770,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="52" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="6:24">
       <c r="F52">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -8804,7 +8822,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="6:24">
       <c r="F53">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -8856,7 +8874,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="54" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="6:24">
       <c r="F54">
         <f t="shared" ref="F54:F71" si="3">IFERROR($F53+1,1)</f>
         <v>46</v>
@@ -8914,7 +8932,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="55" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="6:24">
       <c r="F55">
         <f t="shared" si="3"/>
         <v>47</v>
@@ -8972,7 +8990,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="56" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="6:24">
       <c r="F56">
         <f t="shared" si="3"/>
         <v>48</v>
@@ -9030,7 +9048,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="57" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="6:24">
       <c r="F57">
         <f t="shared" si="3"/>
         <v>49</v>
@@ -9082,7 +9100,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="58" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="58" spans="6:24">
       <c r="F58">
         <f t="shared" si="3"/>
         <v>50</v>
@@ -9134,7 +9152,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="59" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="6:24">
       <c r="F59">
         <f t="shared" si="3"/>
         <v>51</v>
@@ -9186,7 +9204,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="60" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="6:24">
       <c r="F60">
         <f t="shared" si="3"/>
         <v>52</v>
@@ -9238,7 +9256,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="61" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="6:24">
       <c r="F61">
         <f t="shared" si="3"/>
         <v>53</v>
@@ -9290,7 +9308,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="62" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="6:24">
       <c r="F62">
         <f t="shared" si="3"/>
         <v>54</v>
@@ -9342,7 +9360,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="63" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="6:24">
       <c r="F63">
         <f t="shared" si="3"/>
         <v>55</v>
@@ -9400,7 +9418,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="6:24">
       <c r="F64">
         <f t="shared" si="3"/>
         <v>56</v>
@@ -9458,7 +9476,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="65" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="6:24">
       <c r="F65">
         <f t="shared" si="3"/>
         <v>57</v>
@@ -9516,7 +9534,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="66" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="66" spans="6:24">
       <c r="F66">
         <f t="shared" si="3"/>
         <v>58</v>
@@ -9568,7 +9586,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="67" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="67" spans="6:24">
       <c r="F67">
         <f t="shared" si="3"/>
         <v>59</v>
@@ -9620,7 +9638,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="68" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="6:24">
       <c r="F68">
         <f t="shared" si="3"/>
         <v>60</v>
@@ -9672,7 +9690,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="69" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="6:24">
       <c r="F69">
         <f t="shared" si="3"/>
         <v>61</v>
@@ -9724,7 +9742,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="6:24">
       <c r="F70">
         <f t="shared" si="3"/>
         <v>62</v>
@@ -9776,7 +9794,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="71" spans="6:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="6:24">
       <c r="F71">
         <f t="shared" si="3"/>
         <v>63</v>

</xml_diff>